<commit_message>
Version - Snakemake Parallel / gpkg file testing
</commit_message>
<xml_diff>
--- a/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
+++ b/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
@@ -735,16 +735,16 @@
         <v>575362.5352385062</v>
       </c>
       <c r="AI2" t="n">
-        <v>131417.5057127322</v>
+        <v>1363008.883277515</v>
       </c>
       <c r="AJ2" t="n">
-        <v>944648.6901633616</v>
+        <v>1673743.863662873</v>
       </c>
       <c r="AK2" t="n">
-        <v>539928.0690225936</v>
+        <v>1770929.380831994</v>
       </c>
       <c r="AL2" t="n">
-        <v>104732.415828859</v>
+        <v>467882.0219137627</v>
       </c>
       <c r="AM2" t="n">
         <v>0</v>
@@ -853,10 +853,10 @@
         <v>158762.0972720425</v>
       </c>
       <c r="AI3" t="n">
-        <v>750000</v>
+        <v>832559.6176464804</v>
       </c>
       <c r="AJ3" t="n">
-        <v>186000</v>
+        <v>206474.7851763272</v>
       </c>
       <c r="AK3" t="n">
         <v>0</v>
@@ -971,16 +971,16 @@
         <v>2932269.306095038</v>
       </c>
       <c r="AI4" t="n">
-        <v>13270000</v>
+        <v>15051334.48372555</v>
       </c>
       <c r="AJ4" t="n">
-        <v>605883.8709677419</v>
+        <v>687216.3376209416</v>
       </c>
       <c r="AK4" t="n">
-        <v>200476.1169048793</v>
+        <v>227387.5728360064</v>
       </c>
       <c r="AL4" t="n">
-        <v>100000</v>
+        <v>113423.7715427698</v>
       </c>
       <c r="AM4" t="n">
         <v>0</v>
@@ -1361,16 +1361,16 @@
         <v>60683417.27081787</v>
       </c>
       <c r="AI7" t="n">
-        <v>107664839.9740886</v>
+        <v>119940008.774887</v>
       </c>
       <c r="AJ7" t="n">
-        <v>72066090.04175031</v>
+        <v>80282546.03879559</v>
       </c>
       <c r="AK7" t="n">
-        <v>18211624.79784367</v>
+        <v>0</v>
       </c>
       <c r="AL7" t="n">
-        <v>2280000</v>
+        <v>0</v>
       </c>
       <c r="AM7" t="n">
         <v>19531580.67725457</v>
@@ -1597,16 +1597,16 @@
         <v>117845.3385428266</v>
       </c>
       <c r="AI9" t="n">
-        <v>20231.07821681842</v>
+        <v>59164.76512528938</v>
       </c>
       <c r="AJ9" t="n">
-        <v>100352.2102948071</v>
+        <v>95323.25981318217</v>
       </c>
       <c r="AK9" t="n">
-        <v>58894.99231195863</v>
+        <v>55943.58746414888</v>
       </c>
       <c r="AL9" t="n">
-        <v>23358.07893428084</v>
+        <v>29423.27478922973</v>
       </c>
       <c r="AM9" t="n">
         <v>0</v>
@@ -1715,16 +1715,16 @@
         <v>347492.3144530397</v>
       </c>
       <c r="AI10" t="n">
-        <v>79370.08481240895</v>
+        <v>823194.2166234716</v>
       </c>
       <c r="AJ10" t="n">
-        <v>570524.0428173263</v>
+        <v>1010863.748270797</v>
       </c>
       <c r="AK10" t="n">
-        <v>326091.5385549856</v>
+        <v>1069559.297987836</v>
       </c>
       <c r="AL10" t="n">
-        <v>63253.52685597097</v>
+        <v>282579.0640302716</v>
       </c>
       <c r="AM10" t="n">
         <v>0</v>
@@ -1845,16 +1845,16 @@
         <v>123293952.4307478</v>
       </c>
       <c r="AI11" t="n">
-        <v>15260000</v>
+        <v>15826688.59505524</v>
       </c>
       <c r="AJ11" t="n">
-        <v>109463835.6514357</v>
+        <v>124323939.0403684</v>
       </c>
       <c r="AK11" t="n">
-        <v>84360722.85758698</v>
+        <v>117559292.6341728</v>
       </c>
       <c r="AL11" t="n">
-        <v>3130000</v>
+        <v>0</v>
       </c>
       <c r="AM11" t="n">
         <v>0</v>
@@ -1975,16 +1975,16 @@
         <v>7500509.194314021</v>
       </c>
       <c r="AI12" t="n">
-        <v>40670000</v>
+        <v>44169446.79018223</v>
       </c>
       <c r="AJ12" t="n">
-        <v>6390000</v>
+        <v>12480409.26842172</v>
       </c>
       <c r="AK12" t="n">
-        <v>8339999.999999999</v>
+        <v>16324673.29592171</v>
       </c>
       <c r="AL12" t="n">
-        <v>5257820.683570589</v>
+        <v>4348566.670579161</v>
       </c>
       <c r="AM12" t="n">
         <v>0</v>
@@ -2093,16 +2093,16 @@
         <v>18774952.30430221</v>
       </c>
       <c r="AI13" t="n">
-        <v>12488101.88720034</v>
+        <v>18767136.55968409</v>
       </c>
       <c r="AJ13" t="n">
-        <v>10444232.14939149</v>
+        <v>8961818.425286237</v>
       </c>
       <c r="AK13" t="n">
-        <v>8117876.771854715</v>
+        <v>6965656.889621076</v>
       </c>
       <c r="AL13" t="n">
-        <v>1265390.530746279</v>
+        <v>1085785.916227977</v>
       </c>
       <c r="AM13" t="n">
         <v>0</v>
@@ -2211,10 +2211,10 @@
         <v>83184.94485375992</v>
       </c>
       <c r="AI14" t="n">
-        <v>260000</v>
+        <v>309005.0858612613</v>
       </c>
       <c r="AJ14" t="n">
-        <v>26425.94689191903</v>
+        <v>31406.73841654835</v>
       </c>
       <c r="AK14" t="n">
         <v>0</v>
@@ -2341,16 +2341,16 @@
         <v>15098067.49095743</v>
       </c>
       <c r="AI15" t="n">
-        <v>4469000</v>
+        <v>1191990.601808208</v>
       </c>
       <c r="AJ15" t="n">
-        <v>143254752.6201924</v>
+        <v>144445622.292241</v>
       </c>
       <c r="AK15" t="n">
-        <v>227579701.6593201</v>
+        <v>229471560.4613698</v>
       </c>
       <c r="AL15" t="n">
-        <v>23370874.55755456</v>
+        <v>23565155.48164811</v>
       </c>
       <c r="AM15" t="n">
         <v>76003846.62766981</v>
@@ -2459,16 +2459,16 @@
         <v>672411.6375678928</v>
       </c>
       <c r="AI16" t="n">
-        <v>151505.7901671955</v>
+        <v>545573.4897221323</v>
       </c>
       <c r="AJ16" t="n">
-        <v>300856.6681296098</v>
+        <v>218473.7041076912</v>
       </c>
       <c r="AK16" t="n">
-        <v>257623.9713495313</v>
+        <v>187079.3279656295</v>
       </c>
       <c r="AL16" t="n">
-        <v>447373.9760308926</v>
+        <v>693912.1887831823</v>
       </c>
       <c r="AM16" t="n">
         <v>0</v>
@@ -2577,16 +2577,16 @@
         <v>991287.2595073058</v>
       </c>
       <c r="AI17" t="n">
-        <v>1020697.251785475</v>
+        <v>1570680.497848381</v>
       </c>
       <c r="AJ17" t="n">
-        <v>405731.4713999902</v>
+        <v>331196.6035462395</v>
       </c>
       <c r="AK17" t="n">
-        <v>186885.3743395162</v>
+        <v>152553.611432068</v>
       </c>
       <c r="AL17" t="n">
-        <v>92897.63455588174</v>
+        <v>75831.88194946748</v>
       </c>
       <c r="AM17" t="n">
         <v>0</v>
@@ -2707,16 +2707,16 @@
         <v>77396984.64953232</v>
       </c>
       <c r="AI18" t="n">
-        <v>3808849.192346968</v>
+        <v>3814413.379525008</v>
       </c>
       <c r="AJ18" t="n">
-        <v>82222252.07542405</v>
+        <v>82342367.09643011</v>
       </c>
       <c r="AK18" t="n">
-        <v>46990894.99091719</v>
+        <v>47059542.00795279</v>
       </c>
       <c r="AL18" t="n">
-        <v>194326.2252197115</v>
+        <v>0</v>
       </c>
       <c r="AM18" t="n">
         <v>0</v>
@@ -2955,16 +2955,16 @@
         <v>25013557.50999298</v>
       </c>
       <c r="AI20" t="n">
-        <v>193317.7156801162</v>
+        <v>389570.7171572578</v>
       </c>
       <c r="AJ20" t="n">
-        <v>37754909.15149008</v>
+        <v>37582032.90598097</v>
       </c>
       <c r="AK20" t="n">
-        <v>4953419.743480374</v>
+        <v>4930738.49150735</v>
       </c>
       <c r="AL20" t="n">
-        <v>151892.9918271715</v>
+        <v>151197.4878321582</v>
       </c>
       <c r="AM20" t="n">
         <v>0</v>
@@ -3073,16 +3073,16 @@
         <v>1407211.983776106</v>
       </c>
       <c r="AI21" t="n">
-        <v>321418.7187913811</v>
+        <v>3333624.136208863</v>
       </c>
       <c r="AJ21" t="n">
-        <v>2310405.832568222</v>
+        <v>4093614.50992245</v>
       </c>
       <c r="AK21" t="n">
-        <v>1320546.963995018</v>
+        <v>4331309.208540903</v>
       </c>
       <c r="AL21" t="n">
-        <v>256152.776063354</v>
+        <v>1144337.957210769</v>
       </c>
       <c r="AM21" t="n">
         <v>0</v>
@@ -3203,16 +3203,16 @@
         <v>6973671.210240208</v>
       </c>
       <c r="AI22" t="n">
-        <v>6890353.260869565</v>
+        <v>11466334.22998163</v>
       </c>
       <c r="AJ22" t="n">
-        <v>2693185.314820706</v>
+        <v>2599767.222557667</v>
       </c>
       <c r="AK22" t="n">
-        <v>2093303.384754526</v>
+        <v>2020693.301944629</v>
       </c>
       <c r="AL22" t="n">
-        <v>326297.9169912089</v>
+        <v>314979.6728484913</v>
       </c>
       <c r="AM22" t="n">
         <v>0</v>
@@ -3439,16 +3439,16 @@
         <v>34660.39368906664</v>
       </c>
       <c r="AI24" t="n">
-        <v>240000</v>
+        <v>253496.4693464727</v>
       </c>
       <c r="AJ24" t="n">
-        <v>10000</v>
+        <v>10562.35288943636</v>
       </c>
       <c r="AK24" t="n">
         <v>0</v>
       </c>
       <c r="AL24" t="n">
-        <v>150000</v>
+        <v>158435.2933415454</v>
       </c>
       <c r="AM24" t="n">
         <v>0</v>
@@ -3557,16 +3557,16 @@
         <v>452601.7226815937</v>
       </c>
       <c r="AI25" t="n">
-        <v>194907.3735242072</v>
+        <v>737728.202978321</v>
       </c>
       <c r="AJ25" t="n">
-        <v>281535.2184162618</v>
+        <v>191411.3944304526</v>
       </c>
       <c r="AK25" t="n">
-        <v>274410.4770959603</v>
+        <v>186567.3941709226</v>
       </c>
       <c r="AL25" t="n">
-        <v>28168.7148036699</v>
+        <v>45924.55117661731</v>
       </c>
       <c r="AM25" t="n">
         <v>0</v>
@@ -3675,16 +3675,16 @@
         <v>5379293.100543143</v>
       </c>
       <c r="AI26" t="n">
-        <v>2970000</v>
+        <v>6949515.945421916</v>
       </c>
       <c r="AJ26" t="n">
-        <v>4090169.138379251</v>
+        <v>2998820.932478525</v>
       </c>
       <c r="AK26" t="n">
-        <v>1778714.107038585</v>
+        <v>1304113.574920718</v>
       </c>
       <c r="AL26" t="n">
-        <v>420000</v>
+        <v>534686.2334260278</v>
       </c>
       <c r="AM26" t="n">
         <v>0</v>
@@ -3805,16 +3805,16 @@
         <v>44372236.00074311</v>
       </c>
       <c r="AI27" t="n">
-        <v>428650000</v>
+        <v>465544678.9247984</v>
       </c>
       <c r="AJ27" t="n">
-        <v>51480000</v>
+        <v>66130130.22352899</v>
       </c>
       <c r="AK27" t="n">
-        <v>110663772.6149623</v>
+        <v>104359731.7686896</v>
       </c>
       <c r="AL27" t="n">
-        <v>55830000</v>
+        <v>72122753.40601987</v>
       </c>
       <c r="AM27" t="n">
         <v>31396593.56686974</v>
@@ -3923,16 +3923,16 @@
         <v>679343.7163057061</v>
       </c>
       <c r="AI28" t="n">
-        <v>155167.6573475633</v>
+        <v>1609335.789893933</v>
       </c>
       <c r="AJ28" t="n">
-        <v>1115368.332963969</v>
+        <v>1976227.69444532</v>
       </c>
       <c r="AK28" t="n">
-        <v>637505.4308941466</v>
+        <v>2090976.859295608</v>
       </c>
       <c r="AL28" t="n">
-        <v>123659.9608581709</v>
+        <v>552439.0138258884</v>
       </c>
       <c r="AM28" t="n">
         <v>0</v>
@@ -4041,16 +4041,16 @@
         <v>3875032.014437651</v>
       </c>
       <c r="AI29" t="n">
-        <v>665245.4543059705</v>
+        <v>1945476.688531577</v>
       </c>
       <c r="AJ29" t="n">
-        <v>3299816.79734101</v>
+        <v>3134453.072680521</v>
       </c>
       <c r="AK29" t="n">
-        <v>1936605.923669699</v>
+        <v>1839556.787791719</v>
       </c>
       <c r="AL29" t="n">
-        <v>768068.595544882</v>
+        <v>967506.5063046726</v>
       </c>
       <c r="AM29" t="n">
         <v>0</v>
@@ -4159,7 +4159,7 @@
         <v>45271.33903000611</v>
       </c>
       <c r="AI30" t="n">
-        <v>11160000</v>
+        <v>11189380.47217878</v>
       </c>
       <c r="AJ30" t="n">
         <v>0</v>
@@ -4407,16 +4407,16 @@
         <v>316899.3732100427</v>
       </c>
       <c r="AI32" t="n">
-        <v>326301.2978587025</v>
+        <v>455035.188426055</v>
       </c>
       <c r="AJ32" t="n">
-        <v>129706.144959586</v>
+        <v>133747.7982108226</v>
       </c>
       <c r="AK32" t="n">
-        <v>59744.3954033593</v>
+        <v>61606.03526630016</v>
       </c>
       <c r="AL32" t="n">
-        <v>29697.9527186565</v>
+        <v>30623.34316332531</v>
       </c>
       <c r="AM32" t="n">
         <v>0</v>
@@ -4797,16 +4797,16 @@
         <v>21635017.7407154</v>
       </c>
       <c r="AI35" t="n">
-        <v>23300000</v>
+        <v>28378772.73637203</v>
       </c>
       <c r="AJ35" t="n">
-        <v>20271494.21312547</v>
+        <v>34848486.54219296</v>
       </c>
       <c r="AK35" t="n">
-        <v>11586475.31158142</v>
+        <v>36871955.16286499</v>
       </c>
       <c r="AL35" t="n">
-        <v>9545500</v>
+        <v>9741622.178864015</v>
       </c>
       <c r="AM35" t="n">
         <v>0</v>
@@ -4927,16 +4927,16 @@
         <v>4368714592.205109</v>
       </c>
       <c r="AI36" t="n">
-        <v>1322217365.96472</v>
+        <v>1832714516.99946</v>
       </c>
       <c r="AJ36" t="n">
-        <v>5208736087.75141</v>
+        <v>4964986637.61377</v>
       </c>
       <c r="AK36" t="n">
-        <v>3619740381.475604</v>
+        <v>3450350012.53361</v>
       </c>
       <c r="AL36" t="n">
-        <v>2080450430.043601</v>
+        <v>1983093098.088497</v>
       </c>
       <c r="AM36" t="n">
         <v>960873819.1105907</v>
@@ -5045,16 +5045,16 @@
         <v>5316904.391902822</v>
       </c>
       <c r="AI37" t="n">
-        <v>3563181.818181818</v>
+        <v>5064603.899516638</v>
       </c>
       <c r="AJ37" t="n">
-        <v>1671496.605148022</v>
+        <v>1562489.813830086</v>
       </c>
       <c r="AK37" t="n">
-        <v>1431304.801028979</v>
+        <v>1337962.138365115</v>
       </c>
       <c r="AL37" t="n">
-        <v>2485516.065893085</v>
+        <v>5042621.375234686</v>
       </c>
       <c r="AM37" t="n">
         <v>0</v>
@@ -5163,13 +5163,13 @@
         <v>2086555.700081812</v>
       </c>
       <c r="AI38" t="n">
-        <v>8929012.345679013</v>
+        <v>10221578.22586605</v>
       </c>
       <c r="AJ38" t="n">
-        <v>24440</v>
+        <v>27977.94001943099</v>
       </c>
       <c r="AK38" t="n">
-        <v>400952.2338097586</v>
+        <v>458994.1713660514</v>
       </c>
       <c r="AL38" t="n">
         <v>0</v>
@@ -5281,10 +5281,10 @@
         <v>362170.7122400489</v>
       </c>
       <c r="AI39" t="n">
-        <v>13670000</v>
+        <v>13872460.5190593</v>
       </c>
       <c r="AJ39" t="n">
-        <v>2200000</v>
+        <v>2232583.258370919</v>
       </c>
       <c r="AK39" t="n">
         <v>0</v>
@@ -5399,16 +5399,16 @@
         <v>2842152.282503464</v>
       </c>
       <c r="AI40" t="n">
-        <v>1050000</v>
+        <v>2306032.276145094</v>
       </c>
       <c r="AJ40" t="n">
-        <v>1149144.187120315</v>
+        <v>923445.5534448812</v>
       </c>
       <c r="AK40" t="n">
-        <v>984013.7198209835</v>
+        <v>790747.6749062696</v>
       </c>
       <c r="AL40" t="n">
-        <v>1708777.828395444</v>
+        <v>2933030.901042315</v>
       </c>
       <c r="AM40" t="n">
         <v>0</v>
@@ -5529,16 +5529,16 @@
         <v>21330006.27625161</v>
       </c>
       <c r="AI41" t="n">
-        <v>56190000</v>
+        <v>75664835.33247449</v>
       </c>
       <c r="AJ41" t="n">
-        <v>5798561.764705882</v>
+        <v>1970680.179046663</v>
       </c>
       <c r="AK41" t="n">
-        <v>329700</v>
+        <v>10673064.33253591</v>
       </c>
       <c r="AL41" t="n">
-        <v>2270000</v>
+        <v>0</v>
       </c>
       <c r="AM41" t="n">
         <v>0</v>
@@ -5647,16 +5647,16 @@
         <v>97049.10232938659</v>
       </c>
       <c r="AI42" t="n">
-        <v>21866.8150756777</v>
+        <v>78742.56552690566</v>
       </c>
       <c r="AJ42" t="n">
-        <v>43422.61189499523</v>
+        <v>31532.2871908008</v>
       </c>
       <c r="AK42" t="n">
-        <v>37182.84122570554</v>
+        <v>27001.14011875065</v>
       </c>
       <c r="AL42" t="n">
-        <v>64569.43983951026</v>
+        <v>100152.2746697376</v>
       </c>
       <c r="AM42" t="n">
         <v>0</v>
@@ -5765,16 +5765,16 @@
         <v>249554.8345612798</v>
       </c>
       <c r="AI43" t="n">
-        <v>56228.95305174265</v>
+        <v>190453.7965394298</v>
       </c>
       <c r="AJ43" t="n">
-        <v>111658.1448728449</v>
+        <v>95802.76622331506</v>
       </c>
       <c r="AK43" t="n">
-        <v>95613.0202946714</v>
+        <v>82036.03813789655</v>
       </c>
       <c r="AL43" t="n">
-        <v>166035.7024444549</v>
+        <v>242237.2298295735</v>
       </c>
       <c r="AM43" t="n">
         <v>0</v>
@@ -5895,16 +5895,16 @@
         <v>6932.078737813327</v>
       </c>
       <c r="AI44" t="n">
-        <v>8540000</v>
+        <v>8398729.671264056</v>
       </c>
       <c r="AJ44" t="n">
-        <v>80000</v>
+        <v>834570.3748797921</v>
       </c>
       <c r="AK44" t="n">
-        <v>1507443.902439024</v>
+        <v>2075805.590004949</v>
       </c>
       <c r="AL44" t="n">
-        <v>1590000</v>
+        <v>1880582.61760156</v>
       </c>
       <c r="AM44" t="n">
         <v>0</v>
@@ -6013,16 +6013,16 @@
         <v>10100038.72099402</v>
       </c>
       <c r="AI45" t="n">
-        <v>6026817.754243349</v>
+        <v>15446280.03032581</v>
       </c>
       <c r="AJ45" t="n">
-        <v>5499566.079719725</v>
+        <v>3958503.066806858</v>
       </c>
       <c r="AK45" t="n">
-        <v>3856468.412982428</v>
+        <v>2775826.641328894</v>
       </c>
       <c r="AL45" t="n">
-        <v>2001416.939360924</v>
+        <v>1440589.126046681</v>
       </c>
       <c r="AM45" t="n">
         <v>0</v>
@@ -6131,16 +6131,16 @@
         <v>471381.3541713062</v>
       </c>
       <c r="AI46" t="n">
-        <v>107667.3540779011</v>
+        <v>1116681.976661096</v>
       </c>
       <c r="AJ46" t="n">
-        <v>773929.0473627541</v>
+        <v>1371260.032880426</v>
       </c>
       <c r="AK46" t="n">
-        <v>442350.7071510406</v>
+        <v>1450881.902368381</v>
       </c>
       <c r="AL46" t="n">
-        <v>85804.87079954716</v>
+        <v>383325.0300016369</v>
       </c>
       <c r="AM46" t="n">
         <v>0</v>
@@ -6521,16 +6521,16 @@
         <v>155826197.9473058</v>
       </c>
       <c r="AI49" t="n">
-        <v>23906116.72473868</v>
+        <v>29028954.22906934</v>
       </c>
       <c r="AJ49" t="n">
-        <v>60723208.62802869</v>
+        <v>195532749.300047</v>
       </c>
       <c r="AK49" t="n">
-        <v>137480000</v>
+        <v>348493836.6139858</v>
       </c>
       <c r="AL49" t="n">
-        <v>46100000</v>
+        <v>0</v>
       </c>
       <c r="AM49" t="n">
         <v>0</v>
@@ -6757,16 +6757,16 @@
         <v>90117.02359157326</v>
       </c>
       <c r="AI51" t="n">
-        <v>53773.94015453914</v>
+        <v>137818.5589528041</v>
       </c>
       <c r="AJ51" t="n">
-        <v>49069.56694327825</v>
+        <v>35319.51947047984</v>
       </c>
       <c r="AK51" t="n">
-        <v>34409.12104925982</v>
+        <v>24767.15603107454</v>
       </c>
       <c r="AL51" t="n">
-        <v>17857.5293148195</v>
+        <v>12853.57490638768</v>
       </c>
       <c r="AM51" t="n">
         <v>0</v>
@@ -6890,13 +6890,13 @@
         <v>20000</v>
       </c>
       <c r="AJ52" t="n">
-        <v>58186442.32141066</v>
+        <v>58263729.25691126</v>
       </c>
       <c r="AK52" t="n">
-        <v>64926062.68918277</v>
+        <v>65012301.61734492</v>
       </c>
       <c r="AL52" t="n">
-        <v>9022474.348981006</v>
+        <v>8858948.485318279</v>
       </c>
       <c r="AM52" t="n">
         <v>0</v>
@@ -7005,16 +7005,16 @@
         <v>14106178.57933326</v>
       </c>
       <c r="AI53" t="n">
-        <v>8417330.849409444</v>
+        <v>21572985.06601379</v>
       </c>
       <c r="AJ53" t="n">
-        <v>7680946.912422839</v>
+        <v>5528627.434976835</v>
       </c>
       <c r="AK53" t="n">
-        <v>5386121.144863701</v>
+        <v>3876847.147770394</v>
       </c>
       <c r="AL53" t="n">
-        <v>2795270.942837458</v>
+        <v>2011993.026246551</v>
       </c>
       <c r="AM53" t="n">
         <v>0</v>
@@ -7135,7 +7135,7 @@
         <v>66125099.08000133</v>
       </c>
       <c r="AI54" t="n">
-        <v>26461.53846153846</v>
+        <v>26461.53846153845</v>
       </c>
       <c r="AJ54" t="n">
         <v>92507226.5518977</v>
@@ -7265,16 +7265,16 @@
         <v>5497138.439085968</v>
       </c>
       <c r="AI55" t="n">
-        <v>26047287.09055877</v>
+        <v>14715917.85222422</v>
       </c>
       <c r="AJ55" t="n">
-        <v>59199.99999999999</v>
+        <v>324821.052044176</v>
       </c>
       <c r="AK55" t="n">
-        <v>60000</v>
+        <v>167050.8267655763</v>
       </c>
       <c r="AL55" t="n">
-        <v>390000</v>
+        <v>4718837.833571768</v>
       </c>
       <c r="AM55" t="n">
         <v>0</v>
@@ -7395,16 +7395,16 @@
         <v>123890111.2021998</v>
       </c>
       <c r="AI56" t="n">
-        <v>15329222.78150617</v>
+        <v>15372584.08323733</v>
       </c>
       <c r="AJ56" t="n">
-        <v>124694154.956249</v>
+        <v>125046873.4830938</v>
       </c>
       <c r="AK56" t="n">
-        <v>72615808.18542698</v>
+        <v>72821214.29205483</v>
       </c>
       <c r="AL56" t="n">
-        <v>601485.9352038689</v>
+        <v>0</v>
       </c>
       <c r="AM56" t="n">
         <v>0</v>
@@ -7513,16 +7513,16 @@
         <v>270351.0707747198</v>
       </c>
       <c r="AI57" t="n">
-        <v>278371.9777596751</v>
+        <v>404598.2023878155</v>
       </c>
       <c r="AJ57" t="n">
-        <v>110654.0376545428</v>
+        <v>104394.488304592</v>
       </c>
       <c r="AK57" t="n">
-        <v>50968.7384562317</v>
+        <v>48085.5058111876</v>
       </c>
       <c r="AL57" t="n">
-        <v>25335.71851524047</v>
+        <v>23902.51116262925</v>
       </c>
       <c r="AM57" t="n">
         <v>0</v>
@@ -7643,16 +7643,16 @@
         <v>54884397.71935956</v>
       </c>
       <c r="AI58" t="n">
-        <v>25000000</v>
+        <v>21579417.01368233</v>
       </c>
       <c r="AJ58" t="n">
-        <v>449506604.4545861</v>
+        <v>451711714.9137219</v>
       </c>
       <c r="AK58" t="n">
-        <v>211350745.3708981</v>
+        <v>212387552.6937381</v>
       </c>
       <c r="AL58" t="n">
-        <v>36420483.61123092</v>
+        <v>36599148.81557281</v>
       </c>
       <c r="AM58" t="n">
         <v>128032235.0113396</v>
@@ -7903,16 +7903,16 @@
         <v>452713.3903000611</v>
       </c>
       <c r="AI60" t="n">
-        <v>17620000</v>
+        <v>61146290.42179304</v>
       </c>
       <c r="AJ60" t="n">
-        <v>40000</v>
+        <v>4838558.411842873</v>
       </c>
       <c r="AK60" t="n">
-        <v>987000</v>
+        <v>4233738.610362514</v>
       </c>
       <c r="AL60" t="n">
-        <v>40000</v>
+        <v>302409.9007401796</v>
       </c>
       <c r="AM60" t="n">
         <v>0</v>
@@ -8033,16 +8033,16 @@
         <v>3403650.660266344</v>
       </c>
       <c r="AI61" t="n">
-        <v>52298572.39484636</v>
+        <v>53968072.14265956</v>
       </c>
       <c r="AJ61" t="n">
-        <v>92868442.7981234</v>
+        <v>95833033.12500104</v>
       </c>
       <c r="AK61" t="n">
-        <v>231928481.4194311</v>
+        <v>239332212.0283108</v>
       </c>
       <c r="AL61" t="n">
-        <v>12037820.68357059</v>
+        <v>0</v>
       </c>
       <c r="AM61" t="n">
         <v>78163006.78725894</v>
@@ -8151,16 +8151,16 @@
         <v>291147.3069881598</v>
       </c>
       <c r="AI62" t="n">
-        <v>600000</v>
+        <v>747216.005330661</v>
       </c>
       <c r="AJ62" t="n">
-        <v>10000</v>
+        <v>12453.60008884435</v>
       </c>
       <c r="AK62" t="n">
-        <v>40095.22338097586</v>
+        <v>49932.98774595551</v>
       </c>
       <c r="AL62" t="n">
-        <v>120000</v>
+        <v>149443.2010661322</v>
       </c>
       <c r="AM62" t="n">
         <v>0</v>
@@ -8281,16 +8281,16 @@
         <v>29378149.69085288</v>
       </c>
       <c r="AI63" t="n">
-        <v>333438726.958516</v>
+        <v>334362509.4076936</v>
       </c>
       <c r="AJ63" t="n">
-        <v>1975163011.380707</v>
+        <v>1980635143.969569</v>
       </c>
       <c r="AK63" t="n">
-        <v>1474148043.967093</v>
+        <v>1478232128.929053</v>
       </c>
       <c r="AL63" t="n">
-        <v>10480000</v>
+        <v>0</v>
       </c>
       <c r="AM63" t="n">
         <v>763258542.9726716</v>
@@ -8399,16 +8399,16 @@
         <v>180234.0471831465</v>
       </c>
       <c r="AI64" t="n">
-        <v>130000</v>
+        <v>226794.7947868362</v>
       </c>
       <c r="AJ64" t="n">
-        <v>10526.09931581706</v>
+        <v>84407.19096721441</v>
       </c>
       <c r="AK64" t="n">
-        <v>166500</v>
+        <v>208201.7477388646</v>
       </c>
       <c r="AL64" t="n">
-        <v>3194.215607976371</v>
+        <v>64582.19134751985</v>
       </c>
       <c r="AM64" t="n">
         <v>0</v>
@@ -8517,16 +8517,16 @@
         <v>1150725.070477012</v>
       </c>
       <c r="AI65" t="n">
-        <v>1520000</v>
+        <v>1739613.246072689</v>
       </c>
       <c r="AJ65" t="n">
-        <v>197220.422204629</v>
+        <v>225715.3018836979</v>
       </c>
       <c r="AK65" t="n">
-        <v>216122.9859398687</v>
+        <v>247348.9533695903</v>
       </c>
       <c r="AL65" t="n">
-        <v>47293.98713818335</v>
+        <v>54127.13584550996</v>
       </c>
       <c r="AM65" t="n">
         <v>0</v>
@@ -8647,16 +8647,16 @@
         <v>76148884.93487941</v>
       </c>
       <c r="AI66" t="n">
-        <v>9145301.369863015</v>
+        <v>9145301.369863013</v>
       </c>
       <c r="AJ66" t="n">
-        <v>174602909.5935899</v>
+        <v>183549484.7856476</v>
       </c>
       <c r="AK66" t="n">
-        <v>488946973.8805</v>
+        <v>514000398.6884423</v>
       </c>
       <c r="AL66" t="n">
-        <v>34000000</v>
+        <v>0</v>
       </c>
       <c r="AM66" t="n">
         <v>97981601.96125028</v>
@@ -8777,13 +8777,13 @@
         <v>2391567.164545598</v>
       </c>
       <c r="AI67" t="n">
-        <v>10860000</v>
+        <v>13715187.19592379</v>
       </c>
       <c r="AJ67" t="n">
-        <v>113254.0581082244</v>
+        <v>1126912.834928255</v>
       </c>
       <c r="AK67" t="n">
-        <v>93150</v>
+        <v>3683615.179542731</v>
       </c>
       <c r="AL67" t="n">
         <v>0</v>
@@ -8907,16 +8907,16 @@
         <v>10349593.5555553</v>
       </c>
       <c r="AI68" t="n">
-        <v>9213265.822784809</v>
+        <v>2331939.636284772</v>
       </c>
       <c r="AJ68" t="n">
-        <v>2572468.747643123</v>
+        <v>4630711.397087707</v>
       </c>
       <c r="AK68" t="n">
-        <v>2202808.463779406</v>
+        <v>3965284.424998457</v>
       </c>
       <c r="AL68" t="n">
-        <v>3825261.9727628</v>
+        <v>6885869.548599202</v>
       </c>
       <c r="AM68" t="n">
         <v>0</v>
@@ -9025,10 +9025,10 @@
         <v>707072.0312569594</v>
       </c>
       <c r="AI69" t="n">
-        <v>3018518.518518519</v>
+        <v>3472882.709492589</v>
       </c>
       <c r="AJ69" t="n">
-        <v>30000</v>
+        <v>34515.76680599996</v>
       </c>
       <c r="AK69" t="n">
         <v>0</v>
@@ -9143,16 +9143,16 @@
         <v>353536.0156284797</v>
       </c>
       <c r="AI70" t="n">
-        <v>364024.8939934213</v>
+        <v>554093.005508341</v>
       </c>
       <c r="AJ70" t="n">
-        <v>144701.4338559406</v>
+        <v>121717.460294187</v>
       </c>
       <c r="AK70" t="n">
-        <v>66651.42721199531</v>
+        <v>56064.69976865315</v>
       </c>
       <c r="AL70" t="n">
-        <v>33131.32421223754</v>
+        <v>27868.83676157367</v>
       </c>
       <c r="AM70" t="n">
         <v>0</v>
@@ -9261,16 +9261,16 @@
         <v>55456.62990250662</v>
       </c>
       <c r="AI71" t="n">
-        <v>57101.9441558308</v>
+        <v>73185.56187347656</v>
       </c>
       <c r="AJ71" t="n">
-        <v>22698.26413426519</v>
+        <v>27219.81502035261</v>
       </c>
       <c r="AK71" t="n">
-        <v>10455.12583717574</v>
+        <v>12537.81300715512</v>
       </c>
       <c r="AL71" t="n">
-        <v>5197.070464664713</v>
+        <v>6232.339876702693</v>
       </c>
       <c r="AM71" t="n">
         <v>0</v>
@@ -9509,16 +9509,16 @@
         <v>17018253.30133172</v>
       </c>
       <c r="AI73" t="n">
-        <v>3820000</v>
+        <v>5505815.700854395</v>
       </c>
       <c r="AJ73" t="n">
-        <v>12811568.58009193</v>
+        <v>20318059.32204125</v>
       </c>
       <c r="AK73" t="n">
-        <v>11114970.11494253</v>
+        <v>25855001.72575799</v>
       </c>
       <c r="AL73" t="n">
-        <v>1545417.964116031</v>
+        <v>6179629.533354243</v>
       </c>
       <c r="AM73" t="n">
         <v>0</v>
@@ -9627,16 +9627,16 @@
         <v>166369.8897075198</v>
       </c>
       <c r="AI74" t="n">
-        <v>99274.96643914917</v>
+        <v>254434.2626820999</v>
       </c>
       <c r="AJ74" t="n">
-        <v>90589.96974143677</v>
+        <v>65205.26671473201</v>
       </c>
       <c r="AK74" t="n">
-        <v>63524.53116786428</v>
+        <v>45723.98036506068</v>
       </c>
       <c r="AL74" t="n">
-        <v>32967.74642735907</v>
+        <v>23729.67675025418</v>
       </c>
       <c r="AM74" t="n">
         <v>0</v>
@@ -9745,7 +9745,7 @@
         <v>48524.55116469329</v>
       </c>
       <c r="AI75" t="n">
-        <v>470000.0000000001</v>
+        <v>501491.7618084364</v>
       </c>
       <c r="AJ75" t="n">
         <v>0</v>
@@ -9863,16 +9863,16 @@
         <v>2377703.007069971</v>
       </c>
       <c r="AI76" t="n">
-        <v>5650000</v>
+        <v>6512413.058779763</v>
       </c>
       <c r="AJ76" t="n">
-        <v>319418.1818181819</v>
+        <v>368174.0068114011</v>
       </c>
       <c r="AK76" t="n">
-        <v>340000</v>
+        <v>391897.4230062158</v>
       </c>
       <c r="AL76" t="n">
-        <v>3800000</v>
+        <v>4380030.021834177</v>
       </c>
       <c r="AM76" t="n">
         <v>0</v>
@@ -9981,16 +9981,16 @@
         <v>1150725.070477012</v>
       </c>
       <c r="AI77" t="n">
-        <v>197550.5284701092</v>
+        <v>577726.5300469435</v>
       </c>
       <c r="AJ77" t="n">
-        <v>979909.8181728218</v>
+        <v>930803.595822838</v>
       </c>
       <c r="AK77" t="n">
-        <v>575092.2778697135</v>
+        <v>546272.6775911009</v>
       </c>
       <c r="AL77" t="n">
-        <v>228084.7707700364</v>
+        <v>287309.6244124786</v>
       </c>
       <c r="AM77" t="n">
         <v>0</v>
@@ -10099,16 +10099,16 @@
         <v>859577.7634888527</v>
       </c>
       <c r="AI78" t="n">
-        <v>196334.5868479372</v>
+        <v>2036302.428029059</v>
       </c>
       <c r="AJ78" t="n">
-        <v>1411282.380485022</v>
+        <v>2500533.001134895</v>
       </c>
       <c r="AK78" t="n">
-        <v>806639.5248048386</v>
+        <v>2645725.821965872</v>
       </c>
       <c r="AL78" t="n">
-        <v>156467.7055756448</v>
+        <v>699004.4664735734</v>
       </c>
       <c r="AM78" t="n">
         <v>0</v>
@@ -10217,16 +10217,16 @@
         <v>29013911.60171209</v>
       </c>
       <c r="AI79" t="n">
-        <v>4980958.281831192</v>
+        <v>14566560.59974209</v>
       </c>
       <c r="AJ79" t="n">
-        <v>24707045.64586435</v>
+        <v>23468901.42626736</v>
       </c>
       <c r="AK79" t="n">
-        <v>14500141.64201912</v>
+        <v>13773496.01976486</v>
       </c>
       <c r="AL79" t="n">
-        <v>5750836.187200981</v>
+        <v>7244107.440510729</v>
       </c>
       <c r="AM79" t="n">
         <v>0</v>
@@ -10335,16 +10335,16 @@
         <v>4133528.895671517</v>
       </c>
       <c r="AI80" t="n">
-        <v>3880000</v>
+        <v>3846829.506704148</v>
       </c>
       <c r="AJ80" t="n">
-        <v>1139237.364333272</v>
+        <v>2211816.971366774</v>
       </c>
       <c r="AK80" t="n">
-        <v>495426.351001223</v>
+        <v>961864.8804133275</v>
       </c>
       <c r="AL80" t="n">
-        <v>1600000</v>
+        <v>2036899.936861058</v>
       </c>
       <c r="AM80" t="n">
         <v>0</v>
@@ -10465,16 +10465,16 @@
         <v>3611613.022400744</v>
       </c>
       <c r="AI81" t="n">
-        <v>8160000</v>
+        <v>10083528.04372868</v>
       </c>
       <c r="AJ81" t="n">
-        <v>410000</v>
+        <v>976493.1134845085</v>
       </c>
       <c r="AK81" t="n">
-        <v>2380000</v>
+        <v>6104121.337378218</v>
       </c>
       <c r="AL81" t="n">
-        <v>1122200</v>
+        <v>1776370.29238175</v>
       </c>
       <c r="AM81" t="n">
         <v>0</v>
@@ -10583,16 +10583,16 @@
         <v>568430.4565006929</v>
       </c>
       <c r="AI82" t="n">
-        <v>306805.2450829783</v>
+        <v>744932.2897621936</v>
       </c>
       <c r="AJ82" t="n">
-        <v>440559.729087295</v>
+        <v>328405.3642196809</v>
       </c>
       <c r="AK82" t="n">
-        <v>191588.6063898047</v>
+        <v>142815.4275292779</v>
       </c>
       <c r="AL82" t="n">
-        <v>39433.56650727055</v>
+        <v>29394.86729331807</v>
       </c>
       <c r="AM82" t="n">
         <v>0</v>
@@ -10843,16 +10843,16 @@
         <v>206945379.503622</v>
       </c>
       <c r="AI84" t="n">
-        <v>36584532.4412485</v>
+        <v>52951917.40412979</v>
       </c>
       <c r="AJ84" t="n">
-        <v>147602504.6099716</v>
+        <v>140043744.4683294</v>
       </c>
       <c r="AK84" t="n">
-        <v>60123516.89497874</v>
+        <v>57044576.97941303</v>
       </c>
       <c r="AL84" t="n">
-        <v>111885524.4584629</v>
+        <v>106155839.5527894</v>
       </c>
       <c r="AM84" t="n">
         <v>0</v>
@@ -10973,16 +10973,16 @@
         <v>1080397389.78271</v>
       </c>
       <c r="AI85" t="n">
-        <v>149170000</v>
+        <v>206436403.9721107</v>
       </c>
       <c r="AJ85" t="n">
-        <v>1761743809.638026</v>
+        <v>1716419575.178646</v>
       </c>
       <c r="AK85" t="n">
-        <v>388787449.2387473</v>
+        <v>378785147.3105333</v>
       </c>
       <c r="AL85" t="n">
-        <v>75402259.94554318</v>
+        <v>73462392.36102696</v>
       </c>
       <c r="AM85" t="n">
         <v>105131268.5592117</v>
@@ -11103,16 +11103,16 @@
         <v>11964767.9014658</v>
       </c>
       <c r="AI86" t="n">
-        <v>1652833.333333333</v>
+        <v>1953571.186178154</v>
       </c>
       <c r="AJ86" t="n">
-        <v>4981270.532914812</v>
+        <v>8305615.120194698</v>
       </c>
       <c r="AK86" t="n">
-        <v>13018101.11509085</v>
+        <v>40181484.74716677</v>
       </c>
       <c r="AL86" t="n">
-        <v>941651.3093712942</v>
+        <v>0</v>
       </c>
       <c r="AM86" t="n">
         <v>0</v>
@@ -11469,16 +11469,16 @@
         <v>588527.4073900793</v>
       </c>
       <c r="AI89" t="n">
-        <v>14100000</v>
+        <v>13519332.84814011</v>
       </c>
       <c r="AJ89" t="n">
-        <v>18875.67635137073</v>
+        <v>19253.80517362235</v>
       </c>
       <c r="AK89" t="n">
         <v>0</v>
       </c>
       <c r="AL89" t="n">
-        <v>6163413.157894736</v>
+        <v>5909591.061147892</v>
       </c>
       <c r="AM89" t="n">
         <v>0</v>
@@ -11602,13 +11602,13 @@
         <v>2151804.377303027</v>
       </c>
       <c r="AJ90" t="n">
-        <v>79232305.63592936</v>
+        <v>79338754.78813301</v>
       </c>
       <c r="AK90" t="n">
-        <v>2642969.455789121</v>
+        <v>2646520.303585494</v>
       </c>
       <c r="AL90" t="n">
-        <v>110000</v>
+        <v>0</v>
       </c>
       <c r="AM90" t="n">
         <v>0</v>
@@ -11729,16 +11729,16 @@
         <v>100535937.9345067</v>
       </c>
       <c r="AI91" t="n">
-        <v>40520000</v>
+        <v>63808175.17649979</v>
       </c>
       <c r="AJ91" t="n">
-        <v>81546901.41540757</v>
+        <v>84481931.72683112</v>
       </c>
       <c r="AK91" t="n">
-        <v>29276376.55919918</v>
+        <v>82922699.5119182</v>
       </c>
       <c r="AL91" t="n">
-        <v>21700000</v>
+        <v>33422289.8820256</v>
       </c>
       <c r="AM91" t="n">
         <v>0</v>
@@ -11847,16 +11847,16 @@
         <v>2710442.786485011</v>
       </c>
       <c r="AI92" t="n">
-        <v>1617354.661571139</v>
+        <v>4145158.196195879</v>
       </c>
       <c r="AJ92" t="n">
-        <v>1475861.590370907</v>
+        <v>1062302.470227509</v>
       </c>
       <c r="AK92" t="n">
-        <v>1034920.486943122</v>
+        <v>744919.84678078</v>
       </c>
       <c r="AL92" t="n">
-        <v>537099.5355457249</v>
+        <v>386595.9837228908</v>
       </c>
       <c r="AM92" t="n">
         <v>0</v>
@@ -11977,16 +11977,16 @@
         <v>12034607.06110353</v>
       </c>
       <c r="AI93" t="n">
-        <v>415101.4651487241</v>
+        <v>414887.4577948773</v>
       </c>
       <c r="AJ93" t="n">
-        <v>13314972.2394942</v>
+        <v>13308107.64802739</v>
       </c>
       <c r="AK93" t="n">
-        <v>6937722.169514919</v>
+        <v>6934145.396875269</v>
       </c>
       <c r="AL93" t="n">
-        <v>46268.14886183607</v>
+        <v>56923.52032213588</v>
       </c>
       <c r="AM93" t="n">
         <v>0</v>
@@ -12225,16 +12225,16 @@
         <v>67281383.43917617</v>
       </c>
       <c r="AI95" t="n">
-        <v>44752005.64465312</v>
+        <v>67253375.15974137</v>
       </c>
       <c r="AJ95" t="n">
-        <v>37427652.36266184</v>
+        <v>32115316.83336372</v>
       </c>
       <c r="AK95" t="n">
-        <v>29090991.60129336</v>
+        <v>24961929.30348716</v>
       </c>
       <c r="AL95" t="n">
-        <v>4534617.405123006</v>
+        <v>3890991.432550907</v>
       </c>
       <c r="AM95" t="n">
         <v>0</v>
@@ -12473,7 +12473,7 @@
         <v>1252395.558631608</v>
       </c>
       <c r="AI97" t="n">
-        <v>11760000</v>
+        <v>12572787.37619869</v>
       </c>
       <c r="AJ97" t="n">
         <v>0</v>
@@ -12603,16 +12603,16 @@
         <v>5498730.420466315</v>
       </c>
       <c r="AI98" t="n">
-        <v>5344095.802472071</v>
+        <v>5586454.706201179</v>
       </c>
       <c r="AJ98" t="n">
-        <v>2770609.035784183</v>
+        <v>2896258.311806518</v>
       </c>
       <c r="AK98" t="n">
-        <v>1149458.695866076</v>
+        <v>1201587.542299392</v>
       </c>
       <c r="AL98" t="n">
-        <v>200296.2024152406</v>
+        <v>209379.791076957</v>
       </c>
       <c r="AM98" t="n">
         <v>0</v>
@@ -12839,16 +12839,16 @@
         <v>145573.6534940799</v>
       </c>
       <c r="AI100" t="n">
-        <v>33250.21228876356</v>
+        <v>344857.6692629857</v>
       </c>
       <c r="AJ100" t="n">
-        <v>239007.4999208505</v>
+        <v>423477.3630954258</v>
       </c>
       <c r="AK100" t="n">
-        <v>136608.3066201743</v>
+        <v>448066.4698490589</v>
       </c>
       <c r="AL100" t="n">
-        <v>26498.56304103662</v>
+        <v>118379.7886769761</v>
       </c>
       <c r="AM100" t="n">
         <v>0</v>
@@ -13087,16 +13087,16 @@
         <v>57993770.72054631</v>
       </c>
       <c r="AI102" t="n">
-        <v>448205.868953007</v>
+        <v>903217.1789730818</v>
       </c>
       <c r="AJ102" t="n">
-        <v>87534511.79552689</v>
+        <v>87133699.34247705</v>
       </c>
       <c r="AK102" t="n">
-        <v>11484471.52194421</v>
+        <v>11431885.18647182</v>
       </c>
       <c r="AL102" t="n">
-        <v>352162.9155934193</v>
+        <v>350550.3940955912</v>
       </c>
       <c r="AM102" t="n">
         <v>0</v>
@@ -13217,16 +13217,16 @@
         <v>8443271.902656633</v>
       </c>
       <c r="AI103" t="n">
-        <v>40000000</v>
+        <v>76862963.53583883</v>
       </c>
       <c r="AJ103" t="n">
-        <v>90266.66666666667</v>
+        <v>2276011.433750326</v>
       </c>
       <c r="AK103" t="n">
-        <v>0</v>
+        <v>1446428.780784499</v>
       </c>
       <c r="AL103" t="n">
-        <v>40000</v>
+        <v>43696.92256100277</v>
       </c>
       <c r="AM103" t="n">
         <v>0</v>
@@ -13453,16 +13453,16 @@
         <v>180234.0471831465</v>
       </c>
       <c r="AI105" t="n">
-        <v>185581.3185064501</v>
+        <v>289732.8363783678</v>
       </c>
       <c r="AJ105" t="n">
-        <v>73769.35843636187</v>
+        <v>57758.62660678953</v>
       </c>
       <c r="AK105" t="n">
-        <v>33979.15897082115</v>
+        <v>26604.40048562244</v>
       </c>
       <c r="AL105" t="n">
-        <v>16890.47901016032</v>
+        <v>13224.60830670305</v>
       </c>
       <c r="AM105" t="n">
         <v>0</v>
@@ -13571,16 +13571,16 @@
         <v>26537839.08130562</v>
       </c>
       <c r="AI106" t="n">
-        <v>5574.120641983649</v>
+        <v>5906.092935962078</v>
       </c>
       <c r="AJ106" t="n">
-        <v>37129821.6457333</v>
+        <v>37129551.76073276</v>
       </c>
       <c r="AK106" t="n">
-        <v>6674352.254827492</v>
+        <v>6674303.741059256</v>
       </c>
       <c r="AL106" t="n">
-        <v>1867397.478581571</v>
+        <v>1867383.905056378</v>
       </c>
       <c r="AM106" t="n">
         <v>0</v>
@@ -13689,16 +13689,16 @@
         <v>270351.0707747198</v>
       </c>
       <c r="AI107" t="n">
-        <v>161321.8204636174</v>
+        <v>413455.6768584124</v>
       </c>
       <c r="AJ107" t="n">
-        <v>147208.7008298347</v>
+        <v>105958.5584114395</v>
       </c>
       <c r="AK107" t="n">
-        <v>103227.3631477794</v>
+        <v>74301.46809322364</v>
       </c>
       <c r="AL107" t="n">
-        <v>53572.58794445849</v>
+        <v>38560.72471916304</v>
       </c>
       <c r="AM107" t="n">
         <v>0</v>
@@ -13819,16 +13819,16 @@
         <v>7654539.272409679</v>
       </c>
       <c r="AI108" t="n">
-        <v>6060000</v>
+        <v>9176597.972195083</v>
       </c>
       <c r="AJ108" t="n">
-        <v>4236133.872258364</v>
+        <v>6013375.04218645</v>
       </c>
       <c r="AK108" t="n">
-        <v>2761133.962436917</v>
+        <v>7255757.490126238</v>
       </c>
       <c r="AL108" t="n">
-        <v>117787.7155499488</v>
+        <v>421585.0276629135</v>
       </c>
       <c r="AM108" t="n">
         <v>0</v>
@@ -14067,16 +14067,16 @@
         <v>402060.566793173</v>
       </c>
       <c r="AI110" t="n">
-        <v>3753750</v>
+        <v>3335049.847929229</v>
       </c>
       <c r="AJ110" t="n">
-        <v>690000</v>
+        <v>3076328.763119557</v>
       </c>
       <c r="AK110" t="n">
-        <v>2450000</v>
+        <v>12383939.32318082</v>
       </c>
       <c r="AL110" t="n">
-        <v>815825.6546856471</v>
+        <v>0</v>
       </c>
       <c r="AM110" t="n">
         <v>0</v>
@@ -14197,16 +14197,16 @@
         <v>103981.1810671999</v>
       </c>
       <c r="AI111" t="n">
-        <v>3882000</v>
+        <v>123324.1891378865</v>
       </c>
       <c r="AJ111" t="n">
-        <v>290000</v>
+        <v>859445.318100465</v>
       </c>
       <c r="AK111" t="n">
-        <v>490000.0000000001</v>
+        <v>1030037.261549393</v>
       </c>
       <c r="AL111" t="n">
-        <v>397912.8273428236</v>
+        <v>490722.7677961756</v>
       </c>
       <c r="AM111" t="n">
         <v>0</v>
@@ -14327,16 +14327,16 @@
         <v>1019041.98237756</v>
       </c>
       <c r="AI112" t="n">
-        <v>3790000</v>
+        <v>4703137.524421728</v>
       </c>
       <c r="AJ112" t="n">
-        <v>1429181.30510348</v>
+        <v>1534236.475426448</v>
       </c>
       <c r="AK112" t="n">
-        <v>1711961.871683812</v>
+        <v>1837803.460412926</v>
       </c>
       <c r="AL112" t="n">
-        <v>660000</v>
+        <v>834197.0533558771</v>
       </c>
       <c r="AM112" t="n">
         <v>0</v>
@@ -14445,16 +14445,16 @@
         <v>201030.2833965865</v>
       </c>
       <c r="AI113" t="n">
-        <v>34511.83931104319</v>
+        <v>100928.1287431407</v>
       </c>
       <c r="AJ113" t="n">
-        <v>171189.0646205532</v>
+        <v>162610.2667401343</v>
       </c>
       <c r="AK113" t="n">
-        <v>100467.9280615765</v>
+        <v>95433.17861531279</v>
       </c>
       <c r="AL113" t="n">
-        <v>39846.13465259673</v>
+        <v>50192.64522868601</v>
       </c>
       <c r="AM113" t="n">
         <v>0</v>
@@ -14823,16 +14823,16 @@
         <v>1185385.464166079</v>
       </c>
       <c r="AI116" t="n">
-        <v>1220554.056330883</v>
+        <v>1905550.577719265</v>
       </c>
       <c r="AJ116" t="n">
-        <v>485175.3958699185</v>
+        <v>379874.0442215775</v>
       </c>
       <c r="AK116" t="n">
-        <v>223478.3147696313</v>
+        <v>174975.0955015938</v>
       </c>
       <c r="AL116" t="n">
-        <v>111087.3811822082</v>
+        <v>86977.23155562393</v>
       </c>
       <c r="AM116" t="n">
         <v>0</v>
@@ -14941,16 +14941,16 @@
         <v>659435.8576546394</v>
       </c>
       <c r="AI117" t="n">
-        <v>340189.809035482</v>
+        <v>815309.3677071643</v>
       </c>
       <c r="AJ117" t="n">
-        <v>416367.8128257322</v>
+        <v>329836.4085208391</v>
       </c>
       <c r="AK117" t="n">
-        <v>298039.0274910608</v>
+        <v>236099.2358163852</v>
       </c>
       <c r="AL117" t="n">
-        <v>80429.73789734319</v>
+        <v>63714.47328335026</v>
       </c>
       <c r="AM117" t="n">
         <v>0</v>
@@ -15071,16 +15071,16 @@
         <v>184518071.8431152</v>
       </c>
       <c r="AI118" t="n">
-        <v>22195889.70206591</v>
+        <v>24081203.00751879</v>
       </c>
       <c r="AJ118" t="n">
-        <v>306013871.9894084</v>
+        <v>304662295.9132826</v>
       </c>
       <c r="AK118" t="n">
-        <v>109477544.5885376</v>
+        <v>108994013.4689288</v>
       </c>
       <c r="AL118" t="n">
-        <v>11367296.52425375</v>
+        <v>11317090.41453549</v>
       </c>
       <c r="AM118" t="n">
         <v>26809358.66943598</v>
@@ -15201,16 +15201,16 @@
         <v>3253579.609347244</v>
       </c>
       <c r="AI119" t="n">
-        <v>2092069.645603471</v>
+        <v>3651188.2747552</v>
       </c>
       <c r="AJ119" t="n">
-        <v>2196507.902434935</v>
+        <v>1780725.251800799</v>
       </c>
       <c r="AK119" t="n">
-        <v>1039457.16797361</v>
+        <v>842695.6375272046</v>
       </c>
       <c r="AL119" t="n">
-        <v>272053.0965625874</v>
+        <v>220555.463671477</v>
       </c>
       <c r="AM119" t="n">
         <v>0</v>
@@ -15319,16 +15319,16 @@
         <v>1733019.684453332</v>
       </c>
       <c r="AI120" t="n">
-        <v>1784435.754869712</v>
+        <v>2713199.248763638</v>
       </c>
       <c r="AJ120" t="n">
-        <v>709320.7541957871</v>
+        <v>598396.0350228033</v>
       </c>
       <c r="AK120" t="n">
-        <v>326722.6824117417</v>
+        <v>275629.2644064326</v>
       </c>
       <c r="AL120" t="n">
-        <v>162408.4520207723</v>
+        <v>137010.7573598451</v>
       </c>
       <c r="AM120" t="n">
         <v>0</v>
@@ -15579,16 +15579,16 @@
         <v>10931888.16953162</v>
       </c>
       <c r="AI122" t="n">
-        <v>10624462.96011247</v>
+        <v>28518865.75593789</v>
       </c>
       <c r="AJ122" t="n">
-        <v>5508178.402046115</v>
+        <v>243362.3950505636</v>
       </c>
       <c r="AK122" t="n">
-        <v>2285210.03174365</v>
+        <v>0</v>
       </c>
       <c r="AL122" t="n">
-        <v>398203.8612832362</v>
+        <v>0</v>
       </c>
       <c r="AM122" t="n">
         <v>0</v>
@@ -15709,16 +15709,16 @@
         <v>1162698.661024144</v>
       </c>
       <c r="AI123" t="n">
-        <v>2220000</v>
+        <v>4533390.243481529</v>
       </c>
       <c r="AJ123" t="n">
-        <v>20000</v>
+        <v>182741.8517988177</v>
       </c>
       <c r="AK123" t="n">
-        <v>340000</v>
+        <v>624609.7156721494</v>
       </c>
       <c r="AL123" t="n">
-        <v>0</v>
+        <v>122109.9055263712</v>
       </c>
       <c r="AM123" t="n">
         <v>0</v>
@@ -15827,16 +15827,16 @@
         <v>5924008.550835527</v>
       </c>
       <c r="AI124" t="n">
-        <v>1102262.022318216</v>
+        <v>1426676.862765646</v>
       </c>
       <c r="AJ124" t="n">
-        <v>4342245.172084616</v>
+        <v>4187345.308656837</v>
       </c>
       <c r="AK124" t="n">
-        <v>3017584.291249333</v>
+        <v>2909938.735535137</v>
       </c>
       <c r="AL124" t="n">
-        <v>1734360.444343044</v>
+        <v>1672491.02303759</v>
       </c>
       <c r="AM124" t="n">
         <v>0</v>
@@ -15945,16 +15945,16 @@
         <v>2121216.093770878</v>
       </c>
       <c r="AI125" t="n">
-        <v>16170000</v>
+        <v>17527549.59452603</v>
       </c>
       <c r="AJ125" t="n">
-        <v>97387.5</v>
+        <v>105563.6509670318</v>
       </c>
       <c r="AK125" t="n">
         <v>0</v>
       </c>
       <c r="AL125" t="n">
-        <v>130000</v>
+        <v>140914.127847148</v>
       </c>
       <c r="AM125" t="n">
         <v>0</v>
@@ -16063,16 +16063,16 @@
         <v>1227403.264322378</v>
       </c>
       <c r="AI126" t="n">
-        <v>276554.8527499732</v>
+        <v>965085.073387019</v>
       </c>
       <c r="AJ126" t="n">
-        <v>549176.1830462852</v>
+        <v>436481.0041289604</v>
       </c>
       <c r="AK126" t="n">
-        <v>470260.3074298847</v>
+        <v>373759.273481986</v>
       </c>
       <c r="AL126" t="n">
-        <v>816625.1859341976</v>
+        <v>1227486.87070012</v>
       </c>
       <c r="AM126" t="n">
         <v>0</v>
@@ -16299,16 +16299,16 @@
         <v>55456.62990250662</v>
       </c>
       <c r="AI128" t="n">
-        <v>1690000</v>
+        <v>1724756.62201225</v>
       </c>
       <c r="AJ128" t="n">
-        <v>10000</v>
+        <v>10205.66048527958</v>
       </c>
       <c r="AK128" t="n">
         <v>0</v>
       </c>
       <c r="AL128" t="n">
-        <v>50000</v>
+        <v>51028.30242639792</v>
       </c>
       <c r="AM128" t="n">
         <v>0</v>
@@ -16535,13 +16535,13 @@
         <v>27728.31495125331</v>
       </c>
       <c r="AI130" t="n">
-        <v>1320000</v>
+        <v>1332197.27477567</v>
       </c>
       <c r="AJ130" t="n">
-        <v>607466.6666666667</v>
+        <v>613079.8771593893</v>
       </c>
       <c r="AK130" t="n">
-        <v>20000</v>
+        <v>20184.80719357076</v>
       </c>
       <c r="AL130" t="n">
         <v>0</v>
@@ -16653,16 +16653,16 @@
         <v>1580513.952221439</v>
       </c>
       <c r="AI131" t="n">
-        <v>540000</v>
+        <v>793503.9087391761</v>
       </c>
       <c r="AJ131" t="n">
-        <v>1198252.910807171</v>
+        <v>1278453.13161209</v>
       </c>
       <c r="AK131" t="n">
-        <v>703234.096812138</v>
+        <v>750302.2318721144</v>
       </c>
       <c r="AL131" t="n">
-        <v>278906.5232508788</v>
+        <v>394618.0383496698</v>
       </c>
       <c r="AM131" t="n">
         <v>0</v>
@@ -16771,16 +16771,16 @@
         <v>495235.0079470887</v>
       </c>
       <c r="AI132" t="n">
-        <v>509927.8808957859</v>
+        <v>796108.4255105752</v>
       </c>
       <c r="AJ132" t="n">
-        <v>202698.4877854947</v>
+        <v>158705.2743567369</v>
       </c>
       <c r="AK132" t="n">
-        <v>93365.65053022643</v>
+        <v>73101.78455093126</v>
       </c>
       <c r="AL132" t="n">
-        <v>46410.52363611939</v>
+        <v>36337.69036552843</v>
       </c>
       <c r="AM132" t="n">
         <v>0</v>
@@ -16901,16 +16901,16 @@
         <v>23475479.95943453</v>
       </c>
       <c r="AI133" t="n">
-        <v>9570000</v>
+        <v>30953795.13450221</v>
       </c>
       <c r="AJ133" t="n">
-        <v>11295806.09663848</v>
+        <v>1390404.275885058</v>
       </c>
       <c r="AK133" t="n">
-        <v>3588348.551228366</v>
+        <v>441690.9361146545</v>
       </c>
       <c r="AL133" t="n">
-        <v>15952033.30508262</v>
+        <v>30345113.36524026</v>
       </c>
       <c r="AM133" t="n">
         <v>0</v>
@@ -17019,16 +17019,16 @@
         <v>1074472.204361066</v>
       </c>
       <c r="AI134" t="n">
-        <v>650000</v>
+        <v>808064.0019827753</v>
       </c>
       <c r="AJ134" t="n">
-        <v>77550</v>
+        <v>96408.25131348342</v>
       </c>
       <c r="AK134" t="n">
-        <v>560000</v>
+        <v>696178.2170928525</v>
       </c>
       <c r="AL134" t="n">
-        <v>1580000</v>
+        <v>1964217.112511977</v>
       </c>
       <c r="AM134" t="n">
         <v>0</v>
@@ -17149,16 +17149,16 @@
         <v>40892332.47436082</v>
       </c>
       <c r="AI135" t="n">
-        <v>70000</v>
+        <v>70563.07773152841</v>
       </c>
       <c r="AJ135" t="n">
-        <v>34261227.01033684</v>
+        <v>40858425.61703353</v>
       </c>
       <c r="AK135" t="n">
-        <v>55419993.31326406</v>
+        <v>66091435.48196096</v>
       </c>
       <c r="AL135" t="n">
-        <v>23382809.39000924</v>
+        <v>7023652.005595624</v>
       </c>
       <c r="AM135" t="n">
         <v>8718164.658704922</v>
@@ -17279,16 +17279,16 @@
         <v>1608242.267172692</v>
       </c>
       <c r="AI136" t="n">
-        <v>136710000</v>
+        <v>138723937.0295588</v>
       </c>
       <c r="AJ136" t="n">
-        <v>360000</v>
+        <v>3149233.347720816</v>
       </c>
       <c r="AK136" t="n">
-        <v>15981182.60869565</v>
+        <v>25274775.93892141</v>
       </c>
       <c r="AL136" t="n">
-        <v>389564.1367141178</v>
+        <v>930996.0706234857</v>
       </c>
       <c r="AM136" t="n">
         <v>0</v>
@@ -17397,16 +17397,16 @@
         <v>226356.6951500305</v>
       </c>
       <c r="AI137" t="n">
-        <v>12178500</v>
+        <v>12323433.38088073</v>
       </c>
       <c r="AJ137" t="n">
-        <v>119181.8181818182</v>
+        <v>120600.1721538675</v>
       </c>
       <c r="AK137" t="n">
         <v>0</v>
       </c>
       <c r="AL137" t="n">
-        <v>46268.14886183607</v>
+        <v>46818.77490294447</v>
       </c>
       <c r="AM137" t="n">
         <v>0</v>
@@ -17515,16 +17515,16 @@
         <v>27728.31495125331</v>
       </c>
       <c r="AI138" t="n">
-        <v>4760.253698074922</v>
+        <v>13921.12120595045</v>
       </c>
       <c r="AJ138" t="n">
-        <v>23612.28477524872</v>
+        <v>22429.00230898404</v>
       </c>
       <c r="AK138" t="n">
-        <v>13857.64524987262</v>
+        <v>13163.19705038797</v>
       </c>
       <c r="AL138" t="n">
-        <v>5496.018572771962</v>
+        <v>6923.123479818763</v>
       </c>
       <c r="AM138" t="n">
         <v>0</v>
@@ -17645,16 +17645,16 @@
         <v>3764118.754632637</v>
       </c>
       <c r="AI139" t="n">
-        <v>26170000</v>
+        <v>25757512.35697784</v>
       </c>
       <c r="AJ139" t="n">
-        <v>370000</v>
+        <v>1160286.783847251</v>
       </c>
       <c r="AK139" t="n">
-        <v>4082858.490566038</v>
+        <v>7334883.262211051</v>
       </c>
       <c r="AL139" t="n">
-        <v>10795134.28571429</v>
+        <v>12762916.97325536</v>
       </c>
       <c r="AM139" t="n">
         <v>0</v>
@@ -17763,16 +17763,16 @@
         <v>29939648.06861576</v>
       </c>
       <c r="AI140" t="n">
-        <v>231389.0925182927</v>
+        <v>466291.536694327</v>
       </c>
       <c r="AJ140" t="n">
-        <v>45190241.02855375</v>
+        <v>44983319.08440812</v>
       </c>
       <c r="AK140" t="n">
-        <v>5928930.492861228</v>
+        <v>5901782.467173293</v>
       </c>
       <c r="AL140" t="n">
-        <v>181806.3151384148</v>
+        <v>180973.8407959428</v>
       </c>
       <c r="AM140" t="n">
         <v>0</v>
@@ -17893,16 +17893,16 @@
         <v>72740154.90292686</v>
       </c>
       <c r="AI141" t="n">
-        <v>36275187.96992481</v>
+        <v>66815251.17857143</v>
       </c>
       <c r="AJ141" t="n">
-        <v>311808687.5743303</v>
+        <v>284143239.5459946</v>
       </c>
       <c r="AK141" t="n">
-        <v>30384200.94348883</v>
+        <v>27688341.06022559</v>
       </c>
       <c r="AL141" t="n">
-        <v>2014695.533298917</v>
+        <v>1835940.236251223</v>
       </c>
       <c r="AM141" t="n">
         <v>52060788.50578125</v>
@@ -18011,16 +18011,16 @@
         <v>4642462.933997721</v>
       </c>
       <c r="AI142" t="n">
-        <v>6150000</v>
+        <v>10997793.27255371</v>
       </c>
       <c r="AJ142" t="n">
-        <v>4596990.008788687</v>
+        <v>13505039.64398723</v>
       </c>
       <c r="AK142" t="n">
-        <v>2627478.304481852</v>
+        <v>14289206.37982104</v>
       </c>
       <c r="AL142" t="n">
-        <v>509664.4648692706</v>
+        <v>3775228.332025716</v>
       </c>
       <c r="AM142" t="n">
         <v>0</v>
@@ -18129,16 +18129,16 @@
         <v>20179281.2057746</v>
       </c>
       <c r="AI143" t="n">
-        <v>29375127.27272727</v>
+        <v>41726931.86565112</v>
       </c>
       <c r="AJ143" t="n">
-        <v>2594293.787009996</v>
+        <v>3685155.781113921</v>
       </c>
       <c r="AK143" t="n">
-        <v>1819200.260270441</v>
+        <v>2584146.941918314</v>
       </c>
       <c r="AL143" t="n">
-        <v>944122.4008831657</v>
+        <v>1341111.843660422</v>
       </c>
       <c r="AM143" t="n">
         <v>0</v>
@@ -18259,16 +18259,16 @@
         <v>64904415.33317889</v>
       </c>
       <c r="AI144" t="n">
-        <v>11219818.77022654</v>
+        <v>16147265.37216828</v>
       </c>
       <c r="AJ144" t="n">
-        <v>81066276.58046518</v>
+        <v>77091422.47353518</v>
       </c>
       <c r="AK144" t="n">
-        <v>4613930.319829141</v>
+        <v>4387699.380720225</v>
       </c>
       <c r="AL144" t="n">
-        <v>14813984.41406327</v>
+        <v>14087622.85816043</v>
       </c>
       <c r="AM144" t="n">
         <v>0</v>
@@ -18507,16 +18507,16 @@
         <v>84741531.21672203</v>
       </c>
       <c r="AI146" t="n">
-        <v>5166744.897959184</v>
+        <v>2874434.36996092</v>
       </c>
       <c r="AJ146" t="n">
-        <v>56981428.05086883</v>
+        <v>61164566.66090284</v>
       </c>
       <c r="AK146" t="n">
-        <v>74790341.22344761</v>
+        <v>80280873.39737144</v>
       </c>
       <c r="AL146" t="n">
-        <v>8919301.884324515</v>
+        <v>10668260.31658509</v>
       </c>
       <c r="AM146" t="n">
         <v>0</v>
@@ -18625,16 +18625,16 @@
         <v>10807110.75225098</v>
       </c>
       <c r="AI147" t="n">
-        <v>2468432.426580114</v>
+        <v>25601576.49433308</v>
       </c>
       <c r="AJ147" t="n">
-        <v>17743461.54174314</v>
+        <v>31438152.81265565</v>
       </c>
       <c r="AK147" t="n">
-        <v>10141540.47718341</v>
+        <v>33263601.26165156</v>
       </c>
       <c r="AL147" t="n">
-        <v>1967202.846713147</v>
+        <v>8788290.02606694</v>
       </c>
       <c r="AM147" t="n">
         <v>0</v>
@@ -18743,10 +18743,10 @@
         <v>6398308.675001701</v>
       </c>
       <c r="AI148" t="n">
-        <v>16600000</v>
+        <v>20681713.81771406</v>
       </c>
       <c r="AJ148" t="n">
-        <v>150000</v>
+        <v>186882.9561841632</v>
       </c>
       <c r="AK148" t="n">
         <v>0</v>
@@ -18873,16 +18873,16 @@
         <v>8165988.753144099</v>
       </c>
       <c r="AI149" t="n">
-        <v>12040000</v>
+        <v>6610282.023807025</v>
       </c>
       <c r="AJ149" t="n">
-        <v>2289213.365386683</v>
+        <v>29045326.09429788</v>
       </c>
       <c r="AK149" t="n">
-        <v>13246035.58718861</v>
+        <v>31180811.5184059</v>
       </c>
       <c r="AL149" t="n">
-        <v>4010000</v>
+        <v>13526251.61059775</v>
       </c>
       <c r="AM149" t="n">
         <v>0</v>
@@ -18991,16 +18991,16 @@
         <v>135814.0170900183</v>
       </c>
       <c r="AI150" t="n">
-        <v>44000000</v>
+        <v>44087655.77339956</v>
       </c>
       <c r="AJ150" t="n">
-        <v>3775.135270274146</v>
+        <v>3782.656006678779</v>
       </c>
       <c r="AK150" t="n">
         <v>0</v>
       </c>
       <c r="AL150" t="n">
-        <v>240000</v>
+        <v>240478.1224003613</v>
       </c>
       <c r="AM150" t="n">
         <v>0</v>
@@ -19227,16 +19227,16 @@
         <v>325807.7006772264</v>
       </c>
       <c r="AI152" t="n">
-        <v>190000</v>
+        <v>224675.8353426054</v>
       </c>
       <c r="AJ152" t="n">
-        <v>203766.730787622</v>
+        <v>240955.0550249515</v>
       </c>
       <c r="AK152" t="n">
-        <v>119587.2019950013</v>
+        <v>141412.3921290096</v>
       </c>
       <c r="AL152" t="n">
-        <v>47428.94419500321</v>
+        <v>56084.93503384296</v>
       </c>
       <c r="AM152" t="n">
         <v>0</v>
@@ -19345,13 +19345,13 @@
         <v>38126433.0579733</v>
       </c>
       <c r="AI153" t="n">
-        <v>294535.833661497</v>
+        <v>592423.0119883594</v>
       </c>
       <c r="AJ153" t="n">
-        <v>57522786.27246361</v>
+        <v>57259448.80068421</v>
       </c>
       <c r="AK153" t="n">
-        <v>7546952.47917919</v>
+        <v>7512402.772631722</v>
       </c>
       <c r="AL153" t="n">
         <v>259253.5716520039</v>
@@ -19735,16 +19735,16 @@
         <v>318875.6219394131</v>
       </c>
       <c r="AI156" t="n">
-        <v>560000</v>
+        <v>1428969.629171655</v>
       </c>
       <c r="AJ156" t="n">
-        <v>40000</v>
+        <v>15121.37173726619</v>
       </c>
       <c r="AK156" t="n">
         <v>0</v>
       </c>
       <c r="AL156" t="n">
-        <v>0</v>
+        <v>306042.1739468232</v>
       </c>
       <c r="AM156" t="n">
         <v>0</v>
@@ -19983,16 +19983,16 @@
         <v>5675392.587980118</v>
       </c>
       <c r="AI158" t="n">
-        <v>14375000</v>
+        <v>17995289.64595219</v>
       </c>
       <c r="AJ158" t="n">
-        <v>140000</v>
+        <v>175258.4730736214</v>
       </c>
       <c r="AK158" t="n">
         <v>0</v>
       </c>
       <c r="AL158" t="n">
-        <v>110000</v>
+        <v>137703.0859864168</v>
       </c>
       <c r="AM158" t="n">
         <v>0</v>
@@ -20101,16 +20101,16 @@
         <v>4367209.604822396</v>
       </c>
       <c r="AI159" t="n">
-        <v>984006.6784054965</v>
+        <v>3543415.448710754</v>
       </c>
       <c r="AJ159" t="n">
-        <v>1954017.535274786</v>
+        <v>1418952.923586036</v>
       </c>
       <c r="AK159" t="n">
-        <v>1673227.85515675</v>
+        <v>1215051.30534378</v>
       </c>
       <c r="AL159" t="n">
-        <v>2905624.792777963</v>
+        <v>4506852.360138191</v>
       </c>
       <c r="AM159" t="n">
         <v>0</v>
@@ -20467,16 +20467,16 @@
         <v>8021.405396612564</v>
       </c>
       <c r="AI162" t="n">
-        <v>180000</v>
+        <v>182534.8846568901</v>
       </c>
       <c r="AJ162" t="n">
-        <v>41600</v>
+        <v>42185.84000959239</v>
       </c>
       <c r="AK162" t="n">
         <v>0</v>
       </c>
       <c r="AL162" t="n">
-        <v>148058.0763578754</v>
+        <v>150143.1327250323</v>
       </c>
       <c r="AM162" t="n">
         <v>0</v>
@@ -20585,16 +20585,16 @@
         <v>1272549.246998751</v>
       </c>
       <c r="AI163" t="n">
-        <v>2112263.157894737</v>
+        <v>2402836.791055927</v>
       </c>
       <c r="AJ163" t="n">
-        <v>1240000</v>
+        <v>1410580.689140548</v>
       </c>
       <c r="AK163" t="n">
-        <v>151200</v>
+        <v>171999.8388693959</v>
       </c>
       <c r="AL163" t="n">
-        <v>2500000</v>
+        <v>2843912.679718847</v>
       </c>
       <c r="AM163" t="n">
         <v>0</v>
@@ -20703,16 +20703,16 @@
         <v>255331.5668427909</v>
       </c>
       <c r="AI164" t="n">
-        <v>262906.8678841377</v>
+        <v>356198.8415891064</v>
       </c>
       <c r="AJ164" t="n">
-        <v>104506.5911181793</v>
+        <v>113936.9103101186</v>
       </c>
       <c r="AK164" t="n">
-        <v>48137.14187532995</v>
+        <v>52480.87376836137</v>
       </c>
       <c r="AL164" t="n">
-        <v>23928.17859772712</v>
+        <v>26087.37601718103</v>
       </c>
       <c r="AM164" t="n">
         <v>0</v>
@@ -20951,16 +20951,16 @@
         <v>381264.330579733</v>
       </c>
       <c r="AI166" t="n">
-        <v>392575.8660713367</v>
+        <v>571929.494513867</v>
       </c>
       <c r="AJ166" t="n">
-        <v>156050.5659230732</v>
+        <v>146428.5453024366</v>
       </c>
       <c r="AK166" t="n">
-        <v>71878.99013058317</v>
+        <v>67446.95798038931</v>
       </c>
       <c r="AL166" t="n">
-        <v>35729.85944456991</v>
+        <v>33526.76942490553</v>
       </c>
       <c r="AM166" t="n">
         <v>0</v>
@@ -21069,16 +21069,16 @@
         <v>55456.62990250662</v>
       </c>
       <c r="AI167" t="n">
-        <v>12495.32290038726</v>
+        <v>44995.75172966039</v>
       </c>
       <c r="AJ167" t="n">
-        <v>24812.92108285442</v>
+        <v>18018.44982331476</v>
       </c>
       <c r="AK167" t="n">
-        <v>21247.33784326031</v>
+        <v>15429.22292500038</v>
       </c>
       <c r="AL167" t="n">
-        <v>36896.82276543443</v>
+        <v>57229.87123985006</v>
       </c>
       <c r="AM167" t="n">
         <v>0</v>
@@ -21187,16 +21187,16 @@
         <v>831849.4485375993</v>
       </c>
       <c r="AI168" t="n">
-        <v>900000</v>
+        <v>1272171.313410499</v>
       </c>
       <c r="AJ168" t="n">
-        <v>257504.3039865723</v>
+        <v>326026.3335736602</v>
       </c>
       <c r="AK168" t="n">
-        <v>180570.1031929142</v>
+        <v>228619.9018253035</v>
       </c>
       <c r="AL168" t="n">
-        <v>93711.66169956003</v>
+        <v>118648.3837512709</v>
       </c>
       <c r="AM168" t="n">
         <v>0</v>
@@ -21695,16 +21695,16 @@
         <v>45271.33903000611</v>
       </c>
       <c r="AI172" t="n">
-        <v>300000</v>
+        <v>316019.8866841751</v>
       </c>
       <c r="AJ172" t="n">
-        <v>40200</v>
+        <v>42346.66481567945</v>
       </c>
       <c r="AK172" t="n">
         <v>0</v>
       </c>
       <c r="AL172" t="n">
-        <v>210000</v>
+        <v>221213.9206789225</v>
       </c>
       <c r="AM172" t="n">
         <v>0</v>
@@ -21813,16 +21813,16 @@
         <v>374332.2518419197</v>
       </c>
       <c r="AI173" t="n">
-        <v>97293.26317725507</v>
+        <v>298814.9235065168</v>
       </c>
       <c r="AJ173" t="n">
-        <v>262421.7797563582</v>
+        <v>237600.0437916324</v>
       </c>
       <c r="AK173" t="n">
-        <v>221944.2581522901</v>
+        <v>200951.1767858811</v>
       </c>
       <c r="AL173" t="n">
-        <v>62644.42990966739</v>
+        <v>82872.74903110864</v>
       </c>
       <c r="AM173" t="n">
         <v>0</v>
@@ -21931,16 +21931,16 @@
         <v>13468211.74395816</v>
       </c>
       <c r="AI174" t="n">
-        <v>13867793.1968535</v>
+        <v>22697352.57064188</v>
       </c>
       <c r="AJ174" t="n">
-        <v>5512506.405780657</v>
+        <v>4033120.738715849</v>
       </c>
       <c r="AK174" t="n">
-        <v>2539134.614424993</v>
+        <v>1857709.672879459</v>
       </c>
       <c r="AL174" t="n">
-        <v>1262161.901821799</v>
+        <v>923436.8120672774</v>
       </c>
       <c r="AM174" t="n">
         <v>0</v>
@@ -22049,16 +22049,16 @@
         <v>524810.8429808208</v>
       </c>
       <c r="AI175" t="n">
-        <v>540381.1861800636</v>
+        <v>843652.6642740443</v>
       </c>
       <c r="AJ175" t="n">
-        <v>214803.8053420663</v>
+        <v>168183.2816422389</v>
       </c>
       <c r="AK175" t="n">
-        <v>98941.52265878582</v>
+        <v>77467.48222144166</v>
       </c>
       <c r="AL175" t="n">
-        <v>49182.19762698081</v>
+        <v>38507.80661036495</v>
       </c>
       <c r="AM175" t="n">
         <v>0</v>
@@ -22167,16 +22167,16 @@
         <v>506041.7478603729</v>
       </c>
       <c r="AI176" t="n">
-        <v>521055.240421956</v>
+        <v>738649.5566350461</v>
       </c>
       <c r="AJ176" t="n">
-        <v>207121.6602251699</v>
+        <v>206458.2994981266</v>
       </c>
       <c r="AK176" t="n">
-        <v>95403.0232642286</v>
+        <v>95097.47038865833</v>
       </c>
       <c r="AL176" t="n">
-        <v>47423.26799006551</v>
+        <v>47271.38269956301</v>
       </c>
       <c r="AM176" t="n">
         <v>0</v>
@@ -22415,7 +22415,7 @@
         <v>1109132.598050132</v>
       </c>
       <c r="AI178" t="n">
-        <v>20000000</v>
+        <v>20719811.69847854</v>
       </c>
       <c r="AJ178" t="n">
         <v>0</v>
@@ -22533,16 +22533,16 @@
         <v>23416561.97633342</v>
       </c>
       <c r="AI179" t="n">
-        <v>15575454.31108148</v>
+        <v>23406813.99587119</v>
       </c>
       <c r="AJ179" t="n">
-        <v>13026291.9158201</v>
+        <v>11177390.66257306</v>
       </c>
       <c r="AK179" t="n">
-        <v>10124806.78850057</v>
+        <v>8687731.058805911</v>
       </c>
       <c r="AL179" t="n">
-        <v>1578224.823543005</v>
+        <v>1354217.725205954</v>
       </c>
       <c r="AM179" t="n">
         <v>0</v>
@@ -22769,16 +22769,16 @@
         <v>41592.47242687996</v>
       </c>
       <c r="AI181" t="n">
-        <v>7738.98322007</v>
+        <v>8735.411443582007</v>
       </c>
       <c r="AJ181" t="n">
-        <v>30486.90950407379</v>
+        <v>30011.14028363763</v>
       </c>
       <c r="AK181" t="n">
-        <v>21186.46358332352</v>
+        <v>20855.83422709147</v>
       </c>
       <c r="AL181" t="n">
-        <v>12176.94713648501</v>
+        <v>11986.91748964122</v>
       </c>
       <c r="AM181" t="n">
         <v>0</v>
@@ -22887,16 +22887,16 @@
         <v>6578542.722184848</v>
       </c>
       <c r="AI182" t="n">
-        <v>1502592.926763649</v>
+        <v>15584282.29193207</v>
       </c>
       <c r="AJ182" t="n">
-        <v>10800862.73451843</v>
+        <v>19137143.69416948</v>
       </c>
       <c r="AK182" t="n">
-        <v>6173394.427740257</v>
+        <v>20248337.13746461</v>
       </c>
       <c r="AL182" t="n">
-        <v>1197482.682187798</v>
+        <v>5349639.021640493</v>
       </c>
       <c r="AM182" t="n">
         <v>0</v>
@@ -23005,16 +23005,16 @@
         <v>14032958.99919299</v>
       </c>
       <c r="AI183" t="n">
-        <v>484301.7786079692</v>
+        <v>861088.8585990227</v>
       </c>
       <c r="AJ183" t="n">
-        <v>15534671.10840574</v>
+        <v>15287378.07497177</v>
       </c>
       <c r="AK183" t="n">
-        <v>8094288.910737036</v>
+        <v>7965437.695010685</v>
       </c>
       <c r="AL183" t="n">
-        <v>40381.91207881137</v>
+        <v>39739.08124807498</v>
       </c>
       <c r="AM183" t="n">
         <v>0</v>
@@ -23135,16 +23135,16 @@
         <v>128555400.1927482</v>
       </c>
       <c r="AI184" t="n">
-        <v>63720000</v>
+        <v>90684040.6878729</v>
       </c>
       <c r="AJ184" t="n">
-        <v>91864609.9690676</v>
+        <v>105926763.0403001</v>
       </c>
       <c r="AK184" t="n">
-        <v>48508506.61694347</v>
+        <v>55933934.59768645</v>
       </c>
       <c r="AL184" t="n">
-        <v>17177488.80867157</v>
+        <v>32573892.27326827</v>
       </c>
       <c r="AM184" t="n">
         <v>0</v>
@@ -23253,16 +23253,16 @@
         <v>165898508.3533486</v>
       </c>
       <c r="AI185" t="n">
-        <v>47337676.19224791</v>
+        <v>79676601.84218809</v>
       </c>
       <c r="AJ185" t="n">
-        <v>234809058.8747182</v>
+        <v>217036940.5649778</v>
       </c>
       <c r="AK185" t="n">
-        <v>137805412.3230446</v>
+        <v>127375260.6787062</v>
       </c>
       <c r="AL185" t="n">
-        <v>54654386.93943428</v>
+        <v>50517731.24357289</v>
       </c>
       <c r="AM185" t="n">
         <v>38556005.41051597</v>
@@ -23383,16 +23383,16 @@
         <v>5670440.407531301</v>
       </c>
       <c r="AI186" t="n">
-        <v>12253500</v>
+        <v>19748524.35285219</v>
       </c>
       <c r="AJ186" t="n">
-        <v>238350</v>
+        <v>644712.4930925914</v>
       </c>
       <c r="AK186" t="n">
-        <v>0</v>
+        <v>272036.2346545266</v>
       </c>
       <c r="AL186" t="n">
-        <v>70000</v>
+        <v>478237.4361907486</v>
       </c>
       <c r="AM186" t="n">
         <v>0</v>
@@ -23501,16 +23501,16 @@
         <v>196524.4322170078</v>
       </c>
       <c r="AI187" t="n">
-        <v>6831786.40776699</v>
+        <v>6948092.074160345</v>
       </c>
       <c r="AJ187" t="n">
-        <v>190000</v>
+        <v>193234.5971164459</v>
       </c>
       <c r="AK187" t="n">
         <v>0</v>
       </c>
       <c r="AL187" t="n">
-        <v>470000</v>
+        <v>478001.3718143661</v>
       </c>
       <c r="AM187" t="n">
         <v>0</v>
@@ -23749,16 +23749,16 @@
         <v>3196000.459550754</v>
       </c>
       <c r="AI189" t="n">
-        <v>3520000</v>
+        <v>7368299.444017245</v>
       </c>
       <c r="AJ189" t="n">
-        <v>544063.3333333334</v>
+        <v>9048103.890855892</v>
       </c>
       <c r="AK189" t="n">
-        <v>4808226.315789474</v>
+        <v>9573479.771313721</v>
       </c>
       <c r="AL189" t="n">
-        <v>3080000</v>
+        <v>3314606.522768737</v>
       </c>
       <c r="AM189" t="n">
         <v>0</v>
@@ -24009,13 +24009,13 @@
         <v>46934933.63918967</v>
       </c>
       <c r="AI191" t="n">
-        <v>8282589.605740542</v>
+        <v>10363636.36363636</v>
       </c>
       <c r="AJ191" t="n">
-        <v>42103992.6740086</v>
+        <v>40895472.44496736</v>
       </c>
       <c r="AK191" t="n">
-        <v>30398209.06259535</v>
+        <v>29525682.53374077</v>
       </c>
       <c r="AL191" t="n">
         <v>0</v>
@@ -24127,16 +24127,16 @@
         <v>90117.02359157326</v>
       </c>
       <c r="AI192" t="n">
-        <v>53773.94015453914</v>
+        <v>137818.5589528041</v>
       </c>
       <c r="AJ192" t="n">
-        <v>49069.56694327826</v>
+        <v>35319.51947047986</v>
       </c>
       <c r="AK192" t="n">
-        <v>34409.12104925982</v>
+        <v>24767.15603107455</v>
       </c>
       <c r="AL192" t="n">
-        <v>17857.5293148195</v>
+        <v>12853.57490638768</v>
       </c>
       <c r="AM192" t="n">
         <v>0</v>
@@ -24245,16 +24245,16 @@
         <v>450585.1179578663</v>
       </c>
       <c r="AI193" t="n">
-        <v>102917.3237509348</v>
+        <v>1067416.595337813</v>
       </c>
       <c r="AJ193" t="n">
-        <v>739785.1188026324</v>
+        <v>1310763.266723937</v>
       </c>
       <c r="AK193" t="n">
-        <v>422835.2347767299</v>
+        <v>1386872.406675658</v>
       </c>
       <c r="AL193" t="n">
-        <v>82019.36179368477</v>
+        <v>366413.6316192118</v>
       </c>
       <c r="AM193" t="n">
         <v>0</v>
@@ -24375,16 +24375,16 @@
         <v>108071107.5225098</v>
       </c>
       <c r="AI194" t="n">
-        <v>80900000</v>
+        <v>151009883.8965749</v>
       </c>
       <c r="AJ194" t="n">
-        <v>54889977.81496546</v>
+        <v>59034284.23045049</v>
       </c>
       <c r="AK194" t="n">
-        <v>46969413.08596966</v>
+        <v>50515700.54558454</v>
       </c>
       <c r="AL194" t="n">
-        <v>3253482.547600998</v>
+        <v>7312157.674246848</v>
       </c>
       <c r="AM194" t="n">
         <v>0</v>
@@ -24859,16 +24859,16 @@
         <v>1767680.078142399</v>
       </c>
       <c r="AI198" t="n">
-        <v>1820124.469967106</v>
+        <v>2559979.332093298</v>
       </c>
       <c r="AJ198" t="n">
-        <v>723507.1692797028</v>
+        <v>777337.2586919279</v>
       </c>
       <c r="AK198" t="n">
-        <v>333257.1360599765</v>
+        <v>358051.9994601972</v>
       </c>
       <c r="AL198" t="n">
-        <v>165656.6210611877</v>
+        <v>177981.738353845</v>
       </c>
       <c r="AM198" t="n">
         <v>0</v>
@@ -24989,16 +24989,16 @@
         <v>138358097.0171644</v>
       </c>
       <c r="AI199" t="n">
-        <v>10713300.44236536</v>
+        <v>10726504.7400473</v>
       </c>
       <c r="AJ199" t="n">
-        <v>126743136.2299913</v>
+        <v>126899348.9777741</v>
       </c>
       <c r="AK199" t="n">
-        <v>195196862.0620581</v>
+        <v>195437445.0165934</v>
       </c>
       <c r="AL199" t="n">
-        <v>410000</v>
+        <v>0</v>
       </c>
       <c r="AM199" t="n">
         <v>19357512.40079463</v>
@@ -25107,16 +25107,16 @@
         <v>1483464.849892052</v>
       </c>
       <c r="AI200" t="n">
-        <v>22093003.15457413</v>
+        <v>23042323.40396535</v>
       </c>
       <c r="AJ200" t="n">
-        <v>232500</v>
+        <v>242490.3556089323</v>
       </c>
       <c r="AK200" t="n">
         <v>0</v>
       </c>
       <c r="AL200" t="n">
-        <v>80000</v>
+        <v>83437.54171490144</v>
       </c>
       <c r="AM200" t="n">
         <v>0</v>
@@ -25225,16 +25225,16 @@
         <v>2395402.393827022</v>
       </c>
       <c r="AI201" t="n">
-        <v>5460000</v>
+        <v>6948754.67116844</v>
       </c>
       <c r="AJ201" t="n">
-        <v>121425</v>
+        <v>154533.4314920564</v>
       </c>
       <c r="AK201" t="n">
         <v>0</v>
       </c>
       <c r="AL201" t="n">
-        <v>120000</v>
+        <v>152719.8828828229</v>
       </c>
       <c r="AM201" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
---2024 DONE (ready to run cluster)
</commit_message>
<xml_diff>
--- a/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
+++ b/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
@@ -932,7 +932,7 @@
         <v>605883.8709677419</v>
       </c>
       <c r="R4" t="n">
-        <v>200476.1169048793</v>
+        <v>200476.1169048794</v>
       </c>
       <c r="S4" t="n">
         <v>100000</v>
@@ -959,7 +959,7 @@
         <v>605883.8709677419</v>
       </c>
       <c r="AE4" t="n">
-        <v>200476.1169048793</v>
+        <v>200476.1169048794</v>
       </c>
       <c r="AF4" t="n">
         <v>100000</v>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>975633.2705017331</v>
+        <v>975633.2705017327</v>
       </c>
       <c r="V5" t="n">
         <v>3300</v>
@@ -1089,7 +1089,7 @@
         <v>918750</v>
       </c>
       <c r="AE5" t="n">
-        <v>674064.624955536</v>
+        <v>1202856.701429276</v>
       </c>
       <c r="AF5" t="n">
         <v>0</v>
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="AH5" t="n">
-        <v>676316.6650348343</v>
+        <v>676316.6650348339</v>
       </c>
       <c r="AI5" t="n">
         <v>10691952.82795716</v>
@@ -1107,7 +1107,7 @@
         <v>6549206.012784242</v>
       </c>
       <c r="AK5" t="n">
-        <v>2595650.225239041</v>
+        <v>4631893.074348981</v>
       </c>
       <c r="AL5" t="n">
         <v>0</v>
@@ -1116,7 +1116,7 @@
         <v>0</v>
       </c>
       <c r="AN5" t="n">
-        <v>237396.5140773173</v>
+        <v>237396.5140773172</v>
       </c>
     </row>
     <row r="6">
@@ -1231,7 +1231,7 @@
         <v>82443212.4288139</v>
       </c>
       <c r="AI6" t="n">
-        <v>2726843.938943902</v>
+        <v>2726843.938943901</v>
       </c>
       <c r="AJ6" t="n">
         <v>532552046.8877934</v>
@@ -1461,16 +1461,16 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="n">
-        <v>5062516.507214801</v>
+        <v>5000085.53066636</v>
       </c>
       <c r="AD8" t="n">
         <v>770000</v>
       </c>
       <c r="AE8" t="n">
-        <v>1040716.271796942</v>
+        <v>1074334.131152527</v>
       </c>
       <c r="AF8" t="n">
-        <v>220955.2726284793</v>
+        <v>249768.3898213373</v>
       </c>
       <c r="AG8" t="n">
         <v>3066064.909922855</v>
@@ -1479,16 +1479,16 @@
         <v>2578733.290466558</v>
       </c>
       <c r="AI8" t="n">
-        <v>12006819.56886857</v>
+        <v>11805983.65404298</v>
       </c>
       <c r="AJ8" t="n">
-        <v>10041719.07675182</v>
+        <v>9873753.044978499</v>
       </c>
       <c r="AK8" t="n">
-        <v>7805019.734974331</v>
+        <v>8021290.518500813</v>
       </c>
       <c r="AL8" t="n">
-        <v>1216623.304651108</v>
+        <v>1369154.467723533</v>
       </c>
       <c r="AM8" t="n">
         <v>5431113.015357894</v>
@@ -2075,16 +2075,16 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="n">
-        <v>16949820.03516326</v>
+        <v>16762009.87491277</v>
       </c>
       <c r="AD13" t="n">
-        <v>2421689.057840701</v>
+        <v>2394855.863795786</v>
       </c>
       <c r="AE13" t="n">
-        <v>3484423.900541321</v>
+        <v>3601538.25467353</v>
       </c>
       <c r="AF13" t="n">
-        <v>739780.7200304013</v>
+        <v>837309.7201935998</v>
       </c>
       <c r="AG13" t="n">
         <v>0</v>
@@ -2093,16 +2093,16 @@
         <v>18774952.30430221</v>
       </c>
       <c r="AI13" t="n">
-        <v>18767136.55968409</v>
+        <v>18559189.87249773</v>
       </c>
       <c r="AJ13" t="n">
-        <v>8961818.425286237</v>
+        <v>8826630.303857977</v>
       </c>
       <c r="AK13" t="n">
-        <v>6965656.889621076</v>
+        <v>7170623.535359257</v>
       </c>
       <c r="AL13" t="n">
-        <v>1085785.916227977</v>
+        <v>1223954.079104415</v>
       </c>
       <c r="AM13" t="n">
         <v>0</v>
@@ -2441,16 +2441,16 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="n">
-        <v>383836.0467331784</v>
+        <v>377618.8867513154</v>
       </c>
       <c r="AD16" t="n">
-        <v>130211.5094185826</v>
+        <v>128102.4167671102</v>
       </c>
       <c r="AE16" t="n">
-        <v>206406.1670308976</v>
+        <v>222639.9943032189</v>
       </c>
       <c r="AF16" t="n">
-        <v>488199.1451933606</v>
+        <v>480291.5705543747</v>
       </c>
       <c r="AG16" t="n">
         <v>0</v>
@@ -2459,16 +2459,16 @@
         <v>672411.6375678928</v>
       </c>
       <c r="AI16" t="n">
-        <v>545573.4897221323</v>
+        <v>536736.5977826327</v>
       </c>
       <c r="AJ16" t="n">
-        <v>218473.7041076912</v>
+        <v>219526.063140251</v>
       </c>
       <c r="AK16" t="n">
-        <v>187079.3279656295</v>
+        <v>206103.4594661552</v>
       </c>
       <c r="AL16" t="n">
-        <v>693912.1887831823</v>
+        <v>682672.5901895964</v>
       </c>
       <c r="AM16" t="n">
         <v>0</v>
@@ -2559,16 +2559,16 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="n">
-        <v>1258020.255038614</v>
+        <v>1233176.148569172</v>
       </c>
       <c r="AD17" t="n">
         <v>106750</v>
       </c>
       <c r="AE17" t="n">
-        <v>72842.67305581056</v>
+        <v>71404.13411522585</v>
       </c>
       <c r="AF17" t="n">
-        <v>49317.96116653409</v>
+        <v>75600.60657656149</v>
       </c>
       <c r="AG17" t="n">
         <v>0</v>
@@ -2577,16 +2577,16 @@
         <v>991287.2595073058</v>
       </c>
       <c r="AI17" t="n">
-        <v>1570680.497848381</v>
+        <v>1539661.797345165</v>
       </c>
       <c r="AJ17" t="n">
-        <v>331196.6035462395</v>
+        <v>324743.6830382025</v>
       </c>
       <c r="AK17" t="n">
-        <v>152553.611432068</v>
+        <v>149581.3094300408</v>
       </c>
       <c r="AL17" t="n">
-        <v>75831.88194946748</v>
+        <v>116275.8049627474</v>
       </c>
       <c r="AM17" t="n">
         <v>0</v>
@@ -2656,7 +2656,7 @@
         <v>1429492.207792208</v>
       </c>
       <c r="R18" t="n">
-        <v>240571.3402858551</v>
+        <v>240571.3402858552</v>
       </c>
       <c r="S18" t="n">
         <v>194326.2252197115</v>
@@ -2695,7 +2695,7 @@
         <v>4168831.16883117</v>
       </c>
       <c r="AE18" t="n">
-        <v>4410474.571907344</v>
+        <v>4410474.571907346</v>
       </c>
       <c r="AF18" t="n">
         <v>0</v>
@@ -2713,7 +2713,7 @@
         <v>82342367.09643011</v>
       </c>
       <c r="AK18" t="n">
-        <v>47059542.00795279</v>
+        <v>47059542.0079528</v>
       </c>
       <c r="AL18" t="n">
         <v>0</v>
@@ -2937,7 +2937,7 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr"/>
       <c r="AC20" t="n">
-        <v>389570.7171572578</v>
+        <v>389570.7171572576</v>
       </c>
       <c r="AD20" t="n">
         <v>12997543.64845027</v>
@@ -2955,7 +2955,7 @@
         <v>25013557.50999298</v>
       </c>
       <c r="AI20" t="n">
-        <v>389570.7171572578</v>
+        <v>389570.7171572576</v>
       </c>
       <c r="AJ20" t="n">
         <v>37582032.90598097</v>
@@ -3206,13 +3206,13 @@
         <v>11466334.22998163</v>
       </c>
       <c r="AJ22" t="n">
-        <v>2599767.222557667</v>
+        <v>2529631.26718122</v>
       </c>
       <c r="AK22" t="n">
-        <v>2020693.301944629</v>
+        <v>2055034.919985495</v>
       </c>
       <c r="AL22" t="n">
-        <v>314979.6728484913</v>
+        <v>350774.0101840728</v>
       </c>
       <c r="AM22" t="n">
         <v>0</v>
@@ -3303,16 +3303,16 @@
       <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="n">
-        <v>44801334.51514725</v>
+        <v>44304919.46193311</v>
       </c>
       <c r="AD23" t="n">
-        <v>6400947.11017078</v>
+        <v>6330022.292088809</v>
       </c>
       <c r="AE23" t="n">
-        <v>9209940.898303015</v>
+        <v>9519494.589440592</v>
       </c>
       <c r="AF23" t="n">
-        <v>1955369.640337262</v>
+        <v>2213155.820495795</v>
       </c>
       <c r="AG23" t="n">
         <v>29245166.35932423</v>
@@ -3321,16 +3321,16 @@
         <v>20380311.48917118</v>
       </c>
       <c r="AI23" t="n">
-        <v>111720508.981656</v>
+        <v>109851780.0899278</v>
       </c>
       <c r="AJ23" t="n">
-        <v>93435731.24179405</v>
+        <v>91872848.54386473</v>
       </c>
       <c r="AK23" t="n">
-        <v>72623792.87051871</v>
+        <v>74636139.42697795</v>
       </c>
       <c r="AL23" t="n">
-        <v>11320381.22626459</v>
+        <v>12739646.2594628</v>
       </c>
       <c r="AM23" t="n">
         <v>51803796.82647655</v>
@@ -3657,13 +3657,13 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="n">
-        <v>5458896.292083068</v>
+        <v>5412943.896706011</v>
       </c>
       <c r="AD26" t="n">
-        <v>1339121.753292968</v>
+        <v>1327849.171992133</v>
       </c>
       <c r="AE26" t="n">
-        <v>1078031.903250222</v>
+        <v>1135256.879928114</v>
       </c>
       <c r="AF26" t="n">
         <v>420000</v>
@@ -3675,13 +3675,13 @@
         <v>5379293.100543143</v>
       </c>
       <c r="AI26" t="n">
-        <v>6949515.945421916</v>
+        <v>6891015.675895578</v>
       </c>
       <c r="AJ26" t="n">
-        <v>2998820.932478525</v>
+        <v>2983508.443290601</v>
       </c>
       <c r="AK26" t="n">
-        <v>1304113.574920718</v>
+        <v>1377926.33363498</v>
       </c>
       <c r="AL26" t="n">
         <v>534686.2334260278</v>
@@ -3884,7 +3884,7 @@
         <v>90000</v>
       </c>
       <c r="R28" t="n">
-        <v>4009.522338097586</v>
+        <v>4009.522338097587</v>
       </c>
       <c r="S28" t="n">
         <v>0</v>
@@ -4129,7 +4129,7 @@
         <v>0</v>
       </c>
       <c r="U30" t="n">
-        <v>65307.0179123306</v>
+        <v>65307.01791233057</v>
       </c>
       <c r="V30" t="inlineStr"/>
       <c r="W30" t="n">
@@ -4156,7 +4156,7 @@
         <v>0</v>
       </c>
       <c r="AH30" t="n">
-        <v>45271.33903000611</v>
+        <v>45271.33903000609</v>
       </c>
       <c r="AI30" t="n">
         <v>11189380.47217878</v>
@@ -4174,7 +4174,7 @@
         <v>0</v>
       </c>
       <c r="AN30" t="n">
-        <v>15890.86685122908</v>
+        <v>15890.86685122907</v>
       </c>
     </row>
     <row r="31">
@@ -4277,7 +4277,7 @@
         <v>400000</v>
       </c>
       <c r="AE31" t="n">
-        <v>112344.104159256</v>
+        <v>200476.1169048794</v>
       </c>
       <c r="AF31" t="n">
         <v>0</v>
@@ -4289,16 +4289,16 @@
         <v>1793186.329498243</v>
       </c>
       <c r="AI31" t="n">
-        <v>74133.30453690726</v>
+        <v>72537.97080423067</v>
       </c>
       <c r="AJ31" t="n">
-        <v>1289712.424443049</v>
+        <v>1261958.073695852</v>
       </c>
       <c r="AK31" t="n">
-        <v>1413324.731072586</v>
+        <v>1430971.499081032</v>
       </c>
       <c r="AL31" t="n">
-        <v>309276.5045917907</v>
+        <v>320979.4210632184</v>
       </c>
       <c r="AM31" t="n">
         <v>0</v>
@@ -4377,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="U32" t="n">
-        <v>457149.1253863142</v>
+        <v>457149.125386314</v>
       </c>
       <c r="V32" t="inlineStr"/>
       <c r="W32" t="n">
@@ -4389,40 +4389,40 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr"/>
       <c r="AC32" t="n">
-        <v>364455.7149461394</v>
+        <v>357258.2341828102</v>
       </c>
       <c r="AD32" t="n">
         <v>75502.70540548294</v>
       </c>
       <c r="AE32" t="n">
-        <v>21102.94200813838</v>
+        <v>20686.18899007781</v>
       </c>
       <c r="AF32" t="n">
-        <v>14287.69745530323</v>
+        <v>21901.93123669284</v>
       </c>
       <c r="AG32" t="n">
         <v>0</v>
       </c>
       <c r="AH32" t="n">
-        <v>316899.3732100427</v>
+        <v>316899.3732100426</v>
       </c>
       <c r="AI32" t="n">
-        <v>455035.188426055</v>
+        <v>446048.8922012357</v>
       </c>
       <c r="AJ32" t="n">
-        <v>133747.7982108226</v>
+        <v>129195.3954170361</v>
       </c>
       <c r="AK32" t="n">
-        <v>61606.03526630016</v>
+        <v>59509.1372925605</v>
       </c>
       <c r="AL32" t="n">
-        <v>30623.34316332531</v>
+        <v>46258.94015567072</v>
       </c>
       <c r="AM32" t="n">
         <v>0</v>
       </c>
       <c r="AN32" t="n">
-        <v>111236.0679586036</v>
+        <v>111236.0679586035</v>
       </c>
     </row>
     <row r="33">
@@ -5030,13 +5030,13 @@
         <v>3563181.818181818</v>
       </c>
       <c r="AD37" t="n">
-        <v>946239.8143591034</v>
+        <v>923948.7755939463</v>
       </c>
       <c r="AE37" t="n">
-        <v>1499942.16368417</v>
+        <v>1605808.503274991</v>
       </c>
       <c r="AF37" t="n">
-        <v>3547716.101139925</v>
+        <v>3464140.800314261</v>
       </c>
       <c r="AG37" t="n">
         <v>0</v>
@@ -5048,13 +5048,13 @@
         <v>5064603.899516638</v>
       </c>
       <c r="AJ37" t="n">
-        <v>1562489.813830086</v>
+        <v>1557228.995031738</v>
       </c>
       <c r="AK37" t="n">
-        <v>1337962.138365115</v>
+        <v>1462014.480039194</v>
       </c>
       <c r="AL37" t="n">
-        <v>5042621.375234686</v>
+        <v>4923829.852358955</v>
       </c>
       <c r="AM37" t="n">
         <v>0</v>
@@ -5124,7 +5124,7 @@
         <v>24440</v>
       </c>
       <c r="R38" t="n">
-        <v>400952.2338097586</v>
+        <v>400952.2338097587</v>
       </c>
       <c r="S38" t="n">
         <v>0</v>
@@ -5151,7 +5151,7 @@
         <v>24440</v>
       </c>
       <c r="AE38" t="n">
-        <v>400952.2338097586</v>
+        <v>400952.2338097587</v>
       </c>
       <c r="AF38" t="n">
         <v>0</v>
@@ -5251,7 +5251,7 @@
         <v>0</v>
       </c>
       <c r="U39" t="n">
-        <v>522456.1432986448</v>
+        <v>522456.1432986446</v>
       </c>
       <c r="V39" t="inlineStr"/>
       <c r="W39" t="n">
@@ -5278,13 +5278,13 @@
         <v>0</v>
       </c>
       <c r="AH39" t="n">
-        <v>362170.7122400489</v>
+        <v>362170.7122400487</v>
       </c>
       <c r="AI39" t="n">
         <v>13872460.5190593</v>
       </c>
       <c r="AJ39" t="n">
-        <v>2232583.258370919</v>
+        <v>2232583.258370918</v>
       </c>
       <c r="AK39" t="n">
         <v>0</v>
@@ -5381,16 +5381,16 @@
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr"/>
       <c r="AC40" t="n">
-        <v>1622399.785160857</v>
+        <v>1596121.067711746</v>
       </c>
       <c r="AD40" t="n">
-        <v>550378.544965143</v>
+        <v>541463.8234486099</v>
       </c>
       <c r="AE40" t="n">
-        <v>872438.4379656492</v>
+        <v>941055.6460239148</v>
       </c>
       <c r="AF40" t="n">
-        <v>2063522.160095647</v>
+        <v>2030098.391003027</v>
       </c>
       <c r="AG40" t="n">
         <v>0</v>
@@ -5399,16 +5399,16 @@
         <v>2842152.282503464</v>
       </c>
       <c r="AI40" t="n">
-        <v>2306032.276145094</v>
+        <v>2268680.464854427</v>
       </c>
       <c r="AJ40" t="n">
-        <v>923445.5534448812</v>
+        <v>927893.6689433289</v>
       </c>
       <c r="AK40" t="n">
-        <v>790747.6749062696</v>
+        <v>871158.9523827173</v>
       </c>
       <c r="AL40" t="n">
-        <v>2933030.901042315</v>
+        <v>2885523.319358088</v>
       </c>
       <c r="AM40" t="n">
         <v>0</v>
@@ -5629,16 +5629,16 @@
       <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr"/>
       <c r="AC42" t="n">
-        <v>55399.01705427316</v>
+        <v>54501.69499503521</v>
       </c>
       <c r="AD42" t="n">
-        <v>18793.41373051708</v>
+        <v>18489.00860556229</v>
       </c>
       <c r="AE42" t="n">
-        <v>29790.58080858315</v>
+        <v>32133.60742520684</v>
       </c>
       <c r="AF42" t="n">
-        <v>70461.73229594894</v>
+        <v>69320.43286351798</v>
       </c>
       <c r="AG42" t="n">
         <v>0</v>
@@ -5647,16 +5647,16 @@
         <v>97049.10232938659</v>
       </c>
       <c r="AI42" t="n">
-        <v>78742.56552690566</v>
+        <v>77467.13782429749</v>
       </c>
       <c r="AJ42" t="n">
-        <v>31532.2871908008</v>
+        <v>31684.17406147952</v>
       </c>
       <c r="AK42" t="n">
-        <v>27001.14011875065</v>
+        <v>29746.89105697083</v>
       </c>
       <c r="AL42" t="n">
-        <v>100152.2746697376</v>
+        <v>98530.06456344688</v>
       </c>
       <c r="AM42" t="n">
         <v>0</v>
@@ -5747,16 +5747,16 @@
       <c r="AA43" t="inlineStr"/>
       <c r="AB43" t="inlineStr"/>
       <c r="AC43" t="n">
-        <v>133993.0068564222</v>
+        <v>131565.3631036915</v>
       </c>
       <c r="AD43" t="n">
         <v>72100</v>
       </c>
       <c r="AE43" t="n">
-        <v>72054.15747053191</v>
+        <v>77569.5091522187</v>
       </c>
       <c r="AF43" t="n">
-        <v>170425.034245589</v>
+        <v>167337.326316633</v>
       </c>
       <c r="AG43" t="n">
         <v>0</v>
@@ -5765,16 +5765,16 @@
         <v>249554.8345612798</v>
       </c>
       <c r="AI43" t="n">
-        <v>190453.7965394298</v>
+        <v>187003.2137052957</v>
       </c>
       <c r="AJ43" t="n">
-        <v>95802.76622331506</v>
+        <v>95766.84575668676</v>
       </c>
       <c r="AK43" t="n">
-        <v>82036.03813789655</v>
+        <v>89911.32046131881</v>
       </c>
       <c r="AL43" t="n">
-        <v>242237.2298295735</v>
+        <v>237848.4508069138</v>
       </c>
       <c r="AM43" t="n">
         <v>0</v>
@@ -6391,16 +6391,16 @@
         <v>23793638.3469183</v>
       </c>
       <c r="AI48" t="n">
-        <v>59658023.01415314</v>
+        <v>59532838.24175358</v>
       </c>
       <c r="AJ48" t="n">
-        <v>129969670.2651119</v>
+        <v>129696945.4450634</v>
       </c>
       <c r="AK48" t="n">
-        <v>134542642.6314247</v>
+        <v>135023312.4041393</v>
       </c>
       <c r="AL48" t="n">
-        <v>39440170.27281277</v>
+        <v>39357410.09254614</v>
       </c>
       <c r="AM48" t="n">
         <v>65800855.29762293</v>
@@ -7126,7 +7126,7 @@
         <v>10020000</v>
       </c>
       <c r="AF54" t="n">
-        <v>3818433.791669101</v>
+        <v>6225201.145062016</v>
       </c>
       <c r="AG54" t="n">
         <v>0</v>
@@ -7138,13 +7138,13 @@
         <v>26461.53846153845</v>
       </c>
       <c r="AJ54" t="n">
-        <v>92507226.5518977</v>
+        <v>90183073.66110086</v>
       </c>
       <c r="AK54" t="n">
-        <v>16628838.72741269</v>
+        <v>16211055.54398509</v>
       </c>
       <c r="AL54" t="n">
-        <v>4652534.107538296</v>
+        <v>7394470.181762741</v>
       </c>
       <c r="AM54" t="n">
         <v>0</v>
@@ -7495,16 +7495,16 @@
       <c r="AA57" t="inlineStr"/>
       <c r="AB57" t="inlineStr"/>
       <c r="AC57" t="n">
-        <v>324058.7340667534</v>
+        <v>317659.0360815568</v>
       </c>
       <c r="AD57" t="n">
         <v>50000</v>
       </c>
       <c r="AE57" t="n">
-        <v>18763.85083782283</v>
+        <v>18393.29153551866</v>
       </c>
       <c r="AF57" t="n">
-        <v>12704.02125750336</v>
+        <v>19474.27854500419</v>
       </c>
       <c r="AG57" t="n">
         <v>0</v>
@@ -7513,16 +7513,16 @@
         <v>270351.0707747198</v>
       </c>
       <c r="AI57" t="n">
-        <v>404598.2023878155</v>
+        <v>396607.9647289159</v>
       </c>
       <c r="AJ57" t="n">
-        <v>104394.488304592</v>
+        <v>101377.9254172329</v>
       </c>
       <c r="AK57" t="n">
-        <v>48085.5058111876</v>
+        <v>46696.03636116553</v>
       </c>
       <c r="AL57" t="n">
-        <v>23902.51116262925</v>
+        <v>36298.78115890993</v>
       </c>
       <c r="AM57" t="n">
         <v>0</v>
@@ -7861,7 +7861,7 @@
         <v>0</v>
       </c>
       <c r="U60" t="n">
-        <v>653070.1791233061</v>
+        <v>653070.1791233057</v>
       </c>
       <c r="V60" t="n">
         <v>24092</v>
@@ -7900,7 +7900,7 @@
         <v>0</v>
       </c>
       <c r="AH60" t="n">
-        <v>452713.3903000611</v>
+        <v>452713.3903000609</v>
       </c>
       <c r="AI60" t="n">
         <v>61146290.42179304</v>
@@ -7918,7 +7918,7 @@
         <v>0</v>
       </c>
       <c r="AN60" t="n">
-        <v>158908.6685122908</v>
+        <v>158908.6685122907</v>
       </c>
     </row>
     <row r="61">
@@ -8112,7 +8112,7 @@
         <v>10000</v>
       </c>
       <c r="R62" t="n">
-        <v>40095.22338097586</v>
+        <v>40095.22338097587</v>
       </c>
       <c r="S62" t="n">
         <v>120000</v>
@@ -8139,7 +8139,7 @@
         <v>10000</v>
       </c>
       <c r="AE62" t="n">
-        <v>40095.22338097586</v>
+        <v>40095.22338097587</v>
       </c>
       <c r="AF62" t="n">
         <v>120000</v>
@@ -8520,13 +8520,13 @@
         <v>1739613.246072689</v>
       </c>
       <c r="AJ65" t="n">
-        <v>225715.3018836979</v>
+        <v>220741.0488305447</v>
       </c>
       <c r="AK65" t="n">
-        <v>247348.9533695903</v>
+        <v>250304.7891509378</v>
       </c>
       <c r="AL65" t="n">
-        <v>54127.13584550996</v>
+        <v>56145.5531173157</v>
       </c>
       <c r="AM65" t="n">
         <v>0</v>
@@ -8895,7 +8895,7 @@
         <v>664676.4705882353</v>
       </c>
       <c r="AE68" t="n">
-        <v>734730.4412015342</v>
+        <v>1311113.804557911</v>
       </c>
       <c r="AF68" t="n">
         <v>344200</v>
@@ -8907,16 +8907,16 @@
         <v>10349593.5555553</v>
       </c>
       <c r="AI68" t="n">
-        <v>2331939.636284772</v>
+        <v>2282947.008484141</v>
       </c>
       <c r="AJ68" t="n">
-        <v>4630711.397087707</v>
+        <v>4533422.97829694</v>
       </c>
       <c r="AK68" t="n">
-        <v>3965284.424998457</v>
+        <v>4256233.386071423</v>
       </c>
       <c r="AL68" t="n">
-        <v>6885869.548599202</v>
+        <v>6741201.634117634</v>
       </c>
       <c r="AM68" t="n">
         <v>0</v>
@@ -9125,16 +9125,16 @@
       <c r="AA70" t="inlineStr"/>
       <c r="AB70" t="inlineStr"/>
       <c r="AC70" t="n">
-        <v>443795.0461978699</v>
+        <v>435030.7267569141</v>
       </c>
       <c r="AD70" t="n">
         <v>43414.05560815268</v>
       </c>
       <c r="AE70" t="n">
-        <v>25696.89742633557</v>
+        <v>25189.4203383974</v>
       </c>
       <c r="AF70" t="n">
-        <v>17398.02421036133</v>
+        <v>26669.82073925531</v>
       </c>
       <c r="AG70" t="n">
         <v>0</v>
@@ -9143,16 +9143,16 @@
         <v>353536.0156284797</v>
       </c>
       <c r="AI70" t="n">
-        <v>554093.005508341</v>
+        <v>543150.4586235135</v>
       </c>
       <c r="AJ70" t="n">
-        <v>121717.460294187</v>
+        <v>119094.6328084726</v>
       </c>
       <c r="AK70" t="n">
-        <v>56064.69976865315</v>
+        <v>54856.59014184908</v>
       </c>
       <c r="AL70" t="n">
-        <v>27868.83676157367</v>
+        <v>42642.32075891965</v>
       </c>
       <c r="AM70" t="n">
         <v>0</v>
@@ -9243,16 +9243,16 @@
       <c r="AA71" t="inlineStr"/>
       <c r="AB71" t="inlineStr"/>
       <c r="AC71" t="n">
-        <v>58617.21676645073</v>
+        <v>57459.61030625633</v>
       </c>
       <c r="AD71" t="n">
         <v>18875.67635137073</v>
       </c>
       <c r="AE71" t="n">
-        <v>3394.090627125147</v>
+        <v>3327.062176216265</v>
       </c>
       <c r="AF71" t="n">
-        <v>2297.961108813303</v>
+        <v>3522.596019916581</v>
       </c>
       <c r="AG71" t="n">
         <v>0</v>
@@ -9261,16 +9261,16 @@
         <v>55456.62990250662</v>
       </c>
       <c r="AI71" t="n">
-        <v>73185.56187347656</v>
+        <v>71740.25136760174</v>
       </c>
       <c r="AJ71" t="n">
-        <v>27219.81502035261</v>
+        <v>26082.43518098796</v>
       </c>
       <c r="AK71" t="n">
-        <v>12537.81300715512</v>
+        <v>12013.92055111163</v>
       </c>
       <c r="AL71" t="n">
-        <v>6232.339876702693</v>
+        <v>9338.92267798566</v>
       </c>
       <c r="AM71" t="n">
         <v>0</v>
@@ -9382,13 +9382,13 @@
         <v>490000</v>
       </c>
       <c r="AJ72" t="n">
-        <v>341921.221426249</v>
+        <v>334386.0536045576</v>
       </c>
       <c r="AK72" t="n">
-        <v>374692.6129900229</v>
+        <v>379170.2136323334</v>
       </c>
       <c r="AL72" t="n">
-        <v>81993.62757486994</v>
+        <v>85051.19475425087</v>
       </c>
       <c r="AM72" t="n">
         <v>0</v>
@@ -10317,13 +10317,13 @@
       <c r="AA80" t="inlineStr"/>
       <c r="AB80" t="inlineStr"/>
       <c r="AC80" t="n">
-        <v>3021713.09416977</v>
+        <v>2991118.618649601</v>
       </c>
       <c r="AD80" t="n">
         <v>1156362.264150943</v>
       </c>
       <c r="AE80" t="n">
-        <v>596732.9188334733</v>
+        <v>627327.3943536427</v>
       </c>
       <c r="AF80" t="n">
         <v>1600000</v>
@@ -10335,13 +10335,13 @@
         <v>4133528.895671517</v>
       </c>
       <c r="AI80" t="n">
-        <v>3846829.506704148</v>
+        <v>3807880.828419567</v>
       </c>
       <c r="AJ80" t="n">
-        <v>2211816.971366774</v>
+        <v>2197650.727767535</v>
       </c>
       <c r="AK80" t="n">
-        <v>961864.8804133275</v>
+        <v>1014979.802297148</v>
       </c>
       <c r="AL80" t="n">
         <v>2036899.936861058</v>
@@ -10565,16 +10565,16 @@
       <c r="AA82" t="inlineStr"/>
       <c r="AB82" t="inlineStr"/>
       <c r="AC82" t="n">
-        <v>585149.8358118961</v>
+        <v>580404.6553605783</v>
       </c>
       <c r="AD82" t="n">
-        <v>143543.0959199463</v>
+        <v>142379.0557869846</v>
       </c>
       <c r="AE82" t="n">
-        <v>115556.3611094252</v>
+        <v>121728.2851465307</v>
       </c>
       <c r="AF82" t="n">
-        <v>32395.16049295029</v>
+        <v>32132.45704012412</v>
       </c>
       <c r="AG82" t="n">
         <v>0</v>
@@ -10583,16 +10583,16 @@
         <v>568430.4565006929</v>
       </c>
       <c r="AI82" t="n">
-        <v>744932.2897621936</v>
+        <v>738891.3786611414</v>
       </c>
       <c r="AJ82" t="n">
-        <v>328405.3642196809</v>
+        <v>326589.5948586839</v>
       </c>
       <c r="AK82" t="n">
-        <v>142815.4275292779</v>
+        <v>150834.633653868</v>
       </c>
       <c r="AL82" t="n">
-        <v>29394.86729331807</v>
+        <v>29232.34163077721</v>
       </c>
       <c r="AM82" t="n">
         <v>0</v>
@@ -11206,13 +11206,13 @@
         <v>23532341.60958904</v>
       </c>
       <c r="AD87" t="n">
-        <v>48860677.68782314</v>
+        <v>46323916.912671</v>
       </c>
       <c r="AE87" t="n">
-        <v>16258946.93414473</v>
+        <v>15414810.89715936</v>
       </c>
       <c r="AF87" t="n">
-        <v>6195979.280468358</v>
+        <v>9576876.092605876</v>
       </c>
       <c r="AG87" t="n">
         <v>8111024.303540939</v>
@@ -11224,13 +11224,13 @@
         <v>23532341.60958904</v>
       </c>
       <c r="AJ87" t="n">
-        <v>385631708.2248917</v>
+        <v>375943091.6393432</v>
       </c>
       <c r="AK87" t="n">
-        <v>69320070.69362129</v>
+        <v>67578472.24020278</v>
       </c>
       <c r="AL87" t="n">
-        <v>19394859.64870016</v>
+        <v>30825074.68766714</v>
       </c>
       <c r="AM87" t="n">
         <v>14367565.90516989</v>
@@ -11324,13 +11324,13 @@
         <v>2254000</v>
       </c>
       <c r="AD88" t="n">
-        <v>26565364.4601059</v>
+        <v>25186137.28338558</v>
       </c>
       <c r="AE88" t="n">
-        <v>8839927.554887736</v>
+        <v>8380974.004965638</v>
       </c>
       <c r="AF88" t="n">
-        <v>3368730.348452109</v>
+        <v>5206911.075094518</v>
       </c>
       <c r="AG88" t="n">
         <v>0</v>
@@ -11342,13 +11342,13 @@
         <v>2254000</v>
       </c>
       <c r="AJ88" t="n">
-        <v>153388380.6913579</v>
+        <v>149534648.8080605</v>
       </c>
       <c r="AK88" t="n">
-        <v>27572663.67449266</v>
+        <v>26879927.67564516</v>
       </c>
       <c r="AL88" t="n">
-        <v>7714474.852040316</v>
+        <v>12260942.73418524</v>
       </c>
       <c r="AM88" t="n">
         <v>0</v>
@@ -11427,7 +11427,7 @@
         <v>0</v>
       </c>
       <c r="U89" t="n">
-        <v>848991.2328602978</v>
+        <v>848991.2328602974</v>
       </c>
       <c r="V89" t="n">
         <v>2716</v>
@@ -11466,25 +11466,25 @@
         <v>0</v>
       </c>
       <c r="AH89" t="n">
-        <v>588527.4073900793</v>
+        <v>588527.4073900791</v>
       </c>
       <c r="AI89" t="n">
         <v>13519332.84814011</v>
       </c>
       <c r="AJ89" t="n">
-        <v>19253.80517362235</v>
+        <v>19253.80517362236</v>
       </c>
       <c r="AK89" t="n">
         <v>0</v>
       </c>
       <c r="AL89" t="n">
-        <v>5909591.061147892</v>
+        <v>5909591.061147893</v>
       </c>
       <c r="AM89" t="n">
         <v>0</v>
       </c>
       <c r="AN89" t="n">
-        <v>206581.269065978</v>
+        <v>206581.2690659779</v>
       </c>
     </row>
     <row r="90">
@@ -11542,7 +11542,7 @@
         <v>18063</v>
       </c>
       <c r="P90" t="n">
-        <v>2151804.377303027</v>
+        <v>2151804.377303026</v>
       </c>
       <c r="Q90" t="n">
         <v>6970000</v>
@@ -11581,7 +11581,7 @@
         <v>0</v>
       </c>
       <c r="AC90" t="n">
-        <v>2151804.377303027</v>
+        <v>2151804.377303026</v>
       </c>
       <c r="AD90" t="n">
         <v>26214601.76991151</v>
@@ -11599,7 +11599,7 @@
         <v>48882570.29394399</v>
       </c>
       <c r="AI90" t="n">
-        <v>2151804.377303027</v>
+        <v>2151804.377303026</v>
       </c>
       <c r="AJ90" t="n">
         <v>79338754.78813301</v>
@@ -12207,16 +12207,16 @@
       <c r="AA95" t="inlineStr"/>
       <c r="AB95" t="inlineStr"/>
       <c r="AC95" t="n">
-        <v>60740891.50945699</v>
+        <v>60067860.37729848</v>
       </c>
       <c r="AD95" t="n">
-        <v>8678295.81829093</v>
+        <v>8582137.149647066</v>
       </c>
       <c r="AE95" t="n">
-        <v>12486682.08138298</v>
+        <v>12906369.73964643</v>
       </c>
       <c r="AF95" t="n">
-        <v>2651057.082785232</v>
+        <v>3000559.22532415</v>
       </c>
       <c r="AG95" t="n">
         <v>0</v>
@@ -12225,16 +12225,16 @@
         <v>67281383.43917617</v>
       </c>
       <c r="AI95" t="n">
-        <v>67253375.15974137</v>
+        <v>66508183.34413895</v>
       </c>
       <c r="AJ95" t="n">
-        <v>32115316.83336372</v>
+        <v>31630860.53825226</v>
       </c>
       <c r="AK95" t="n">
-        <v>24961929.30348716</v>
+        <v>25696441.92757475</v>
       </c>
       <c r="AL95" t="n">
-        <v>3890991.432550907</v>
+        <v>4386126.919177202</v>
       </c>
       <c r="AM95" t="n">
         <v>0</v>
@@ -12603,16 +12603,16 @@
         <v>5498730.420466315</v>
       </c>
       <c r="AI98" t="n">
-        <v>5586454.706201179</v>
+        <v>5466969.016705413</v>
       </c>
       <c r="AJ98" t="n">
-        <v>2896258.311806518</v>
+        <v>2834311.793031399</v>
       </c>
       <c r="AK98" t="n">
-        <v>1201587.542299392</v>
+        <v>1387498.062848641</v>
       </c>
       <c r="AL98" t="n">
-        <v>209379.791076957</v>
+        <v>204901.4787985922</v>
       </c>
       <c r="AM98" t="n">
         <v>0</v>
@@ -12703,16 +12703,16 @@
       <c r="AA99" t="inlineStr"/>
       <c r="AB99" t="inlineStr"/>
       <c r="AC99" t="n">
-        <v>10195.87196380173</v>
+        <v>10082.04004009017</v>
       </c>
       <c r="AD99" t="n">
         <v>3397.621743246732</v>
       </c>
       <c r="AE99" t="n">
-        <v>693.5270099022373</v>
+        <v>809.1966239260577</v>
       </c>
       <c r="AF99" t="n">
-        <v>164.6010584906397</v>
+        <v>162.7633681783771</v>
       </c>
       <c r="AG99" t="n">
         <v>0</v>
@@ -12721,16 +12721,16 @@
         <v>20796.23621343998</v>
       </c>
       <c r="AI99" t="n">
-        <v>20211.40702621268</v>
+        <v>19779.11605972084</v>
       </c>
       <c r="AJ99" t="n">
-        <v>10478.46240084866</v>
+        <v>10254.34417727638</v>
       </c>
       <c r="AK99" t="n">
-        <v>4347.260681820514</v>
+        <v>5019.872096194815</v>
       </c>
       <c r="AL99" t="n">
-        <v>757.5216130942982</v>
+        <v>741.319388784121</v>
       </c>
       <c r="AM99" t="n">
         <v>0</v>
@@ -12800,7 +12800,7 @@
         <v>0</v>
       </c>
       <c r="R100" t="n">
-        <v>8820.949143814689</v>
+        <v>8820.949143814692</v>
       </c>
       <c r="S100" t="n">
         <v>0</v>
@@ -13069,7 +13069,7 @@
       <c r="AA102" t="inlineStr"/>
       <c r="AB102" t="inlineStr"/>
       <c r="AC102" t="n">
-        <v>903217.1789730818</v>
+        <v>903217.1789730814</v>
       </c>
       <c r="AD102" t="n">
         <v>30134720.58012468</v>
@@ -13087,7 +13087,7 @@
         <v>57993770.72054631</v>
       </c>
       <c r="AI102" t="n">
-        <v>903217.1789730818</v>
+        <v>903217.1789730814</v>
       </c>
       <c r="AJ102" t="n">
         <v>87133699.34247705</v>
@@ -13205,7 +13205,7 @@
         <v>2121333.333333333</v>
       </c>
       <c r="AE103" t="n">
-        <v>1348129.249911072</v>
+        <v>2405713.402858553</v>
       </c>
       <c r="AF103" t="n">
         <v>40727.27272727273</v>
@@ -13217,16 +13217,16 @@
         <v>8443271.902656633</v>
       </c>
       <c r="AI103" t="n">
-        <v>76862963.53583883</v>
+        <v>76790471.39743949</v>
       </c>
       <c r="AJ103" t="n">
-        <v>2276011.433750326</v>
+        <v>2273864.848083265</v>
       </c>
       <c r="AK103" t="n">
-        <v>1446428.780784499</v>
+        <v>2578692.869888201</v>
       </c>
       <c r="AL103" t="n">
-        <v>43696.92256100277</v>
+        <v>43655.71047117176</v>
       </c>
       <c r="AM103" t="n">
         <v>0</v>
@@ -13435,16 +13435,16 @@
       <c r="AA105" t="inlineStr"/>
       <c r="AB105" t="inlineStr"/>
       <c r="AC105" t="n">
-        <v>232058.5104437706</v>
+        <v>227737.8389953337</v>
       </c>
       <c r="AD105" t="n">
-        <v>15758.41217318877</v>
+        <v>15465.00805963485</v>
       </c>
       <c r="AE105" t="n">
-        <v>13436.79653675778</v>
+        <v>13186.61832504814</v>
       </c>
       <c r="AF105" t="n">
-        <v>9097.35162100259</v>
+        <v>13961.60539470309</v>
       </c>
       <c r="AG105" t="n">
         <v>0</v>
@@ -13453,16 +13453,16 @@
         <v>180234.0471831465</v>
       </c>
       <c r="AI105" t="n">
-        <v>289732.8363783678</v>
+        <v>284338.3331066681</v>
       </c>
       <c r="AJ105" t="n">
-        <v>57758.62660678953</v>
+        <v>56625.04883938785</v>
       </c>
       <c r="AK105" t="n">
-        <v>26604.40048562244</v>
+        <v>26082.25931507724</v>
       </c>
       <c r="AL105" t="n">
-        <v>13224.60830670305</v>
+        <v>20274.83051634959</v>
       </c>
       <c r="AM105" t="n">
         <v>0</v>
@@ -13553,16 +13553,16 @@
       <c r="AA106" t="inlineStr"/>
       <c r="AB106" t="inlineStr"/>
       <c r="AC106" t="n">
-        <v>5906.092935962078</v>
+        <v>5599.633872683997</v>
       </c>
       <c r="AD106" t="n">
-        <v>6720784.660670296</v>
+        <v>6372052.361003697</v>
       </c>
       <c r="AE106" t="n">
-        <v>2236417.633251222</v>
+        <v>2120372.989115749</v>
       </c>
       <c r="AF106" t="n">
-        <v>852256.752803503</v>
+        <v>1317340.155668855</v>
       </c>
       <c r="AG106" t="n">
         <v>0</v>
@@ -13571,16 +13571,16 @@
         <v>26537839.08130562</v>
       </c>
       <c r="AI106" t="n">
-        <v>5906.092935962078</v>
+        <v>5599.633872683997</v>
       </c>
       <c r="AJ106" t="n">
-        <v>37129551.76073276</v>
+        <v>36196951.25202408</v>
       </c>
       <c r="AK106" t="n">
-        <v>6674303.741059256</v>
+        <v>6506662.097974005</v>
       </c>
       <c r="AL106" t="n">
-        <v>1867383.905056378</v>
+        <v>2967932.515913589</v>
       </c>
       <c r="AM106" t="n">
         <v>0</v>
@@ -13922,13 +13922,13 @@
         <v>480000</v>
       </c>
       <c r="AD109" t="n">
-        <v>27394.3473363351</v>
+        <v>28407.60245145304</v>
       </c>
       <c r="AE109" t="n">
-        <v>43424.44271826455</v>
+        <v>49371.96820773368</v>
       </c>
       <c r="AF109" t="n">
-        <v>102709.0232840831</v>
+        <v>106507.9983767778</v>
       </c>
       <c r="AG109" t="n">
         <v>0</v>
@@ -13940,13 +13940,13 @@
         <v>480000</v>
       </c>
       <c r="AJ109" t="n">
-        <v>683089.9974306475</v>
+        <v>683941.9830081606</v>
       </c>
       <c r="AK109" t="n">
-        <v>584930.887592665</v>
+        <v>642123.3395055498</v>
       </c>
       <c r="AL109" t="n">
-        <v>1015755.077118082</v>
+        <v>1017021.979984827</v>
       </c>
       <c r="AM109" t="n">
         <v>0</v>
@@ -14805,16 +14805,16 @@
       <c r="AA116" t="inlineStr"/>
       <c r="AB116" t="inlineStr"/>
       <c r="AC116" t="n">
-        <v>1526230.97253403</v>
+        <v>1497814.248777002</v>
       </c>
       <c r="AD116" t="n">
-        <v>103641.8646775107</v>
+        <v>101712.1683922138</v>
       </c>
       <c r="AE116" t="n">
-        <v>88372.77722252229</v>
+        <v>86727.37436858581</v>
       </c>
       <c r="AF116" t="n">
-        <v>59832.58181505548</v>
+        <v>91824.40471131647</v>
       </c>
       <c r="AG116" t="n">
         <v>0</v>
@@ -14823,16 +14823,16 @@
         <v>1185385.464166079</v>
       </c>
       <c r="AI116" t="n">
-        <v>1905550.577719265</v>
+        <v>1870071.344663087</v>
       </c>
       <c r="AJ116" t="n">
-        <v>379874.0442215775</v>
+        <v>372418.5904436662</v>
       </c>
       <c r="AK116" t="n">
-        <v>174975.0955015938</v>
+        <v>171541.0131876233</v>
       </c>
       <c r="AL116" t="n">
-        <v>86977.23155562393</v>
+        <v>133346.0007036838</v>
       </c>
       <c r="AM116" t="n">
         <v>0</v>
@@ -14923,16 +14923,16 @@
       <c r="AA117" t="inlineStr"/>
       <c r="AB117" t="inlineStr"/>
       <c r="AC117" t="n">
-        <v>640431.5522448984</v>
+        <v>634849.6534134895</v>
       </c>
       <c r="AD117" t="n">
-        <v>133906.5357726938</v>
+        <v>132739.4278547163</v>
       </c>
       <c r="AE117" t="n">
-        <v>177437.0995930693</v>
+        <v>180832.4928930639</v>
       </c>
       <c r="AF117" t="n">
-        <v>65219.55700842418</v>
+        <v>68573.17045781578</v>
       </c>
       <c r="AG117" t="n">
         <v>0</v>
@@ -14941,16 +14941,16 @@
         <v>659435.8576546394</v>
       </c>
       <c r="AI117" t="n">
-        <v>815309.3677071643</v>
+        <v>808203.2618463757</v>
       </c>
       <c r="AJ117" t="n">
-        <v>329836.4085208391</v>
+        <v>328088.3280163931</v>
       </c>
       <c r="AK117" t="n">
-        <v>236099.2358163852</v>
+        <v>241446.3484779999</v>
       </c>
       <c r="AL117" t="n">
-        <v>63714.47328335026</v>
+        <v>67221.54698697005</v>
       </c>
       <c r="AM117" t="n">
         <v>0</v>
@@ -15023,7 +15023,7 @@
         <v>24650831.96721312</v>
       </c>
       <c r="S118" t="n">
-        <v>9726597.052959697</v>
+        <v>9726597.052959695</v>
       </c>
       <c r="T118" t="n">
         <v>12390000</v>
@@ -15062,7 +15062,7 @@
         <v>37562158.46994536</v>
       </c>
       <c r="AF118" t="n">
-        <v>5312177.527558546</v>
+        <v>5312177.527558545</v>
       </c>
       <c r="AG118" t="n">
         <v>15134878.18085425</v>
@@ -15301,16 +15301,16 @@
       <c r="AA120" t="inlineStr"/>
       <c r="AB120" t="inlineStr"/>
       <c r="AC120" t="n">
-        <v>2173108.799387215</v>
+        <v>2130192.998814512</v>
       </c>
       <c r="AD120" t="n">
         <v>215400</v>
       </c>
       <c r="AE120" t="n">
-        <v>125828.7004159636</v>
+        <v>123343.7629775359</v>
       </c>
       <c r="AF120" t="n">
-        <v>85192.02687681891</v>
+        <v>130592.7648879501</v>
       </c>
       <c r="AG120" t="n">
         <v>0</v>
@@ -15319,16 +15319,16 @@
         <v>1733019.684453332</v>
       </c>
       <c r="AI120" t="n">
-        <v>2713199.248763638</v>
+        <v>2659617.431826179</v>
       </c>
       <c r="AJ120" t="n">
-        <v>598396.0350228033</v>
+        <v>585383.4448685346</v>
       </c>
       <c r="AK120" t="n">
-        <v>275629.2644064326</v>
+        <v>269635.4903131487</v>
       </c>
       <c r="AL120" t="n">
-        <v>137010.7573598451</v>
+        <v>209598.9385448575</v>
       </c>
       <c r="AM120" t="n">
         <v>0</v>
@@ -15528,7 +15528,7 @@
         <v>214438.8888888889</v>
       </c>
       <c r="R122" t="n">
-        <v>841999.691000493</v>
+        <v>841999.6910004934</v>
       </c>
       <c r="S122" t="n">
         <v>270000</v>
@@ -15700,7 +15700,7 @@
         <v>538333.3333333333</v>
       </c>
       <c r="AF123" t="n">
-        <v>105243.0515018339</v>
+        <v>171577.9820900486</v>
       </c>
       <c r="AG123" t="n">
         <v>0</v>
@@ -15709,16 +15709,16 @@
         <v>1162698.661024144</v>
       </c>
       <c r="AI123" t="n">
-        <v>4533390.243481529</v>
+        <v>4524690.417759132</v>
       </c>
       <c r="AJ123" t="n">
-        <v>182741.8517988177</v>
+        <v>182391.1601139085</v>
       </c>
       <c r="AK123" t="n">
-        <v>624609.7156721494</v>
+        <v>623411.0552041526</v>
       </c>
       <c r="AL123" t="n">
-        <v>122109.9055263712</v>
+        <v>198694.013989888</v>
       </c>
       <c r="AM123" t="n">
         <v>0</v>
@@ -16066,10 +16066,10 @@
         <v>965085.073387019</v>
       </c>
       <c r="AJ126" t="n">
-        <v>436481.0041289604</v>
+        <v>417895.960910767</v>
       </c>
       <c r="AK126" t="n">
-        <v>373759.273481986</v>
+        <v>392344.3167001793</v>
       </c>
       <c r="AL126" t="n">
         <v>1227486.87070012</v>
@@ -16166,10 +16166,10 @@
         <v>90000</v>
       </c>
       <c r="AD127" t="n">
-        <v>165367.6385476666</v>
+        <v>161605.6987988589</v>
       </c>
       <c r="AE127" t="n">
-        <v>335464.2665640436</v>
+        <v>339226.2063128514</v>
       </c>
       <c r="AF127" t="n">
         <v>320000</v>
@@ -16184,13 +16184,13 @@
         <v>90000</v>
       </c>
       <c r="AJ127" t="n">
-        <v>1355537.293489406</v>
+        <v>1325664.327569368</v>
       </c>
       <c r="AK127" t="n">
-        <v>1485458.575470499</v>
+        <v>1503209.900265977</v>
       </c>
       <c r="AL127" t="n">
-        <v>325061.4850479269</v>
+        <v>337183.1261724865</v>
       </c>
       <c r="AM127" t="n">
         <v>0</v>
@@ -16753,16 +16753,16 @@
       <c r="AA132" t="inlineStr"/>
       <c r="AB132" t="inlineStr"/>
       <c r="AC132" t="n">
-        <v>637634.7868781403</v>
+        <v>625762.7361055741</v>
       </c>
       <c r="AD132" t="n">
-        <v>43299.90642607282</v>
+        <v>42493.7103117508</v>
       </c>
       <c r="AE132" t="n">
-        <v>36920.72693070443</v>
+        <v>36233.30404584676</v>
       </c>
       <c r="AF132" t="n">
-        <v>24997.09168571544</v>
+        <v>38362.76145746145</v>
       </c>
       <c r="AG132" t="n">
         <v>0</v>
@@ -16771,16 +16771,16 @@
         <v>495235.0079470887</v>
       </c>
       <c r="AI132" t="n">
-        <v>796108.4255105752</v>
+        <v>781285.7717867977</v>
       </c>
       <c r="AJ132" t="n">
-        <v>158705.2743567369</v>
+        <v>155590.5055135485</v>
       </c>
       <c r="AK132" t="n">
-        <v>73101.78455093126</v>
+        <v>71667.08011641508</v>
       </c>
       <c r="AL132" t="n">
-        <v>36337.69036552843</v>
+        <v>55709.81736701058</v>
       </c>
       <c r="AM132" t="n">
         <v>0</v>
@@ -16850,7 +16850,7 @@
         <v>100000</v>
       </c>
       <c r="R133" t="n">
-        <v>40095.22338097586</v>
+        <v>40095.22338097587</v>
       </c>
       <c r="S133" t="n">
         <v>60000</v>
@@ -16889,7 +16889,7 @@
         <v>5454545.454545455</v>
       </c>
       <c r="AE133" t="n">
-        <v>3207617.870478068</v>
+        <v>3207617.87047807</v>
       </c>
       <c r="AF133" t="n">
         <v>19422000</v>
@@ -16907,7 +16907,7 @@
         <v>1390404.275885058</v>
       </c>
       <c r="AK133" t="n">
-        <v>441690.9361146545</v>
+        <v>441690.9361146546</v>
       </c>
       <c r="AL133" t="n">
         <v>30345113.36524026</v>
@@ -17270,7 +17270,7 @@
         <v>25117826.08695652</v>
       </c>
       <c r="AF136" t="n">
-        <v>925214.8246960299</v>
+        <v>925214.8246960298</v>
       </c>
       <c r="AG136" t="n">
         <v>0</v>
@@ -17288,7 +17288,7 @@
         <v>25274775.93892141</v>
       </c>
       <c r="AL136" t="n">
-        <v>930996.0706234857</v>
+        <v>930996.0706234856</v>
       </c>
       <c r="AM136" t="n">
         <v>0</v>
@@ -17367,7 +17367,7 @@
         <v>0</v>
       </c>
       <c r="U137" t="n">
-        <v>326535.089561653</v>
+        <v>326535.0895616529</v>
       </c>
       <c r="V137" t="inlineStr"/>
       <c r="W137" t="n">
@@ -17412,7 +17412,7 @@
         <v>0</v>
       </c>
       <c r="AN137" t="n">
-        <v>79454.33425614539</v>
+        <v>79454.33425614538</v>
       </c>
     </row>
     <row r="138">
@@ -17745,7 +17745,7 @@
       <c r="AA140" t="inlineStr"/>
       <c r="AB140" t="inlineStr"/>
       <c r="AC140" t="n">
-        <v>466291.536694327</v>
+        <v>466291.5366943267</v>
       </c>
       <c r="AD140" t="n">
         <v>15557238.60692786</v>
@@ -17763,7 +17763,7 @@
         <v>29939648.06861576</v>
       </c>
       <c r="AI140" t="n">
-        <v>466291.536694327</v>
+        <v>466291.5366943267</v>
       </c>
       <c r="AJ140" t="n">
         <v>44983319.08440812</v>
@@ -18359,13 +18359,13 @@
       <c r="AA145" t="inlineStr"/>
       <c r="AB145" t="inlineStr"/>
       <c r="AC145" t="n">
-        <v>1408463.557093569</v>
+        <v>1393713.099053373</v>
       </c>
       <c r="AD145" t="n">
-        <v>124744.047278783</v>
+        <v>123437.6365975249</v>
       </c>
       <c r="AE145" t="n">
-        <v>95804.21593908973</v>
+        <v>111861.0846605432</v>
       </c>
       <c r="AF145" t="n">
         <v>110000</v>
@@ -18377,13 +18377,13 @@
         <v>2502480.424350611</v>
       </c>
       <c r="AI145" t="n">
-        <v>2421235.170412616</v>
+        <v>2368353.46936605</v>
       </c>
       <c r="AJ145" t="n">
-        <v>1255272.414427998</v>
+        <v>1227856.266933135</v>
       </c>
       <c r="AK145" t="n">
-        <v>520782.1723705163</v>
+        <v>601080.0209119461</v>
       </c>
       <c r="AL145" t="n">
         <v>110000</v>
@@ -18961,7 +18961,7 @@
         <v>0</v>
       </c>
       <c r="U150" t="n">
-        <v>195921.0537369918</v>
+        <v>195921.0537369917</v>
       </c>
       <c r="V150" t="inlineStr"/>
       <c r="W150" t="n">
@@ -19006,7 +19006,7 @@
         <v>0</v>
       </c>
       <c r="AN150" t="n">
-        <v>47672.60055368724</v>
+        <v>47672.60055368721</v>
       </c>
     </row>
     <row r="151">
@@ -19079,7 +19079,7 @@
         <v>0</v>
       </c>
       <c r="U151" t="n">
-        <v>682943.2893512131</v>
+        <v>682943.2893512129</v>
       </c>
       <c r="V151" t="inlineStr"/>
       <c r="W151" t="n">
@@ -19091,34 +19091,34 @@
       <c r="AA151" t="inlineStr"/>
       <c r="AB151" t="inlineStr"/>
       <c r="AC151" t="n">
-        <v>446.514679893511</v>
+        <v>446.5146798935019</v>
       </c>
       <c r="AD151" t="n">
         <v>340000</v>
       </c>
       <c r="AE151" t="n">
-        <v>2360.033951017612</v>
+        <v>2360.033951017564</v>
       </c>
       <c r="AF151" t="n">
-        <v>16.03674881513017</v>
+        <v>16.03674881512984</v>
       </c>
       <c r="AG151" t="n">
         <v>0</v>
       </c>
       <c r="AH151" t="n">
-        <v>473421.6655243839</v>
+        <v>473421.6655243838</v>
       </c>
       <c r="AI151" t="n">
-        <v>16338.60361582983</v>
+        <v>16338.60361582982</v>
       </c>
       <c r="AJ151" t="n">
-        <v>524084.0417147883</v>
+        <v>524084.0417147881</v>
       </c>
       <c r="AK151" t="n">
-        <v>273072.2535123955</v>
+        <v>273072.2535123954</v>
       </c>
       <c r="AL151" t="n">
-        <v>1362.340763235291</v>
+        <v>1362.34076323529</v>
       </c>
       <c r="AM151" t="n">
         <v>0</v>
@@ -19327,13 +19327,13 @@
       <c r="AA153" t="inlineStr"/>
       <c r="AB153" t="inlineStr"/>
       <c r="AC153" t="n">
-        <v>592423.0119883594</v>
+        <v>592423.0119883593</v>
       </c>
       <c r="AD153" t="n">
         <v>19765458.79231679</v>
       </c>
       <c r="AE153" t="n">
-        <v>4800486.662691715</v>
+        <v>4800486.662691716</v>
       </c>
       <c r="AF153" t="n">
         <v>259253.5716520039</v>
@@ -19345,7 +19345,7 @@
         <v>38126433.0579733</v>
       </c>
       <c r="AI153" t="n">
-        <v>592423.0119883594</v>
+        <v>592423.0119883593</v>
       </c>
       <c r="AJ153" t="n">
         <v>57259448.80068421</v>
@@ -19557,7 +19557,7 @@
         <v>4750000</v>
       </c>
       <c r="S155" t="n">
-        <v>989564.1367141178</v>
+        <v>989564.1367141177</v>
       </c>
       <c r="T155" t="n">
         <v>217380000</v>
@@ -19596,7 +19596,7 @@
         <v>5654761.904761905</v>
       </c>
       <c r="AF155" t="n">
-        <v>2090628.457846728</v>
+        <v>2090628.457846727</v>
       </c>
       <c r="AG155" t="n">
         <v>265538322.7565857</v>
@@ -19605,16 +19605,16 @@
         <v>521132883.2725925</v>
       </c>
       <c r="AI155" t="n">
-        <v>525590235.6205999</v>
+        <v>524487351.369709</v>
       </c>
       <c r="AJ155" t="n">
-        <v>1145039445.942852</v>
+        <v>1142636726.322142</v>
       </c>
       <c r="AK155" t="n">
-        <v>1185327566.501702</v>
+        <v>1189562291.796519</v>
       </c>
       <c r="AL155" t="n">
-        <v>347469918.3659917</v>
+        <v>346740796.9427755</v>
       </c>
       <c r="AM155" t="n">
         <v>470364680.1906371</v>
@@ -19726,7 +19726,7 @@
         <v>0</v>
       </c>
       <c r="AF156" t="n">
-        <v>269853.9782098305</v>
+        <v>439943.5438206373</v>
       </c>
       <c r="AG156" t="n">
         <v>0</v>
@@ -19735,16 +19735,16 @@
         <v>318875.6219394131</v>
       </c>
       <c r="AI156" t="n">
-        <v>1428969.629171655</v>
+        <v>1412194.774382879</v>
       </c>
       <c r="AJ156" t="n">
-        <v>15121.37173726619</v>
+        <v>14943.86004637966</v>
       </c>
       <c r="AK156" t="n">
         <v>0</v>
       </c>
       <c r="AL156" t="n">
-        <v>306042.1739468232</v>
+        <v>493084.1060372929</v>
       </c>
       <c r="AM156" t="n">
         <v>0</v>
@@ -20083,16 +20083,16 @@
       <c r="AA159" t="inlineStr"/>
       <c r="AB159" t="inlineStr"/>
       <c r="AC159" t="n">
-        <v>2492955.767442293</v>
+        <v>2452576.274776584</v>
       </c>
       <c r="AD159" t="n">
-        <v>845703.6178732684</v>
+        <v>832005.3872503029</v>
       </c>
       <c r="AE159" t="n">
-        <v>1340576.136386242</v>
+        <v>1446012.334134308</v>
       </c>
       <c r="AF159" t="n">
-        <v>3170777.953317702</v>
+        <v>3119419.478858309</v>
       </c>
       <c r="AG159" t="n">
         <v>0</v>
@@ -20101,16 +20101,16 @@
         <v>4367209.604822396</v>
       </c>
       <c r="AI159" t="n">
-        <v>3543415.448710754</v>
+        <v>3486021.202093387</v>
       </c>
       <c r="AJ159" t="n">
-        <v>1418952.923586036</v>
+        <v>1425787.832766579</v>
       </c>
       <c r="AK159" t="n">
-        <v>1215051.30534378</v>
+        <v>1338610.097563688</v>
       </c>
       <c r="AL159" t="n">
-        <v>4506852.360138191</v>
+        <v>4433852.905355109</v>
       </c>
       <c r="AM159" t="n">
         <v>0</v>
@@ -20331,16 +20331,16 @@
       <c r="AA161" t="inlineStr"/>
       <c r="AB161" t="inlineStr"/>
       <c r="AC161" t="n">
-        <v>41076.80498820011</v>
+        <v>40652.47950978388</v>
       </c>
       <c r="AD161" t="n">
-        <v>3638.068502164998</v>
+        <v>3600.487070061512</v>
       </c>
       <c r="AE161" t="n">
-        <v>2794.059580283457</v>
+        <v>3262.816755610319</v>
       </c>
       <c r="AF161" t="n">
-        <v>663.1395141559084</v>
+        <v>656.2892493487565</v>
       </c>
       <c r="AG161" t="n">
         <v>0</v>
@@ -20349,16 +20349,16 @@
         <v>69320.78737813327</v>
       </c>
       <c r="AI161" t="n">
-        <v>67371.35675404228</v>
+        <v>65930.38686573616</v>
       </c>
       <c r="AJ161" t="n">
-        <v>34928.20800282888</v>
+        <v>34181.14725758793</v>
       </c>
       <c r="AK161" t="n">
-        <v>14490.86893940171</v>
+        <v>16732.90698731605</v>
       </c>
       <c r="AL161" t="n">
-        <v>2525.072043647661</v>
+        <v>2471.064629280404</v>
       </c>
       <c r="AM161" t="n">
         <v>0</v>
@@ -20685,16 +20685,16 @@
       <c r="AA164" t="inlineStr"/>
       <c r="AB164" t="inlineStr"/>
       <c r="AC164" t="n">
-        <v>285293.7679905175</v>
+        <v>279659.622817865</v>
       </c>
       <c r="AD164" t="n">
         <v>70000</v>
       </c>
       <c r="AE164" t="n">
-        <v>16519.25760603566</v>
+        <v>16193.02581992829</v>
       </c>
       <c r="AF164" t="n">
-        <v>11184.32466763316</v>
+        <v>17144.70162639305</v>
       </c>
       <c r="AG164" t="n">
         <v>0</v>
@@ -20703,16 +20703,16 @@
         <v>255331.5668427909</v>
       </c>
       <c r="AI164" t="n">
-        <v>356198.8415891064</v>
+        <v>349164.4223027013</v>
       </c>
       <c r="AJ164" t="n">
-        <v>113936.9103101186</v>
+        <v>109717.4575488064</v>
       </c>
       <c r="AK164" t="n">
-        <v>52480.87376836137</v>
+        <v>50537.33705900823</v>
       </c>
       <c r="AL164" t="n">
-        <v>26087.37601718103</v>
+        <v>39284.78477425148</v>
       </c>
       <c r="AM164" t="n">
         <v>0</v>
@@ -20933,16 +20933,16 @@
       <c r="AA166" t="inlineStr"/>
       <c r="AB166" t="inlineStr"/>
       <c r="AC166" t="n">
-        <v>458080.9970825106</v>
+        <v>449034.5504791552</v>
       </c>
       <c r="AD166" t="n">
         <v>69333.33333333333</v>
       </c>
       <c r="AE166" t="n">
-        <v>26524.09146030548</v>
+        <v>26000.27846953226</v>
       </c>
       <c r="AF166" t="n">
-        <v>17958.07399345016</v>
+        <v>27528.33358757876</v>
       </c>
       <c r="AG166" t="n">
         <v>0</v>
@@ -20951,16 +20951,16 @@
         <v>381264.330579733</v>
       </c>
       <c r="AI166" t="n">
-        <v>571929.494513867</v>
+        <v>560634.7024007773</v>
       </c>
       <c r="AJ166" t="n">
-        <v>146428.5453024366</v>
+        <v>142245.3846769523</v>
       </c>
       <c r="AK166" t="n">
-        <v>67446.95798038931</v>
+        <v>65520.13791706413</v>
       </c>
       <c r="AL166" t="n">
-        <v>33526.76942490553</v>
+        <v>50931.54222680466</v>
       </c>
       <c r="AM166" t="n">
         <v>0</v>
@@ -21051,16 +21051,16 @@
       <c r="AA167" t="inlineStr"/>
       <c r="AB167" t="inlineStr"/>
       <c r="AC167" t="n">
-        <v>31656.58117387038</v>
+        <v>31143.82571144869</v>
       </c>
       <c r="AD167" t="n">
-        <v>10739.09356029547</v>
+        <v>10565.14777460702</v>
       </c>
       <c r="AE167" t="n">
-        <v>17023.18903347609</v>
+        <v>18362.06138583248</v>
       </c>
       <c r="AF167" t="n">
-        <v>40263.84702625653</v>
+        <v>39611.67592201028</v>
       </c>
       <c r="AG167" t="n">
         <v>0</v>
@@ -21069,16 +21069,16 @@
         <v>55456.62990250662</v>
       </c>
       <c r="AI167" t="n">
-        <v>44995.75172966039</v>
+        <v>44266.93589959857</v>
       </c>
       <c r="AJ167" t="n">
-        <v>18018.44982331476</v>
+        <v>18105.24232084544</v>
       </c>
       <c r="AK167" t="n">
-        <v>15429.22292500038</v>
+        <v>16998.22346112619</v>
       </c>
       <c r="AL167" t="n">
-        <v>57229.87123985006</v>
+        <v>56302.89403625536</v>
       </c>
       <c r="AM167" t="n">
         <v>0</v>
@@ -21305,7 +21305,7 @@
         <v>1355555.555555556</v>
       </c>
       <c r="AE169" t="n">
-        <v>1685161.56238884</v>
+        <v>3007141.75357319</v>
       </c>
       <c r="AF169" t="n">
         <v>2151543.637950003</v>
@@ -21317,16 +21317,16 @@
         <v>2426227.558234665</v>
       </c>
       <c r="AI169" t="n">
-        <v>40109280.30861887</v>
+        <v>40025116.08605734</v>
       </c>
       <c r="AJ169" t="n">
-        <v>87381204.95621219</v>
+        <v>87197846.61307956</v>
       </c>
       <c r="AK169" t="n">
-        <v>90455705.60536198</v>
+        <v>90778869.49306105</v>
       </c>
       <c r="AL169" t="n">
-        <v>26516414.1379042</v>
+        <v>26460772.8158993</v>
       </c>
       <c r="AM169" t="n">
         <v>49002736.49067763</v>
@@ -21435,7 +21435,7 @@
         <v>3282524.27184466</v>
       </c>
       <c r="AE170" t="n">
-        <v>343772.9587273233</v>
+        <v>613456.9177289308</v>
       </c>
       <c r="AF170" t="n">
         <v>87000</v>
@@ -21447,16 +21447,16 @@
         <v>2526546.509025285</v>
       </c>
       <c r="AI170" t="n">
-        <v>18209357.01012741</v>
+        <v>17674193.5342041</v>
       </c>
       <c r="AJ170" t="n">
-        <v>45678344.71771745</v>
+        <v>44335882.06404101</v>
       </c>
       <c r="AK170" t="n">
-        <v>2584207.942683534</v>
+        <v>4475945.694902288</v>
       </c>
       <c r="AL170" t="n">
-        <v>480159.0277031825</v>
+        <v>466047.4050841805</v>
       </c>
       <c r="AM170" t="n">
         <v>12766988.45668056</v>
@@ -21577,16 +21577,16 @@
         <v>1615174.345910505</v>
       </c>
       <c r="AI171" t="n">
-        <v>88307176.35555273</v>
+        <v>88121874.97922829</v>
       </c>
       <c r="AJ171" t="n">
-        <v>192384092.0818216</v>
+        <v>191980398.5371186</v>
       </c>
       <c r="AK171" t="n">
-        <v>199153110.8460748</v>
+        <v>199864609.2874132</v>
       </c>
       <c r="AL171" t="n">
-        <v>58380246.20675147</v>
+        <v>58257742.68644056</v>
       </c>
       <c r="AM171" t="n">
         <v>109195658.3974819</v>
@@ -21665,7 +21665,7 @@
         <v>0</v>
       </c>
       <c r="U172" t="n">
-        <v>65307.0179123306</v>
+        <v>65307.01791233057</v>
       </c>
       <c r="V172" t="inlineStr"/>
       <c r="W172" t="n">
@@ -21692,7 +21692,7 @@
         <v>0</v>
       </c>
       <c r="AH172" t="n">
-        <v>45271.33903000611</v>
+        <v>45271.33903000609</v>
       </c>
       <c r="AI172" t="n">
         <v>316019.8866841751</v>
@@ -21710,7 +21710,7 @@
         <v>0</v>
       </c>
       <c r="AN172" t="n">
-        <v>15890.86685122908</v>
+        <v>15890.86685122907</v>
       </c>
     </row>
     <row r="173">
@@ -21795,16 +21795,16 @@
       <c r="AA173" t="inlineStr"/>
       <c r="AB173" t="inlineStr"/>
       <c r="AC173" t="n">
-        <v>234721.3375376719</v>
+        <v>234396.8830381975</v>
       </c>
       <c r="AD173" t="n">
-        <v>108154.0739266977</v>
+        <v>108004.57292142</v>
       </c>
       <c r="AE173" t="n">
-        <v>169329.8747123422</v>
+        <v>169893.8137961988</v>
       </c>
       <c r="AF173" t="n">
-        <v>65097.15870191938</v>
+        <v>65007.17512281486</v>
       </c>
       <c r="AG173" t="n">
         <v>0</v>
@@ -21813,16 +21813,16 @@
         <v>374332.2518419197</v>
       </c>
       <c r="AI173" t="n">
-        <v>298814.9235065168</v>
+        <v>298401.8726630833</v>
       </c>
       <c r="AJ173" t="n">
-        <v>237600.0437916324</v>
+        <v>237372.5905010509</v>
       </c>
       <c r="AK173" t="n">
-        <v>200951.1767858811</v>
+        <v>201706.235636519</v>
       </c>
       <c r="AL173" t="n">
-        <v>82872.74903110864</v>
+        <v>82758.19431448581</v>
       </c>
       <c r="AM173" t="n">
         <v>0</v>
@@ -21913,16 +21913,16 @@
       <c r="AA174" t="inlineStr"/>
       <c r="AB174" t="inlineStr"/>
       <c r="AC174" t="n">
-        <v>17828938.70034235</v>
+        <v>17496983.68498356</v>
       </c>
       <c r="AD174" t="n">
-        <v>1210710.885428133</v>
+        <v>1188168.7948796</v>
       </c>
       <c r="AE174" t="n">
-        <v>1032342.32316972</v>
+        <v>1013121.256929991</v>
       </c>
       <c r="AF174" t="n">
-        <v>698944.9517543832</v>
+        <v>1072663.123901442</v>
       </c>
       <c r="AG174" t="n">
         <v>0</v>
@@ -21931,16 +21931,16 @@
         <v>13468211.74395816</v>
       </c>
       <c r="AI174" t="n">
-        <v>22697352.57064188</v>
+        <v>22274753.10200121</v>
       </c>
       <c r="AJ174" t="n">
-        <v>4033120.738715849</v>
+        <v>3979213.630488961</v>
       </c>
       <c r="AK174" t="n">
-        <v>1857709.672879459</v>
+        <v>1832879.333577013</v>
       </c>
       <c r="AL174" t="n">
-        <v>923436.8120672774</v>
+        <v>1424773.728237264</v>
       </c>
       <c r="AM174" t="n">
         <v>0</v>
@@ -22031,16 +22031,16 @@
       <c r="AA175" t="inlineStr"/>
       <c r="AB175" t="inlineStr"/>
       <c r="AC175" t="n">
-        <v>675714.8518288225</v>
+        <v>663133.7925864854</v>
       </c>
       <c r="AD175" t="n">
-        <v>45885.81184245725</v>
+        <v>45031.46904444083</v>
       </c>
       <c r="AE175" t="n">
-        <v>39125.66259055312</v>
+        <v>38397.1862552836</v>
       </c>
       <c r="AF175" t="n">
-        <v>26489.93820939816</v>
+        <v>40653.81658502125</v>
       </c>
       <c r="AG175" t="n">
         <v>0</v>
@@ -22049,16 +22049,16 @@
         <v>524810.8429808208</v>
       </c>
       <c r="AI175" t="n">
-        <v>843652.6642740443</v>
+        <v>827944.7896869157</v>
       </c>
       <c r="AJ175" t="n">
-        <v>168183.2816422389</v>
+        <v>164882.4962856859</v>
       </c>
       <c r="AK175" t="n">
-        <v>77467.48222144166</v>
+        <v>75947.09607824881</v>
       </c>
       <c r="AL175" t="n">
-        <v>38507.80661036495</v>
+        <v>59036.85269723932</v>
       </c>
       <c r="AM175" t="n">
         <v>0</v>
@@ -22149,16 +22149,16 @@
       <c r="AA176" t="inlineStr"/>
       <c r="AB176" t="inlineStr"/>
       <c r="AC176" t="n">
-        <v>591613.7017650041</v>
+        <v>579930.1746226054</v>
       </c>
       <c r="AD176" t="n">
         <v>110000</v>
       </c>
       <c r="AE176" t="n">
-        <v>34255.98537098533</v>
+        <v>33579.47849888707</v>
       </c>
       <c r="AF176" t="n">
-        <v>23192.93465456991</v>
+        <v>35552.96866906678</v>
       </c>
       <c r="AG176" t="n">
         <v>0</v>
@@ -22167,16 +22167,16 @@
         <v>506041.7478603729</v>
       </c>
       <c r="AI176" t="n">
-        <v>738649.5566350461</v>
+        <v>724062.280988928</v>
       </c>
       <c r="AJ176" t="n">
-        <v>206458.2994981266</v>
+        <v>199824.5522301774</v>
       </c>
       <c r="AK176" t="n">
-        <v>95097.47038865833</v>
+        <v>92041.87714821627</v>
       </c>
       <c r="AL176" t="n">
-        <v>47271.38269956301</v>
+        <v>71547.99885407199</v>
       </c>
       <c r="AM176" t="n">
         <v>0</v>
@@ -22515,16 +22515,16 @@
       <c r="AA179" t="inlineStr"/>
       <c r="AB179" t="inlineStr"/>
       <c r="AC179" t="n">
-        <v>21140214.09525225</v>
+        <v>20905972.84733798</v>
       </c>
       <c r="AD179" t="n">
-        <v>3020387.535010724</v>
+        <v>2986920.544459076</v>
       </c>
       <c r="AE179" t="n">
-        <v>4345855.419304927</v>
+        <v>4491923.195531805</v>
       </c>
       <c r="AF179" t="n">
-        <v>922671.9087599986</v>
+        <v>1044312.370999045</v>
       </c>
       <c r="AG179" t="n">
         <v>0</v>
@@ -22533,16 +22533,16 @@
         <v>23416561.97633342</v>
       </c>
       <c r="AI179" t="n">
-        <v>23406813.99587119</v>
+        <v>23147457.99808489</v>
       </c>
       <c r="AJ179" t="n">
-        <v>11177390.66257306</v>
+        <v>11008780.85879936</v>
       </c>
       <c r="AK179" t="n">
-        <v>8687731.058805911</v>
+        <v>8943370.278827228</v>
       </c>
       <c r="AL179" t="n">
-        <v>1354217.725205954</v>
+        <v>1526544.306744637</v>
       </c>
       <c r="AM179" t="n">
         <v>0</v>
@@ -22633,16 +22633,16 @@
       <c r="AA180" t="inlineStr"/>
       <c r="AB180" t="inlineStr"/>
       <c r="AC180" t="n">
-        <v>209491.7054398206</v>
+        <v>207327.6454998978</v>
       </c>
       <c r="AD180" t="n">
-        <v>18554.14936104149</v>
+        <v>18362.48405731371</v>
       </c>
       <c r="AE180" t="n">
-        <v>14249.70385944563</v>
+        <v>16640.36545361263</v>
       </c>
       <c r="AF180" t="n">
-        <v>3382.011522195134</v>
+        <v>3347.075171678659</v>
       </c>
       <c r="AG180" t="n">
         <v>0</v>
@@ -22651,16 +22651,16 @@
         <v>353536.0156284797</v>
       </c>
       <c r="AI180" t="n">
-        <v>343593.9194456156</v>
+        <v>336244.9730152544</v>
       </c>
       <c r="AJ180" t="n">
-        <v>178133.8608144273</v>
+        <v>174323.8510136984</v>
       </c>
       <c r="AK180" t="n">
-        <v>73903.43159094875</v>
+        <v>85337.82563531186</v>
       </c>
       <c r="AL180" t="n">
-        <v>12877.86742260307</v>
+        <v>12602.42960933006</v>
       </c>
       <c r="AM180" t="n">
         <v>0</v>
@@ -22730,7 +22730,7 @@
         <v>10000</v>
       </c>
       <c r="R181" t="n">
-        <v>5613.33127333662</v>
+        <v>5613.331273336622</v>
       </c>
       <c r="S181" t="n">
         <v>0</v>
@@ -23371,7 +23371,7 @@
         <v>532500</v>
       </c>
       <c r="AE186" t="n">
-        <v>224688.208318512</v>
+        <v>400952.2338097587</v>
       </c>
       <c r="AF186" t="n">
         <v>395000</v>
@@ -23383,16 +23383,16 @@
         <v>5670440.407531301</v>
       </c>
       <c r="AI186" t="n">
-        <v>19748524.35285219</v>
+        <v>19714177.94298904</v>
       </c>
       <c r="AJ186" t="n">
-        <v>644712.4930925914</v>
+        <v>643591.2164272567</v>
       </c>
       <c r="AK186" t="n">
-        <v>272036.2346545266</v>
+        <v>484599.6918062882</v>
       </c>
       <c r="AL186" t="n">
-        <v>478237.4361907486</v>
+        <v>477405.6910587163</v>
       </c>
       <c r="AM186" t="n">
         <v>0</v>
@@ -23958,7 +23958,7 @@
         <v>2649600</v>
       </c>
       <c r="R191" t="n">
-        <v>4009522.338097586</v>
+        <v>4009522.338097587</v>
       </c>
       <c r="S191" t="n">
         <v>0</v>
@@ -24012,10 +24012,10 @@
         <v>10363636.36363636</v>
       </c>
       <c r="AJ191" t="n">
-        <v>40895472.44496736</v>
+        <v>40895472.44496735</v>
       </c>
       <c r="AK191" t="n">
-        <v>29525682.53374077</v>
+        <v>29525682.53374078</v>
       </c>
       <c r="AL191" t="n">
         <v>0</v>
@@ -24454,7 +24454,7 @@
         <v>2076.324398650781</v>
       </c>
       <c r="R195" t="n">
-        <v>13632.37594953179</v>
+        <v>13632.3759495318</v>
       </c>
       <c r="S195" t="n">
         <v>0</v>
@@ -24475,16 +24475,16 @@
       <c r="AA195" t="inlineStr"/>
       <c r="AB195" t="inlineStr"/>
       <c r="AC195" t="n">
-        <v>13823.40056182755</v>
+        <v>13823.40056182754</v>
       </c>
       <c r="AD195" t="n">
         <v>1224.303550172448</v>
       </c>
       <c r="AE195" t="n">
-        <v>13632.37594953179</v>
+        <v>13632.3759495318</v>
       </c>
       <c r="AF195" t="n">
-        <v>223.1634893508913</v>
+        <v>223.1634893508911</v>
       </c>
       <c r="AG195" t="n">
         <v>0</v>
@@ -24493,16 +24493,16 @@
         <v>41592.47242687996</v>
       </c>
       <c r="AI195" t="n">
-        <v>37249.22840443785</v>
+        <v>37249.22840443784</v>
       </c>
       <c r="AJ195" t="n">
         <v>19311.60155205015</v>
       </c>
       <c r="AK195" t="n">
-        <v>13632.37594953179</v>
+        <v>13632.3759495318</v>
       </c>
       <c r="AL195" t="n">
-        <v>1396.097537932528</v>
+        <v>1396.097537932527</v>
       </c>
       <c r="AM195" t="n">
         <v>0</v>
@@ -24593,16 +24593,16 @@
       <c r="AA196" t="inlineStr"/>
       <c r="AB196" t="inlineStr"/>
       <c r="AC196" t="n">
-        <v>21541.81435729166</v>
+        <v>21301.31053601639</v>
       </c>
       <c r="AD196" t="n">
         <v>20000</v>
       </c>
       <c r="AE196" t="n">
-        <v>1465.282238941628</v>
+        <v>1709.668727995932</v>
       </c>
       <c r="AF196" t="n">
-        <v>347.7687300907361</v>
+        <v>343.8860623117075</v>
       </c>
       <c r="AG196" t="n">
         <v>0</v>
@@ -24611,16 +24611,16 @@
         <v>62388.70864031995</v>
       </c>
       <c r="AI196" t="n">
-        <v>60634.22107863805</v>
+        <v>59337.34817916254</v>
       </c>
       <c r="AJ196" t="n">
-        <v>31435.38720254599</v>
+        <v>30763.03253182913</v>
       </c>
       <c r="AK196" t="n">
-        <v>13041.78204546154</v>
+        <v>15059.61628858444</v>
       </c>
       <c r="AL196" t="n">
-        <v>2272.564839282894</v>
+        <v>2223.958166352363</v>
       </c>
       <c r="AM196" t="n">
         <v>0</v>
@@ -24732,7 +24732,7 @@
         <v>835052.1428571427</v>
       </c>
       <c r="AF197" t="n">
-        <v>68731.80825004382</v>
+        <v>112053.6206111163</v>
       </c>
       <c r="AG197" t="n">
         <v>0</v>
@@ -24741,16 +24741,16 @@
         <v>3833439.54201077</v>
       </c>
       <c r="AI197" t="n">
-        <v>474294.8368299662</v>
+        <v>464987.9577084708</v>
       </c>
       <c r="AJ197" t="n">
-        <v>2447108.874009134</v>
+        <v>2399090.332125436</v>
       </c>
       <c r="AK197" t="n">
-        <v>3467218.906673224</v>
+        <v>3399183.193976357</v>
       </c>
       <c r="AL197" t="n">
-        <v>209524.8499052824</v>
+        <v>334885.983607343</v>
       </c>
       <c r="AM197" t="n">
         <v>0</v>
@@ -24841,16 +24841,16 @@
       <c r="AA198" t="inlineStr"/>
       <c r="AB198" t="inlineStr"/>
       <c r="AC198" t="n">
-        <v>2010882.742556967</v>
+        <v>1971170.675319928</v>
       </c>
       <c r="AD198" t="n">
         <v>520000</v>
       </c>
       <c r="AE198" t="n">
-        <v>116435.3861418175</v>
+        <v>114135.9532681956</v>
       </c>
       <c r="AF198" t="n">
-        <v>78832.30545030771</v>
+        <v>120843.8055609684</v>
       </c>
       <c r="AG198" t="n">
         <v>0</v>
@@ -24859,16 +24859,16 @@
         <v>1767680.078142399</v>
       </c>
       <c r="AI198" t="n">
-        <v>2559979.332093298</v>
+        <v>2509423.390063457</v>
       </c>
       <c r="AJ198" t="n">
-        <v>777337.2586919279</v>
+        <v>749959.4638913326</v>
       </c>
       <c r="AK198" t="n">
-        <v>358051.9994601972</v>
+        <v>345441.4188408408</v>
       </c>
       <c r="AL198" t="n">
-        <v>177981.738353845</v>
+        <v>268526.0558036377</v>
       </c>
       <c r="AM198" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Clustered facilities due to CHN (p1_a)
</commit_message>
<xml_diff>
--- a/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
+++ b/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
@@ -1970,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>224948.8426581834</v>
+        <v>224948.8426581833</v>
       </c>
       <c r="W3">
         <v>60.36830343223809</v>
@@ -1991,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>204199.3492318432</v>
+        <v>204199.3492318431</v>
       </c>
       <c r="AI3">
         <v>799010.6069763988</v>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="AN3">
-        <v>147895.9639373562</v>
+        <v>147895.9639373561</v>
       </c>
     </row>
     <row r="4" spans="1:40">
@@ -2178,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <v>642008.4255763415</v>
+        <v>642008.4255763419</v>
       </c>
       <c r="V5">
         <v>3300</v>
@@ -2217,7 +2217,7 @@
         <v>0</v>
       </c>
       <c r="AH5">
-        <v>582788.9628365686</v>
+        <v>582788.9628365689</v>
       </c>
       <c r="AI5">
         <v>9603916.688964158</v>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="AN5">
-        <v>422097.9927458329</v>
+        <v>422097.9927458332</v>
       </c>
     </row>
     <row r="6" spans="1:40">
@@ -3094,7 +3094,7 @@
         <v>80000</v>
       </c>
       <c r="S13">
-        <v>297584.0373009848</v>
+        <v>297584.0373009847</v>
       </c>
       <c r="T13">
         <v>0</v>
@@ -3192,13 +3192,13 @@
         <v>260000</v>
       </c>
       <c r="Q14">
-        <v>25648.25627919202</v>
+        <v>25648.25627919203</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14">
-        <v>9881.45149493586</v>
+        <v>9881.451494935858</v>
       </c>
       <c r="T14">
         <v>0</v>
@@ -3213,13 +3213,13 @@
         <v>260000</v>
       </c>
       <c r="AD14">
-        <v>25648.25627919202</v>
+        <v>25648.25627919203</v>
       </c>
       <c r="AE14">
         <v>0</v>
       </c>
       <c r="AF14">
-        <v>9881.45149493586</v>
+        <v>9881.451494935858</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -3231,7 +3231,7 @@
         <v>286424.342787744</v>
       </c>
       <c r="AJ14">
-        <v>28254.94210930462</v>
+        <v>28254.94210930463</v>
       </c>
       <c r="AK14">
         <v>0</v>
@@ -3302,7 +3302,7 @@
         <v>14080000</v>
       </c>
       <c r="S15">
-        <v>3894331.553934014</v>
+        <v>3894331.553934013</v>
       </c>
       <c r="T15">
         <v>32820244.89795918</v>
@@ -3341,7 +3341,7 @@
         <v>27908571.42857143</v>
       </c>
       <c r="AF15">
-        <v>4436580.251317232</v>
+        <v>4436580.251317231</v>
       </c>
       <c r="AG15">
         <v>38284764.67859285</v>
@@ -3668,7 +3668,7 @@
         <v>5011764.705882354</v>
       </c>
       <c r="AE18">
-        <v>4372284.820731441</v>
+        <v>4372284.82073144</v>
       </c>
       <c r="AF18">
         <v>0</v>
@@ -3686,7 +3686,7 @@
         <v>106593626.8717267</v>
       </c>
       <c r="AK18">
-        <v>49567159.9340803</v>
+        <v>49567159.93408028</v>
       </c>
       <c r="AL18">
         <v>0</v>
@@ -3888,7 +3888,7 @@
         <v>40</v>
       </c>
       <c r="AC20">
-        <v>542384.9822387614</v>
+        <v>542384.9822387615</v>
       </c>
       <c r="AD20">
         <v>17056192.34151518</v>
@@ -3906,7 +3906,7 @@
         <v>35348871.47753028</v>
       </c>
       <c r="AI20">
-        <v>542384.9822387614</v>
+        <v>542384.9822387615</v>
       </c>
       <c r="AJ20">
         <v>48210351.55919283</v>
@@ -4741,7 +4741,7 @@
         <v>90000</v>
       </c>
       <c r="R28">
-        <v>3974.804382483129</v>
+        <v>3974.804382483127</v>
       </c>
       <c r="S28">
         <v>0</v>
@@ -4958,7 +4958,7 @@
         <v>0</v>
       </c>
       <c r="U30">
-        <v>64200.84255763415</v>
+        <v>64200.84255763418</v>
       </c>
       <c r="W30">
         <v>39.43333333333333</v>
@@ -4979,7 +4979,7 @@
         <v>0</v>
       </c>
       <c r="AH30">
-        <v>58278.89628365686</v>
+        <v>58278.89628365689</v>
       </c>
       <c r="AI30">
         <v>11176069.09700907</v>
@@ -4997,7 +4997,7 @@
         <v>0</v>
       </c>
       <c r="AN30">
-        <v>42209.7992745833</v>
+        <v>42209.79927458332</v>
       </c>
     </row>
     <row r="31" spans="1:40">
@@ -5172,7 +5172,7 @@
         <v>140000</v>
       </c>
       <c r="Q32">
-        <v>73280.7322262629</v>
+        <v>73280.73222626293</v>
       </c>
       <c r="R32">
         <v>0</v>
@@ -5184,46 +5184,46 @@
         <v>0</v>
       </c>
       <c r="U32">
-        <v>449405.8979034391</v>
+        <v>449405.8979034393</v>
       </c>
       <c r="W32">
         <v>60</v>
       </c>
       <c r="AC32">
-        <v>504305.6797883198</v>
+        <v>504305.67978832</v>
       </c>
       <c r="AD32">
-        <v>73280.7322262629</v>
+        <v>73280.73222626293</v>
       </c>
       <c r="AE32">
-        <v>29200.62185475807</v>
+        <v>29200.62185475808</v>
       </c>
       <c r="AF32">
-        <v>5141.377109056216</v>
+        <v>5141.377109056217</v>
       </c>
       <c r="AG32">
         <v>0</v>
       </c>
       <c r="AH32">
-        <v>407952.2739855981</v>
+        <v>407952.2739855982</v>
       </c>
       <c r="AI32">
-        <v>554096.1401805036</v>
+        <v>554096.1401805037</v>
       </c>
       <c r="AJ32">
-        <v>112815.4664275034</v>
+        <v>112815.4664275035</v>
       </c>
       <c r="AK32">
-        <v>51273.97097974449</v>
+        <v>51273.97097974453</v>
       </c>
       <c r="AL32">
-        <v>6226.512454160588</v>
+        <v>6226.512454160595</v>
       </c>
       <c r="AM32">
         <v>0</v>
       </c>
       <c r="AN32">
-        <v>295468.5949220831</v>
+        <v>295468.5949220833</v>
       </c>
     </row>
     <row r="33" spans="1:40">
@@ -5871,7 +5871,7 @@
         <v>20366.66666666666</v>
       </c>
       <c r="R38">
-        <v>397480.4382483129</v>
+        <v>397480.4382483127</v>
       </c>
       <c r="S38">
         <v>0</v>
@@ -5892,7 +5892,7 @@
         <v>20366.66666666666</v>
       </c>
       <c r="AE38">
-        <v>397480.4382483129</v>
+        <v>397480.4382483127</v>
       </c>
       <c r="AF38">
         <v>0</v>
@@ -5910,7 +5910,7 @@
         <v>22008.2823170145</v>
       </c>
       <c r="AK38">
-        <v>429518.57776397</v>
+        <v>429518.5777639698</v>
       </c>
       <c r="AL38">
         <v>0</v>
@@ -5984,7 +5984,7 @@
         <v>0</v>
       </c>
       <c r="U39">
-        <v>513606.7404610732</v>
+        <v>513606.7404610735</v>
       </c>
       <c r="W39">
         <v>60</v>
@@ -6005,7 +6005,7 @@
         <v>0</v>
       </c>
       <c r="AH39">
-        <v>466231.1702692549</v>
+        <v>466231.1702692552</v>
       </c>
       <c r="AI39">
         <v>13780731.97535679</v>
@@ -6023,7 +6023,7 @@
         <v>0</v>
       </c>
       <c r="AN39">
-        <v>337678.3941966664</v>
+        <v>337678.3941966666</v>
       </c>
     </row>
     <row r="40" spans="1:40">
@@ -6076,7 +6076,7 @@
         <v>1050000</v>
       </c>
       <c r="Q40">
-        <v>3664.036611313145</v>
+        <v>3664.036611313147</v>
       </c>
       <c r="R40">
         <v>0</v>
@@ -6183,7 +6183,7 @@
         <v>8058254.676258993</v>
       </c>
       <c r="R41">
-        <v>436831.0016348959</v>
+        <v>436831.0016348957</v>
       </c>
       <c r="S41">
         <v>2270000</v>
@@ -6222,7 +6222,7 @@
         <v>2309352.517985611</v>
       </c>
       <c r="AE41">
-        <v>11924413.14744939</v>
+        <v>11924413.14744938</v>
       </c>
       <c r="AF41">
         <v>0</v>
@@ -6234,7 +6234,7 @@
         <v>28313004.98051037</v>
       </c>
       <c r="AI41">
-        <v>63946953.45801272</v>
+        <v>63946953.45801274</v>
       </c>
       <c r="AJ41">
         <v>2560028.175415531</v>
@@ -6302,7 +6302,7 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <v>4763.247594707089</v>
+        <v>4763.247594707091</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -7316,7 +7316,7 @@
         <v>20530000</v>
       </c>
       <c r="S51">
-        <v>7694384.040326446</v>
+        <v>7694384.040326445</v>
       </c>
       <c r="T51">
         <v>0</v>
@@ -7355,7 +7355,7 @@
         <v>36129566.92913385</v>
       </c>
       <c r="AF51">
-        <v>6838639.807704589</v>
+        <v>6838639.807704587</v>
       </c>
       <c r="AG51">
         <v>0</v>
@@ -7373,7 +7373,7 @@
         <v>167134960.0077859</v>
       </c>
       <c r="AL51">
-        <v>21818999.09986462</v>
+        <v>21818999.09986461</v>
       </c>
       <c r="AM51">
         <v>0</v>
@@ -7786,7 +7786,7 @@
         <v>6140000</v>
       </c>
       <c r="S55">
-        <v>642294.3471708309</v>
+        <v>642294.3471708308</v>
       </c>
       <c r="T55">
         <v>0</v>
@@ -8262,7 +8262,7 @@
         <v>0</v>
       </c>
       <c r="U59">
-        <v>642008.4255763415</v>
+        <v>642008.4255763419</v>
       </c>
       <c r="V59">
         <v>24092</v>
@@ -8301,7 +8301,7 @@
         <v>0</v>
       </c>
       <c r="AH59">
-        <v>582788.9628365686</v>
+        <v>582788.9628365689</v>
       </c>
       <c r="AI59">
         <v>61030872.14316869</v>
@@ -8319,7 +8319,7 @@
         <v>0</v>
       </c>
       <c r="AN59">
-        <v>422097.9927458329</v>
+        <v>422097.9927458332</v>
       </c>
     </row>
     <row r="60" spans="1:40">
@@ -8497,7 +8497,7 @@
         <v>10000</v>
       </c>
       <c r="R61">
-        <v>39748.04382483129</v>
+        <v>39748.04382483127</v>
       </c>
       <c r="S61">
         <v>120000</v>
@@ -8518,7 +8518,7 @@
         <v>10000</v>
       </c>
       <c r="AE61">
-        <v>39748.04382483129</v>
+        <v>39748.04382483127</v>
       </c>
       <c r="AF61">
         <v>120000</v>
@@ -8536,7 +8536,7 @@
         <v>11365.68783657478</v>
       </c>
       <c r="AK61">
-        <v>45176.38582275261</v>
+        <v>45176.38582275259</v>
       </c>
       <c r="AL61">
         <v>136388.2540388973</v>
@@ -9398,7 +9398,7 @@
         <v>0</v>
       </c>
       <c r="Q69">
-        <v>42136.42103010117</v>
+        <v>42136.42103010118</v>
       </c>
       <c r="R69">
         <v>0</v>
@@ -9419,7 +9419,7 @@
         <v>610711.2931188598</v>
       </c>
       <c r="AD69">
-        <v>42136.42103010117</v>
+        <v>42136.42103010118</v>
       </c>
       <c r="AE69">
         <v>35361.78601097557</v>
@@ -10468,7 +10468,7 @@
         <v>0</v>
       </c>
       <c r="U79">
-        <v>12580310.37505007</v>
+        <v>12580310.37505008</v>
       </c>
       <c r="V79">
         <v>6186.999999999999</v>
@@ -10507,25 +10507,25 @@
         <v>0</v>
       </c>
       <c r="AH79">
-        <v>11419890.67987043</v>
+        <v>11419890.67987044</v>
       </c>
       <c r="AI79">
-        <v>8132020.753552009</v>
+        <v>8132020.753552016</v>
       </c>
       <c r="AJ79">
-        <v>4623026.948227281</v>
+        <v>4623026.948227284</v>
       </c>
       <c r="AK79">
-        <v>13649895.72681979</v>
+        <v>13649895.7268198</v>
       </c>
       <c r="AL79">
-        <v>2971246.346484521</v>
+        <v>2971246.346484524</v>
       </c>
       <c r="AM79">
         <v>0</v>
       </c>
       <c r="AN79">
-        <v>8271112.256293562</v>
+        <v>8271112.256293569</v>
       </c>
     </row>
     <row r="80" spans="1:40">
@@ -11176,7 +11176,7 @@
         <v>0</v>
       </c>
       <c r="S85">
-        <v>494072.574746793</v>
+        <v>494072.5747467929</v>
       </c>
       <c r="T85">
         <v>0</v>
@@ -11286,7 +11286,7 @@
         <v>0</v>
       </c>
       <c r="U86">
-        <v>834610.9532492439</v>
+        <v>834610.9532492445</v>
       </c>
       <c r="V86">
         <v>2716</v>
@@ -11313,7 +11313,7 @@
         <v>13025714.28571429</v>
       </c>
       <c r="AD86">
-        <v>18320.18305656572</v>
+        <v>18320.18305656573</v>
       </c>
       <c r="AE86">
         <v>0</v>
@@ -11325,13 +11325,13 @@
         <v>0</v>
       </c>
       <c r="AH86">
-        <v>757625.6516875392</v>
+        <v>757625.6516875396</v>
       </c>
       <c r="AI86">
         <v>17972636.26402408</v>
       </c>
       <c r="AJ86">
-        <v>111061.9048032908</v>
+        <v>111061.9048032909</v>
       </c>
       <c r="AK86">
         <v>0</v>
@@ -11343,7 +11343,7 @@
         <v>0</v>
       </c>
       <c r="AN86">
-        <v>548727.3905695828</v>
+        <v>548727.3905695832</v>
       </c>
     </row>
     <row r="87" spans="1:40">
@@ -11393,7 +11393,7 @@
         <v>18063</v>
       </c>
       <c r="P87">
-        <v>2217291.09589254</v>
+        <v>2217291.095892541</v>
       </c>
       <c r="Q87">
         <v>6969999.999999999</v>
@@ -11432,7 +11432,7 @@
         <v>0</v>
       </c>
       <c r="AC87">
-        <v>2217291.09589254</v>
+        <v>2217291.095892541</v>
       </c>
       <c r="AD87">
         <v>21465579.71014493</v>
@@ -11750,7 +11750,7 @@
         <v>1750000</v>
       </c>
       <c r="S90">
-        <v>64229.43471708309</v>
+        <v>64229.43471708308</v>
       </c>
       <c r="T90">
         <v>0</v>
@@ -11789,7 +11789,7 @@
         <v>2143130.501339457</v>
       </c>
       <c r="AF90">
-        <v>78658.32035769838</v>
+        <v>78658.32035769837</v>
       </c>
       <c r="AG90">
         <v>0</v>
@@ -11807,7 +11807,7 @@
         <v>6206935.713709597</v>
       </c>
       <c r="AL90">
-        <v>78658.32035769838</v>
+        <v>78658.32035769837</v>
       </c>
       <c r="AM90">
         <v>0</v>
@@ -12440,7 +12440,7 @@
         <v>0</v>
       </c>
       <c r="Q96">
-        <v>3297.632950181831</v>
+        <v>3297.632950181832</v>
       </c>
       <c r="R96">
         <v>0</v>
@@ -12461,13 +12461,13 @@
         <v>13559.81221752944</v>
       </c>
       <c r="AD96">
-        <v>3297.632950181831</v>
+        <v>3297.632950181832</v>
       </c>
       <c r="AE96">
-        <v>1781.792621683487</v>
+        <v>1781.792621683486</v>
       </c>
       <c r="AF96">
-        <v>285.2306821534571</v>
+        <v>285.230682153457</v>
       </c>
       <c r="AG96">
         <v>0</v>
@@ -12547,7 +12547,7 @@
         <v>0</v>
       </c>
       <c r="R97">
-        <v>8744.569641462884</v>
+        <v>8744.569641462882</v>
       </c>
       <c r="S97">
         <v>0</v>
@@ -12788,7 +12788,7 @@
         <v>40</v>
       </c>
       <c r="AC99">
-        <v>1194364.322963179</v>
+        <v>1194364.32296318</v>
       </c>
       <c r="AD99">
         <v>37558760.44764078</v>
@@ -12806,7 +12806,7 @@
         <v>77840339.11762628</v>
       </c>
       <c r="AI99">
-        <v>1194364.322963179</v>
+        <v>1194364.32296318</v>
       </c>
       <c r="AJ99">
         <v>106162091.1075757</v>
@@ -13308,7 +13308,7 @@
         <v>0</v>
       </c>
       <c r="Q104">
-        <v>8793.687867151548</v>
+        <v>8793.687867151551</v>
       </c>
       <c r="R104">
         <v>0</v>
@@ -13534,7 +13534,7 @@
         <v>480000</v>
       </c>
       <c r="Q106">
-        <v>54960.54916969718</v>
+        <v>54960.5491696972</v>
       </c>
       <c r="R106">
         <v>0</v>
@@ -14010,7 +14010,7 @@
         <v>0</v>
       </c>
       <c r="S110">
-        <v>290020.6013763675</v>
+        <v>290020.6013763674</v>
       </c>
       <c r="T110">
         <v>0</v>
@@ -14022,16 +14022,16 @@
         <v>58.73</v>
       </c>
       <c r="AC110">
-        <v>28303.7845814145</v>
+        <v>28303.78458141454</v>
       </c>
       <c r="AD110">
-        <v>29584.30053026898</v>
+        <v>29584.30053026902</v>
       </c>
       <c r="AE110">
-        <v>26714.04011989464</v>
+        <v>26714.04011989468</v>
       </c>
       <c r="AF110">
-        <v>290020.6013763675</v>
+        <v>290020.6013763674</v>
       </c>
       <c r="AG110">
         <v>0</v>
@@ -14040,16 +14040,16 @@
         <v>263250.1264619431</v>
       </c>
       <c r="AI110">
-        <v>18244.62213867973</v>
+        <v>18244.62213867975</v>
       </c>
       <c r="AJ110">
-        <v>83787.01920478707</v>
+        <v>83787.01920478714</v>
       </c>
       <c r="AK110">
-        <v>40327.38237111169</v>
+        <v>40327.38237111171</v>
       </c>
       <c r="AL110">
-        <v>304849.0140354747</v>
+        <v>304849.0140354746</v>
       </c>
       <c r="AM110">
         <v>0</v>
@@ -14242,7 +14242,7 @@
         <v>0</v>
       </c>
       <c r="U112">
-        <v>9764156.371198734</v>
+        <v>9764156.371198736</v>
       </c>
       <c r="V112">
         <v>934.9999999999999</v>
@@ -14284,22 +14284,22 @@
         <v>8863501.377628464</v>
       </c>
       <c r="AI112">
-        <v>403769.6854969042</v>
+        <v>403769.6854969044</v>
       </c>
       <c r="AJ112">
-        <v>1912171.808597188</v>
+        <v>1912171.808597189</v>
       </c>
       <c r="AK112">
         <v>11282632.24679526</v>
       </c>
       <c r="AL112">
-        <v>726286.1423423956</v>
+        <v>726286.1423423961</v>
       </c>
       <c r="AM112">
         <v>0</v>
       </c>
       <c r="AN112">
-        <v>6419589.900926216</v>
+        <v>6419589.900926217</v>
       </c>
     </row>
     <row r="113" spans="1:40">
@@ -14566,7 +14566,7 @@
         <v>22487479.50819672</v>
       </c>
       <c r="S115">
-        <v>8690133.268765895</v>
+        <v>8690133.268765893</v>
       </c>
       <c r="T115">
         <v>12310000</v>
@@ -14605,7 +14605,7 @@
         <v>49634016.39344262</v>
       </c>
       <c r="AF115">
-        <v>4916973.274954379</v>
+        <v>4916973.274954378</v>
       </c>
       <c r="AG115">
         <v>14359595.87317959</v>
@@ -14962,7 +14962,7 @@
         <v>1670276.664448191</v>
       </c>
       <c r="AI118">
-        <v>16543.47613183032</v>
+        <v>16543.47613183033</v>
       </c>
       <c r="AJ118">
         <v>2285737.059171806</v>
@@ -15033,7 +15033,7 @@
         <v>207350</v>
       </c>
       <c r="R119">
-        <v>834708.9203214571</v>
+        <v>834708.9203214567</v>
       </c>
       <c r="S119">
         <v>270000</v>
@@ -16231,7 +16231,7 @@
         <v>100000</v>
       </c>
       <c r="R130">
-        <v>39748.04382483129</v>
+        <v>39748.04382483127</v>
       </c>
       <c r="S130">
         <v>60000</v>
@@ -16270,7 +16270,7 @@
         <v>4285714.285714286</v>
       </c>
       <c r="AE130">
-        <v>3179843.505986502</v>
+        <v>3179843.505986501</v>
       </c>
       <c r="AF130">
         <v>19422000</v>
@@ -16288,7 +16288,7 @@
         <v>10590337.76543967</v>
       </c>
       <c r="AK130">
-        <v>4188296.013050891</v>
+        <v>4188296.01305089</v>
       </c>
       <c r="AL130">
         <v>17643555.97894776</v>
@@ -16704,13 +16704,13 @@
         <v>0</v>
       </c>
       <c r="S134">
-        <v>49407.2574746793</v>
+        <v>49407.25747467929</v>
       </c>
       <c r="T134">
         <v>0</v>
       </c>
       <c r="U134">
-        <v>321004.2127881707</v>
+        <v>321004.212788171</v>
       </c>
       <c r="W134">
         <v>39.43333333333333</v>
@@ -16725,13 +16725,13 @@
         <v>0</v>
       </c>
       <c r="AF134">
-        <v>49407.2574746793</v>
+        <v>49407.25747467929</v>
       </c>
       <c r="AG134">
         <v>0</v>
       </c>
       <c r="AH134">
-        <v>291394.4814182843</v>
+        <v>291394.4814182845</v>
       </c>
       <c r="AI134">
         <v>12257748.43528943</v>
@@ -16743,13 +16743,13 @@
         <v>0</v>
       </c>
       <c r="AL134">
-        <v>49728.7624093437</v>
+        <v>49728.76240934369</v>
       </c>
       <c r="AM134">
         <v>0</v>
       </c>
       <c r="AN134">
-        <v>211048.9963729165</v>
+        <v>211048.9963729166</v>
       </c>
     </row>
     <row r="135" spans="1:40">
@@ -16942,7 +16942,7 @@
         <v>40</v>
       </c>
       <c r="AC136">
-        <v>578448.4003808845</v>
+        <v>578448.4003808846</v>
       </c>
       <c r="AD136">
         <v>18190266.13866498</v>
@@ -16960,7 +16960,7 @@
         <v>37699233.62746379</v>
       </c>
       <c r="AI136">
-        <v>578448.4003808845</v>
+        <v>578448.4003808846</v>
       </c>
       <c r="AJ136">
         <v>51415879.22679437</v>
@@ -18036,7 +18036,7 @@
         <v>44000000</v>
       </c>
       <c r="Q146">
-        <v>3664.036611313145</v>
+        <v>3664.036611313147</v>
       </c>
       <c r="R146">
         <v>0</v>
@@ -18048,7 +18048,7 @@
         <v>0</v>
       </c>
       <c r="U146">
-        <v>192602.5276729024</v>
+        <v>192602.5276729026</v>
       </c>
       <c r="W146">
         <v>62.82165000000001</v>
@@ -18057,7 +18057,7 @@
         <v>44000000</v>
       </c>
       <c r="AD146">
-        <v>3664.036611313145</v>
+        <v>3664.036611313147</v>
       </c>
       <c r="AE146">
         <v>0</v>
@@ -18069,13 +18069,13 @@
         <v>0</v>
       </c>
       <c r="AH146">
-        <v>174836.6888509705</v>
+        <v>174836.6888509707</v>
       </c>
       <c r="AI146">
         <v>44047941.79802655</v>
       </c>
       <c r="AJ146">
-        <v>3668.02889547636</v>
+        <v>3668.028895476362</v>
       </c>
       <c r="AK146">
         <v>0</v>
@@ -18087,7 +18087,7 @@
         <v>0</v>
       </c>
       <c r="AN146">
-        <v>126629.3978237499</v>
+        <v>126629.39782375</v>
       </c>
     </row>
     <row r="147" spans="1:40">
@@ -18152,7 +18152,7 @@
         <v>0</v>
       </c>
       <c r="U147">
-        <v>668066.37255526</v>
+        <v>668066.3725552601</v>
       </c>
       <c r="W147">
         <v>50.10275</v>
@@ -18191,7 +18191,7 @@
         <v>0</v>
       </c>
       <c r="AN147">
-        <v>439230.1777401418</v>
+        <v>439230.1777401419</v>
       </c>
     </row>
     <row r="148" spans="1:40">
@@ -18250,7 +18250,7 @@
         <v>0</v>
       </c>
       <c r="S148">
-        <v>275730.5835345644</v>
+        <v>275730.5835345643</v>
       </c>
       <c r="T148">
         <v>0</v>
@@ -18262,7 +18262,7 @@
         <v>40</v>
       </c>
       <c r="AC148">
-        <v>814814.1445288165</v>
+        <v>814814.1445288167</v>
       </c>
       <c r="AD148">
         <v>25623177.68148089</v>
@@ -18280,7 +18280,7 @@
         <v>53103904.82077128</v>
       </c>
       <c r="AI148">
-        <v>814814.1445288165</v>
+        <v>814814.1445288167</v>
       </c>
       <c r="AJ148">
         <v>72425449.91012451</v>
@@ -18848,7 +18848,7 @@
         <v>0</v>
       </c>
       <c r="U153">
-        <v>7530214.063828213</v>
+        <v>7530214.063828212</v>
       </c>
       <c r="W153">
         <v>60</v>
@@ -18869,13 +18869,13 @@
         <v>0</v>
       </c>
       <c r="AH153">
-        <v>6835620.015821654</v>
+        <v>6835620.015821653</v>
       </c>
       <c r="AI153">
         <v>16227550.45802562</v>
       </c>
       <c r="AJ153">
-        <v>158042.2305477277</v>
+        <v>158042.2305477278</v>
       </c>
       <c r="AK153">
         <v>0</v>
@@ -18887,7 +18887,7 @@
         <v>0</v>
       </c>
       <c r="AN153">
-        <v>4950851.28896081</v>
+        <v>4950851.288960809</v>
       </c>
     </row>
     <row r="154" spans="1:40">
@@ -19172,7 +19172,7 @@
         <v>0</v>
       </c>
       <c r="S156">
-        <v>158103.2239189738</v>
+        <v>158103.2239189737</v>
       </c>
       <c r="T156">
         <v>0</v>
@@ -19193,7 +19193,7 @@
         <v>0</v>
       </c>
       <c r="AF156">
-        <v>158103.2239189738</v>
+        <v>158103.2239189737</v>
       </c>
       <c r="AG156">
         <v>0</v>
@@ -20186,7 +20186,7 @@
         <v>0</v>
       </c>
       <c r="U165">
-        <v>64200.84255763415</v>
+        <v>64200.84255763418</v>
       </c>
       <c r="W165">
         <v>62.02077895833333</v>
@@ -20207,7 +20207,7 @@
         <v>0</v>
       </c>
       <c r="AH165">
-        <v>58278.89628365686</v>
+        <v>58278.89628365689</v>
       </c>
       <c r="AI165">
         <v>308761.7759046202</v>
@@ -20219,13 +20219,13 @@
         <v>0</v>
       </c>
       <c r="AL165">
-        <v>216133.2431332341</v>
+        <v>216133.2431332342</v>
       </c>
       <c r="AM165">
         <v>0</v>
       </c>
       <c r="AN165">
-        <v>42209.7992745833</v>
+        <v>42209.79927458332</v>
       </c>
     </row>
     <row r="166" spans="1:40">
@@ -20498,40 +20498,40 @@
         <v>0</v>
       </c>
       <c r="U168">
-        <v>744846.52797455</v>
+        <v>744846.5279745499</v>
       </c>
       <c r="W168">
         <v>60</v>
       </c>
       <c r="AC168">
-        <v>892788.3993013304</v>
+        <v>892788.3993013303</v>
       </c>
       <c r="AD168">
-        <v>60626.63917271329</v>
+        <v>60626.63917271328</v>
       </c>
       <c r="AE168">
-        <v>51694.79045973796</v>
+        <v>51694.79045973795</v>
       </c>
       <c r="AF168">
-        <v>9101.943569871159</v>
+        <v>9101.943569871157</v>
       </c>
       <c r="AG168">
         <v>0</v>
       </c>
       <c r="AH168">
-        <v>676141.1816691019</v>
+        <v>676141.1816691018</v>
       </c>
       <c r="AI168">
-        <v>980934.0363932481</v>
+        <v>980934.0363932482</v>
       </c>
       <c r="AJ168">
         <v>145532.5538148287</v>
       </c>
       <c r="AK168">
-        <v>66143.69622541801</v>
+        <v>66143.69622541797</v>
       </c>
       <c r="AL168">
-        <v>8032.234298265624</v>
+        <v>8032.234298265622</v>
       </c>
       <c r="AM168">
         <v>0</v>
@@ -21131,7 +21131,7 @@
         <v>10000</v>
       </c>
       <c r="R174">
-        <v>5564.72613547638</v>
+        <v>5564.726135476378</v>
       </c>
       <c r="S174">
         <v>0</v>
@@ -21146,16 +21146,16 @@
         <v>33.725</v>
       </c>
       <c r="AC174">
-        <v>8757.498586650619</v>
+        <v>8757.498586650621</v>
       </c>
       <c r="AD174">
         <v>10000</v>
       </c>
       <c r="AE174">
-        <v>5564.72613547638</v>
+        <v>5564.726135476378</v>
       </c>
       <c r="AF174">
-        <v>3393.361115136333</v>
+        <v>3393.361115136334</v>
       </c>
       <c r="AG174">
         <v>0</v>
@@ -21170,7 +21170,7 @@
         <v>45188.12582118752</v>
       </c>
       <c r="AK174">
-        <v>5564.72613547638</v>
+        <v>5564.726135476378</v>
       </c>
       <c r="AL174">
         <v>14347.71222798183</v>
@@ -21363,7 +21363,7 @@
         <v>5984311.873583687</v>
       </c>
       <c r="AF176">
-        <v>96053.31544351934</v>
+        <v>96053.31544351931</v>
       </c>
       <c r="AG176">
         <v>0</v>
@@ -21381,7 +21381,7 @@
         <v>6728463.073520347</v>
       </c>
       <c r="AL176">
-        <v>96053.31544351934</v>
+        <v>96053.31544351931</v>
       </c>
       <c r="AM176">
         <v>0</v>
@@ -22243,7 +22243,7 @@
         <v>1409361.70212766</v>
       </c>
       <c r="R184">
-        <v>3974804.382483129</v>
+        <v>3974804.382483128</v>
       </c>
       <c r="S184">
         <v>0</v>
@@ -22282,7 +22282,7 @@
         <v>4787234.042553192</v>
       </c>
       <c r="AE184">
-        <v>11924413.14744939</v>
+        <v>11924413.14744938</v>
       </c>
       <c r="AF184">
         <v>0</v>
@@ -22300,7 +22300,7 @@
         <v>38862218.90627506</v>
       </c>
       <c r="AK184">
-        <v>51597061.97087712</v>
+        <v>51597061.9708771</v>
       </c>
       <c r="AL184">
         <v>0</v>
@@ -22591,7 +22591,7 @@
         <v>10000</v>
       </c>
       <c r="R187">
-        <v>13514.33490044264</v>
+        <v>13514.33490044263</v>
       </c>
       <c r="S187">
         <v>0</v>
@@ -22606,16 +22606,16 @@
         <v>41</v>
       </c>
       <c r="AC187">
-        <v>14039.2856360056</v>
+        <v>14039.28563600561</v>
       </c>
       <c r="AD187">
         <v>10000</v>
       </c>
       <c r="AE187">
-        <v>13514.33490044264</v>
+        <v>13514.33490044263</v>
       </c>
       <c r="AF187">
-        <v>295.3164066481965</v>
+        <v>295.3164066481967</v>
       </c>
       <c r="AG187">
         <v>0</v>

</xml_diff>

<commit_message>
Filtered facilities out of eez (p1_a)
</commit_message>
<xml_diff>
--- a/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
+++ b/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
@@ -1970,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>224948.8426581833</v>
+        <v>224948.8426581832</v>
       </c>
       <c r="W3">
         <v>60.36830343223809</v>
@@ -1991,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>204199.3492318431</v>
+        <v>204199.349231843</v>
       </c>
       <c r="AI3">
         <v>799010.6069763988</v>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="AN3">
-        <v>147895.9639373561</v>
+        <v>147895.963937356</v>
       </c>
     </row>
     <row r="4" spans="1:40">
@@ -2342,7 +2342,7 @@
         <v>109847923.4591715</v>
       </c>
       <c r="AI6">
-        <v>2190022.675978827</v>
+        <v>2190022.675978826</v>
       </c>
       <c r="AJ6">
         <v>302585499.6266484</v>
@@ -2636,7 +2636,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>18320.18305656573</v>
+        <v>18320.18305656572</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -3192,7 +3192,7 @@
         <v>260000</v>
       </c>
       <c r="Q14">
-        <v>25648.25627919203</v>
+        <v>25648.25627919201</v>
       </c>
       <c r="R14">
         <v>0</v>
@@ -3213,7 +3213,7 @@
         <v>260000</v>
       </c>
       <c r="AD14">
-        <v>25648.25627919203</v>
+        <v>25648.25627919201</v>
       </c>
       <c r="AE14">
         <v>0</v>
@@ -3231,7 +3231,7 @@
         <v>286424.342787744</v>
       </c>
       <c r="AJ14">
-        <v>28254.94210930463</v>
+        <v>28254.94210930461</v>
       </c>
       <c r="AK14">
         <v>0</v>
@@ -3549,7 +3549,7 @@
         <v>99246.68717788679</v>
       </c>
       <c r="AF17">
-        <v>17474.44448765757</v>
+        <v>17474.44448765756</v>
       </c>
       <c r="AG17">
         <v>0</v>
@@ -3668,7 +3668,7 @@
         <v>5011764.705882354</v>
       </c>
       <c r="AE18">
-        <v>4372284.82073144</v>
+        <v>4372284.820731441</v>
       </c>
       <c r="AF18">
         <v>0</v>
@@ -3686,7 +3686,7 @@
         <v>106593626.8717267</v>
       </c>
       <c r="AK18">
-        <v>49567159.93408028</v>
+        <v>49567159.9340803</v>
       </c>
       <c r="AL18">
         <v>0</v>
@@ -3888,7 +3888,7 @@
         <v>40</v>
       </c>
       <c r="AC20">
-        <v>542384.9822387615</v>
+        <v>542384.9822387614</v>
       </c>
       <c r="AD20">
         <v>17056192.34151518</v>
@@ -3906,7 +3906,7 @@
         <v>35348871.47753028</v>
       </c>
       <c r="AI20">
-        <v>542384.9822387615</v>
+        <v>542384.9822387614</v>
       </c>
       <c r="AJ20">
         <v>48210351.55919283</v>
@@ -3986,19 +3986,19 @@
         <v>0</v>
       </c>
       <c r="U21">
-        <v>2436083.738639096</v>
+        <v>2436083.738639095</v>
       </c>
       <c r="W21">
         <v>89.49593836999999</v>
       </c>
       <c r="AC21">
-        <v>7948580.752319796</v>
+        <v>7948580.752319794</v>
       </c>
       <c r="AD21">
-        <v>3742593.197986537</v>
+        <v>3742593.197986536</v>
       </c>
       <c r="AE21">
-        <v>5262562.920187896</v>
+        <v>5262562.920187895</v>
       </c>
       <c r="AF21">
         <v>1887476.514225975</v>
@@ -4007,16 +4007,16 @@
         <v>0</v>
       </c>
       <c r="AH21">
-        <v>2211377.076788363</v>
+        <v>2211377.076788362</v>
       </c>
       <c r="AI21">
-        <v>8205811.973943212</v>
+        <v>8205811.97394321</v>
       </c>
       <c r="AJ21">
-        <v>3863710.646541941</v>
+        <v>3863710.64654194</v>
       </c>
       <c r="AK21">
-        <v>5432869.48572602</v>
+        <v>5432869.485726019</v>
       </c>
       <c r="AL21">
         <v>1948558.851396438</v>
@@ -4025,7 +4025,7 @@
         <v>0</v>
       </c>
       <c r="AN21">
-        <v>1601639.503900958</v>
+        <v>1601639.503900957</v>
       </c>
     </row>
     <row r="22" spans="1:40">
@@ -4408,7 +4408,7 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>10992.10983393944</v>
+        <v>10992.10983393943</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -4741,7 +4741,7 @@
         <v>90000</v>
       </c>
       <c r="R28">
-        <v>3974.804382483127</v>
+        <v>3974.804382483129</v>
       </c>
       <c r="S28">
         <v>0</v>
@@ -4842,7 +4842,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>18320.18305656573</v>
+        <v>18320.18305656572</v>
       </c>
       <c r="R29">
         <v>0</v>
@@ -5172,7 +5172,7 @@
         <v>140000</v>
       </c>
       <c r="Q32">
-        <v>73280.73222626293</v>
+        <v>73280.73222626289</v>
       </c>
       <c r="R32">
         <v>0</v>
@@ -5193,7 +5193,7 @@
         <v>504305.67978832</v>
       </c>
       <c r="AD32">
-        <v>73280.73222626293</v>
+        <v>73280.73222626289</v>
       </c>
       <c r="AE32">
         <v>29200.62185475808</v>
@@ -5208,16 +5208,16 @@
         <v>407952.2739855982</v>
       </c>
       <c r="AI32">
-        <v>554096.1401805037</v>
+        <v>554096.1401805036</v>
       </c>
       <c r="AJ32">
         <v>112815.4664275035</v>
       </c>
       <c r="AK32">
-        <v>51273.97097974453</v>
+        <v>51273.97097974452</v>
       </c>
       <c r="AL32">
-        <v>6226.512454160595</v>
+        <v>6226.512454160593</v>
       </c>
       <c r="AM32">
         <v>0</v>
@@ -5871,7 +5871,7 @@
         <v>20366.66666666666</v>
       </c>
       <c r="R38">
-        <v>397480.4382483127</v>
+        <v>397480.4382483129</v>
       </c>
       <c r="S38">
         <v>0</v>
@@ -5892,7 +5892,7 @@
         <v>20366.66666666666</v>
       </c>
       <c r="AE38">
-        <v>397480.4382483127</v>
+        <v>397480.4382483129</v>
       </c>
       <c r="AF38">
         <v>0</v>
@@ -5910,7 +5910,7 @@
         <v>22008.2823170145</v>
       </c>
       <c r="AK38">
-        <v>429518.5777639698</v>
+        <v>429518.57776397</v>
       </c>
       <c r="AL38">
         <v>0</v>
@@ -6076,7 +6076,7 @@
         <v>1050000</v>
       </c>
       <c r="Q40">
-        <v>3664.036611313147</v>
+        <v>3664.036611313144</v>
       </c>
       <c r="R40">
         <v>0</v>
@@ -6183,7 +6183,7 @@
         <v>8058254.676258993</v>
       </c>
       <c r="R41">
-        <v>436831.0016348957</v>
+        <v>436831.0016348959</v>
       </c>
       <c r="S41">
         <v>2270000</v>
@@ -6222,7 +6222,7 @@
         <v>2309352.517985611</v>
       </c>
       <c r="AE41">
-        <v>11924413.14744938</v>
+        <v>11924413.14744939</v>
       </c>
       <c r="AF41">
         <v>0</v>
@@ -6234,7 +6234,7 @@
         <v>28313004.98051037</v>
       </c>
       <c r="AI41">
-        <v>63946953.45801274</v>
+        <v>63946953.45801272</v>
       </c>
       <c r="AJ41">
         <v>2560028.175415531</v>
@@ -6302,7 +6302,7 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <v>4763.247594707091</v>
+        <v>4763.247594707088</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -7316,7 +7316,7 @@
         <v>20530000</v>
       </c>
       <c r="S51">
-        <v>7694384.040326445</v>
+        <v>7694384.040326446</v>
       </c>
       <c r="T51">
         <v>0</v>
@@ -7355,7 +7355,7 @@
         <v>36129566.92913385</v>
       </c>
       <c r="AF51">
-        <v>6838639.807704587</v>
+        <v>6838639.807704589</v>
       </c>
       <c r="AG51">
         <v>0</v>
@@ -7373,7 +7373,7 @@
         <v>167134960.0077859</v>
       </c>
       <c r="AL51">
-        <v>21818999.09986461</v>
+        <v>21818999.09986462</v>
       </c>
       <c r="AM51">
         <v>0</v>
@@ -7599,7 +7599,7 @@
         <v>20075795.50267576</v>
       </c>
       <c r="AL53">
-        <v>9117133.588664468</v>
+        <v>9117133.588664467</v>
       </c>
       <c r="AM53">
         <v>0</v>
@@ -7929,7 +7929,7 @@
         <v>26077.60118195906</v>
       </c>
       <c r="AF56">
-        <v>4591.504333123472</v>
+        <v>4591.504333123471</v>
       </c>
       <c r="AG56">
         <v>0</v>
@@ -8497,7 +8497,7 @@
         <v>10000</v>
       </c>
       <c r="R61">
-        <v>39748.04382483127</v>
+        <v>39748.04382483129</v>
       </c>
       <c r="S61">
         <v>120000</v>
@@ -8518,7 +8518,7 @@
         <v>10000</v>
       </c>
       <c r="AE61">
-        <v>39748.04382483127</v>
+        <v>39748.04382483129</v>
       </c>
       <c r="AF61">
         <v>120000</v>
@@ -8536,7 +8536,7 @@
         <v>11365.68783657478</v>
       </c>
       <c r="AK61">
-        <v>45176.38582275259</v>
+        <v>45176.38582275261</v>
       </c>
       <c r="AL61">
         <v>136388.2540388973</v>
@@ -9050,7 +9050,7 @@
         <v>11340000</v>
       </c>
       <c r="Q66">
-        <v>238162.3797353545</v>
+        <v>238162.3797353544</v>
       </c>
       <c r="R66">
         <v>93150</v>
@@ -9107,7 +9107,7 @@
         <v>13808143.68723957</v>
       </c>
       <c r="AJ66">
-        <v>1042325.168689836</v>
+        <v>1042325.168689835</v>
       </c>
       <c r="AK66">
         <v>3510426.35669307</v>
@@ -9398,7 +9398,7 @@
         <v>0</v>
       </c>
       <c r="Q69">
-        <v>42136.42103010118</v>
+        <v>42136.42103010116</v>
       </c>
       <c r="R69">
         <v>0</v>
@@ -9419,13 +9419,13 @@
         <v>610711.2931188598</v>
       </c>
       <c r="AD69">
-        <v>42136.42103010118</v>
+        <v>42136.42103010116</v>
       </c>
       <c r="AE69">
         <v>35361.78601097557</v>
       </c>
       <c r="AF69">
-        <v>6226.178265534079</v>
+        <v>6226.178265534078</v>
       </c>
       <c r="AG69">
         <v>0</v>
@@ -9443,7 +9443,7 @@
         <v>45482.48240117538</v>
       </c>
       <c r="AL69">
-        <v>5523.216511335428</v>
+        <v>5523.216511335427</v>
       </c>
       <c r="AM69">
         <v>0</v>
@@ -9502,7 +9502,7 @@
         <v>0</v>
       </c>
       <c r="Q70">
-        <v>18320.18305656573</v>
+        <v>18320.18305656572</v>
       </c>
       <c r="R70">
         <v>0</v>
@@ -9520,16 +9520,16 @@
         <v>60</v>
       </c>
       <c r="AC70">
-        <v>84833.91875074671</v>
+        <v>84833.91875074673</v>
       </c>
       <c r="AD70">
-        <v>18320.18305656573</v>
+        <v>18320.18305656572</v>
       </c>
       <c r="AE70">
-        <v>4912.106448885565</v>
+        <v>4912.106448885566</v>
       </c>
       <c r="AF70">
-        <v>864.8785556405031</v>
+        <v>864.8785556405029</v>
       </c>
       <c r="AG70">
         <v>0</v>
@@ -9538,16 +9538,16 @@
         <v>72620.72454122569</v>
       </c>
       <c r="AI70">
-        <v>93209.63221335487</v>
+        <v>93209.63221335488</v>
       </c>
       <c r="AJ70">
         <v>23677.09880764629</v>
       </c>
       <c r="AK70">
-        <v>10761.10320323803</v>
+        <v>10761.10320323802</v>
       </c>
       <c r="AL70">
-        <v>1306.786695766915</v>
+        <v>1306.786695766914</v>
       </c>
       <c r="AM70">
         <v>0</v>
@@ -11105,13 +11105,13 @@
         <v>19438662.98811545</v>
       </c>
       <c r="AJ84">
-        <v>437096196.5808171</v>
+        <v>437096196.5808172</v>
       </c>
       <c r="AK84">
         <v>79250187.29037516</v>
       </c>
       <c r="AL84">
-        <v>35990331.95754199</v>
+        <v>35990331.95754198</v>
       </c>
       <c r="AM84">
         <v>14325794.57373152</v>
@@ -11197,7 +11197,7 @@
         <v>10354833.87947028</v>
       </c>
       <c r="AF85">
-        <v>6818174.979413335</v>
+        <v>6818174.979413333</v>
       </c>
       <c r="AG85">
         <v>0</v>
@@ -11209,10 +11209,10 @@
         <v>2254000</v>
       </c>
       <c r="AJ85">
-        <v>170658239.1648673</v>
+        <v>170658239.1648674</v>
       </c>
       <c r="AK85">
-        <v>30942153.05980298</v>
+        <v>30942153.05980299</v>
       </c>
       <c r="AL85">
         <v>14051933.48027116</v>
@@ -11274,7 +11274,7 @@
         <v>14100000</v>
       </c>
       <c r="Q86">
-        <v>18320.18305656573</v>
+        <v>18320.18305656572</v>
       </c>
       <c r="R86">
         <v>0</v>
@@ -11313,7 +11313,7 @@
         <v>13025714.28571429</v>
       </c>
       <c r="AD86">
-        <v>18320.18305656573</v>
+        <v>18320.18305656572</v>
       </c>
       <c r="AE86">
         <v>0</v>
@@ -11331,7 +11331,7 @@
         <v>17972636.26402408</v>
       </c>
       <c r="AJ86">
-        <v>111061.9048032909</v>
+        <v>111061.9048032908</v>
       </c>
       <c r="AK86">
         <v>0</v>
@@ -11393,7 +11393,7 @@
         <v>18063</v>
       </c>
       <c r="P87">
-        <v>2217291.095892541</v>
+        <v>2217291.09589254</v>
       </c>
       <c r="Q87">
         <v>6969999.999999999</v>
@@ -11432,7 +11432,7 @@
         <v>0</v>
       </c>
       <c r="AC87">
-        <v>2217291.095892541</v>
+        <v>2217291.09589254</v>
       </c>
       <c r="AD87">
         <v>21465579.71014493</v>
@@ -12440,7 +12440,7 @@
         <v>0</v>
       </c>
       <c r="Q96">
-        <v>3297.632950181832</v>
+        <v>3297.63295018183</v>
       </c>
       <c r="R96">
         <v>0</v>
@@ -12461,13 +12461,13 @@
         <v>13559.81221752944</v>
       </c>
       <c r="AD96">
-        <v>3297.632950181832</v>
+        <v>3297.63295018183</v>
       </c>
       <c r="AE96">
-        <v>1781.792621683486</v>
+        <v>1781.792621683487</v>
       </c>
       <c r="AF96">
-        <v>285.230682153457</v>
+        <v>285.2306821534571</v>
       </c>
       <c r="AG96">
         <v>0</v>
@@ -12547,7 +12547,7 @@
         <v>0</v>
       </c>
       <c r="R97">
-        <v>8744.569641462882</v>
+        <v>8744.569641462884</v>
       </c>
       <c r="S97">
         <v>0</v>
@@ -12788,7 +12788,7 @@
         <v>40</v>
       </c>
       <c r="AC99">
-        <v>1194364.32296318</v>
+        <v>1194364.322963179</v>
       </c>
       <c r="AD99">
         <v>37558760.44764078</v>
@@ -12806,7 +12806,7 @@
         <v>77840339.11762628</v>
       </c>
       <c r="AI99">
-        <v>1194364.32296318</v>
+        <v>1194364.322963179</v>
       </c>
       <c r="AJ99">
         <v>106162091.1075757</v>
@@ -13008,7 +13008,7 @@
         <v>0</v>
       </c>
       <c r="U101">
-        <v>4691553.589176392</v>
+        <v>4691553.58917639</v>
       </c>
       <c r="W101">
         <v>50.10275</v>
@@ -13017,7 +13017,7 @@
         <v>700000</v>
       </c>
       <c r="AD101">
-        <v>2152374.959876993</v>
+        <v>2152374.959876992</v>
       </c>
       <c r="AE101">
         <v>1393965.01418051</v>
@@ -13029,16 +13029,16 @@
         <v>0</v>
       </c>
       <c r="AH101">
-        <v>4258800.260874718</v>
+        <v>4258800.260874717</v>
       </c>
       <c r="AI101">
         <v>700000</v>
       </c>
       <c r="AJ101">
-        <v>4573954.934667157</v>
+        <v>4573954.934667154</v>
       </c>
       <c r="AK101">
-        <v>1578958.984845793</v>
+        <v>1578958.984845792</v>
       </c>
       <c r="AL101">
         <v>30000</v>
@@ -13047,7 +13047,7 @@
         <v>0</v>
       </c>
       <c r="AN101">
-        <v>3084531.719460099</v>
+        <v>3084531.719460098</v>
       </c>
     </row>
     <row r="102" spans="1:40">
@@ -13127,7 +13127,7 @@
         <v>18044.85221416123</v>
       </c>
       <c r="AF102">
-        <v>3177.171725028648</v>
+        <v>3177.171725028647</v>
       </c>
       <c r="AG102">
         <v>0</v>
@@ -13145,7 +13145,7 @@
         <v>23088.46235126211</v>
       </c>
       <c r="AL102">
-        <v>2803.773447434826</v>
+        <v>2803.773447434825</v>
       </c>
       <c r="AM102">
         <v>0</v>
@@ -13249,7 +13249,7 @@
         <v>7888875.420821341</v>
       </c>
       <c r="AL103">
-        <v>3582619.232516765</v>
+        <v>3582619.232516764</v>
       </c>
       <c r="AM103">
         <v>0</v>
@@ -13308,7 +13308,7 @@
         <v>0</v>
       </c>
       <c r="Q104">
-        <v>8793.687867151551</v>
+        <v>8793.687867151546</v>
       </c>
       <c r="R104">
         <v>0</v>
@@ -13534,7 +13534,7 @@
         <v>480000</v>
       </c>
       <c r="Q106">
-        <v>54960.5491696972</v>
+        <v>54960.54916969717</v>
       </c>
       <c r="R106">
         <v>0</v>
@@ -14468,40 +14468,40 @@
         <v>0</v>
       </c>
       <c r="U114">
-        <v>946186.0533227292</v>
+        <v>946186.0533227291</v>
       </c>
       <c r="W114">
         <v>60.36830343223809</v>
       </c>
       <c r="AC114">
-        <v>806462.8688798032</v>
+        <v>806462.8688798031</v>
       </c>
       <c r="AD114">
         <v>206935.0890681745</v>
       </c>
       <c r="AE114">
-        <v>206807.2399870346</v>
+        <v>206807.2399870345</v>
       </c>
       <c r="AF114">
-        <v>88113.17259844433</v>
+        <v>88113.1725984443</v>
       </c>
       <c r="AG114">
         <v>0</v>
       </c>
       <c r="AH114">
-        <v>858908.9592887425</v>
+        <v>858908.9592887424</v>
       </c>
       <c r="AI114">
-        <v>897678.7004032622</v>
+        <v>897678.7004032618</v>
       </c>
       <c r="AJ114">
-        <v>358444.5050520056</v>
+        <v>358444.5050520057</v>
       </c>
       <c r="AK114">
-        <v>190940.7182530578</v>
+        <v>190940.7182530579</v>
       </c>
       <c r="AL114">
-        <v>98079.30571738283</v>
+        <v>98079.30571738277</v>
       </c>
       <c r="AM114">
         <v>0</v>
@@ -14566,7 +14566,7 @@
         <v>22487479.50819672</v>
       </c>
       <c r="S115">
-        <v>8690133.268765893</v>
+        <v>8690133.268765895</v>
       </c>
       <c r="T115">
         <v>12310000</v>
@@ -14605,7 +14605,7 @@
         <v>49634016.39344262</v>
       </c>
       <c r="AF115">
-        <v>4916973.274954378</v>
+        <v>4916973.274954379</v>
       </c>
       <c r="AG115">
         <v>14359595.87317959</v>
@@ -14962,7 +14962,7 @@
         <v>1670276.664448191</v>
       </c>
       <c r="AI118">
-        <v>16543.47613183033</v>
+        <v>16543.47613183032</v>
       </c>
       <c r="AJ118">
         <v>2285737.059171806</v>
@@ -15033,7 +15033,7 @@
         <v>207350</v>
       </c>
       <c r="R119">
-        <v>834708.9203214567</v>
+        <v>834708.9203214571</v>
       </c>
       <c r="S119">
         <v>270000</v>
@@ -16151,7 +16151,7 @@
         <v>54134.55664248372</v>
       </c>
       <c r="AF129">
-        <v>9531.515175085948</v>
+        <v>9531.515175085946</v>
       </c>
       <c r="AG129">
         <v>0</v>
@@ -16231,7 +16231,7 @@
         <v>100000</v>
       </c>
       <c r="R130">
-        <v>39748.04382483127</v>
+        <v>39748.04382483129</v>
       </c>
       <c r="S130">
         <v>60000</v>
@@ -16270,7 +16270,7 @@
         <v>4285714.285714286</v>
       </c>
       <c r="AE130">
-        <v>3179843.505986501</v>
+        <v>3179843.505986502</v>
       </c>
       <c r="AF130">
         <v>19422000</v>
@@ -16288,7 +16288,7 @@
         <v>10590337.76543967</v>
       </c>
       <c r="AK130">
-        <v>4188296.01305089</v>
+        <v>4188296.013050891</v>
       </c>
       <c r="AL130">
         <v>17643555.97894776</v>
@@ -16942,7 +16942,7 @@
         <v>40</v>
       </c>
       <c r="AC136">
-        <v>578448.4003808846</v>
+        <v>578448.4003808844</v>
       </c>
       <c r="AD136">
         <v>18190266.13866498</v>
@@ -16960,7 +16960,7 @@
         <v>37699233.62746379</v>
       </c>
       <c r="AI136">
-        <v>578448.4003808846</v>
+        <v>578448.4003808844</v>
       </c>
       <c r="AJ136">
         <v>51415879.22679437</v>
@@ -17480,7 +17480,7 @@
         <v>1000000</v>
       </c>
       <c r="Q141">
-        <v>1832.018305656573</v>
+        <v>1832.018305656572</v>
       </c>
       <c r="R141">
         <v>0</v>
@@ -17819,7 +17819,7 @@
         <v>0</v>
       </c>
       <c r="T144">
-        <v>36078.38559683512</v>
+        <v>36078.38559683513</v>
       </c>
       <c r="U144">
         <v>9230000</v>
@@ -17840,7 +17840,7 @@
         <v>0</v>
       </c>
       <c r="AG144">
-        <v>42085.38074145373</v>
+        <v>42085.38074145374</v>
       </c>
       <c r="AH144">
         <v>8378616.093943913</v>
@@ -17858,7 +17858,7 @@
         <v>0</v>
       </c>
       <c r="AM144">
-        <v>70319.93749824952</v>
+        <v>70319.93749824954</v>
       </c>
       <c r="AN144">
         <v>6068400.846214077</v>
@@ -18036,7 +18036,7 @@
         <v>44000000</v>
       </c>
       <c r="Q146">
-        <v>3664.036611313147</v>
+        <v>3664.036611313144</v>
       </c>
       <c r="R146">
         <v>0</v>
@@ -18057,7 +18057,7 @@
         <v>44000000</v>
       </c>
       <c r="AD146">
-        <v>3664.036611313147</v>
+        <v>3664.036611313144</v>
       </c>
       <c r="AE146">
         <v>0</v>
@@ -18075,7 +18075,7 @@
         <v>44047941.79802655</v>
       </c>
       <c r="AJ146">
-        <v>3668.028895476362</v>
+        <v>3668.028895476359</v>
       </c>
       <c r="AK146">
         <v>0</v>
@@ -18152,7 +18152,7 @@
         <v>0</v>
       </c>
       <c r="U147">
-        <v>668066.3725552601</v>
+        <v>668066.37255526</v>
       </c>
       <c r="W147">
         <v>50.10275</v>
@@ -18191,7 +18191,7 @@
         <v>0</v>
       </c>
       <c r="AN147">
-        <v>439230.1777401419</v>
+        <v>439230.1777401418</v>
       </c>
     </row>
     <row r="148" spans="1:40">
@@ -18262,7 +18262,7 @@
         <v>40</v>
       </c>
       <c r="AC148">
-        <v>814814.1445288167</v>
+        <v>814814.1445288163</v>
       </c>
       <c r="AD148">
         <v>25623177.68148089</v>
@@ -18280,7 +18280,7 @@
         <v>53103904.82077128</v>
       </c>
       <c r="AI148">
-        <v>814814.1445288167</v>
+        <v>814814.1445288163</v>
       </c>
       <c r="AJ148">
         <v>72425449.91012451</v>
@@ -18637,7 +18637,7 @@
         <v>0</v>
       </c>
       <c r="AF151">
-        <v>46626.87273695783</v>
+        <v>46626.87273695782</v>
       </c>
       <c r="AG151">
         <v>0</v>
@@ -18655,7 +18655,7 @@
         <v>0</v>
       </c>
       <c r="AL151">
-        <v>50693.96501806913</v>
+        <v>50693.96501806912</v>
       </c>
       <c r="AM151">
         <v>0</v>
@@ -18848,7 +18848,7 @@
         <v>0</v>
       </c>
       <c r="U153">
-        <v>7530214.063828212</v>
+        <v>7530214.063828211</v>
       </c>
       <c r="W153">
         <v>60</v>
@@ -18869,13 +18869,13 @@
         <v>0</v>
       </c>
       <c r="AH153">
-        <v>6835620.015821653</v>
+        <v>6835620.015821652</v>
       </c>
       <c r="AI153">
         <v>16227550.45802562</v>
       </c>
       <c r="AJ153">
-        <v>158042.2305477278</v>
+        <v>158042.2305477277</v>
       </c>
       <c r="AK153">
         <v>0</v>
@@ -19282,7 +19282,7 @@
         <v>0</v>
       </c>
       <c r="U157">
-        <v>1667014.005252742</v>
+        <v>1667014.005252741</v>
       </c>
       <c r="W157">
         <v>62.82165000000001</v>
@@ -19303,7 +19303,7 @@
         <v>0</v>
       </c>
       <c r="AH157">
-        <v>1513247.061022809</v>
+        <v>1513247.061022808</v>
       </c>
       <c r="AI157">
         <v>2817839.26845601</v>
@@ -19401,7 +19401,7 @@
         <v>23394.03976500734</v>
       </c>
       <c r="AF158">
-        <v>4119.007503826878</v>
+        <v>4119.007503826877</v>
       </c>
       <c r="AG158">
         <v>0</v>
@@ -19627,7 +19627,7 @@
         <v>34960.7312074493</v>
       </c>
       <c r="AF160">
-        <v>6155.564221881752</v>
+        <v>6155.564221881751</v>
       </c>
       <c r="AG160">
         <v>0</v>
@@ -19645,7 +19645,7 @@
         <v>67184.58094349066</v>
       </c>
       <c r="AL160">
-        <v>8158.635307131997</v>
+        <v>8158.635307131995</v>
       </c>
       <c r="AM160">
         <v>0</v>
@@ -20409,7 +20409,7 @@
         <v>1369686.60401564</v>
       </c>
       <c r="AF167">
-        <v>241161.8282478286</v>
+        <v>241161.8282478285</v>
       </c>
       <c r="AG167">
         <v>0</v>
@@ -20498,46 +20498,46 @@
         <v>0</v>
       </c>
       <c r="U168">
-        <v>744846.5279745499</v>
+        <v>744846.5279745497</v>
       </c>
       <c r="W168">
         <v>60</v>
       </c>
       <c r="AC168">
-        <v>892788.3993013303</v>
+        <v>892788.39930133</v>
       </c>
       <c r="AD168">
-        <v>60626.63917271328</v>
+        <v>60626.63917271326</v>
       </c>
       <c r="AE168">
-        <v>51694.79045973795</v>
+        <v>51694.79045973793</v>
       </c>
       <c r="AF168">
-        <v>9101.943569871157</v>
+        <v>9101.943569871151</v>
       </c>
       <c r="AG168">
         <v>0</v>
       </c>
       <c r="AH168">
-        <v>676141.1816691018</v>
+        <v>676141.1816691016</v>
       </c>
       <c r="AI168">
-        <v>980934.0363932482</v>
+        <v>980934.0363932474</v>
       </c>
       <c r="AJ168">
         <v>145532.5538148287</v>
       </c>
       <c r="AK168">
-        <v>66143.69622541797</v>
+        <v>66143.69622541798</v>
       </c>
       <c r="AL168">
-        <v>8032.234298265622</v>
+        <v>8032.234298265621</v>
       </c>
       <c r="AM168">
         <v>0</v>
       </c>
       <c r="AN168">
-        <v>489710.4334409942</v>
+        <v>489710.433440994</v>
       </c>
     </row>
     <row r="169" spans="1:40">
@@ -20635,7 +20635,7 @@
         <v>80489.78483523068</v>
       </c>
       <c r="AL169">
-        <v>9774.367737331184</v>
+        <v>9774.36773733118</v>
       </c>
       <c r="AM169">
         <v>0</v>
@@ -21131,7 +21131,7 @@
         <v>10000</v>
       </c>
       <c r="R174">
-        <v>5564.726135476378</v>
+        <v>5564.72613547638</v>
       </c>
       <c r="S174">
         <v>0</v>
@@ -21146,16 +21146,16 @@
         <v>33.725</v>
       </c>
       <c r="AC174">
-        <v>8757.498586650621</v>
+        <v>8757.498586650619</v>
       </c>
       <c r="AD174">
         <v>10000</v>
       </c>
       <c r="AE174">
-        <v>5564.726135476378</v>
+        <v>5564.72613547638</v>
       </c>
       <c r="AF174">
-        <v>3393.361115136334</v>
+        <v>3393.361115136333</v>
       </c>
       <c r="AG174">
         <v>0</v>
@@ -21170,7 +21170,7 @@
         <v>45188.12582118752</v>
       </c>
       <c r="AK174">
-        <v>5564.726135476378</v>
+        <v>5564.72613547638</v>
       </c>
       <c r="AL174">
         <v>14347.71222798183</v>
@@ -22026,19 +22026,19 @@
         <v>0</v>
       </c>
       <c r="U182">
-        <v>4397330.383764587</v>
+        <v>4397330.383764585</v>
       </c>
       <c r="W182">
         <v>89.49593836999999</v>
       </c>
       <c r="AC182">
-        <v>14172984.41348478</v>
+        <v>14172984.41348477</v>
       </c>
       <c r="AD182">
-        <v>6673356.755619111</v>
+        <v>6673356.755619106</v>
       </c>
       <c r="AE182">
-        <v>9383589.922142765</v>
+        <v>9383589.922142759</v>
       </c>
       <c r="AF182">
         <v>3780000</v>
@@ -22047,25 +22047,25 @@
         <v>0</v>
       </c>
       <c r="AH182">
-        <v>3991716.481451629</v>
+        <v>3991716.481451627</v>
       </c>
       <c r="AI182">
-        <v>14631649.20010927</v>
+        <v>14631649.20010926</v>
       </c>
       <c r="AJ182">
-        <v>6889319.298375663</v>
+        <v>6889319.298375659</v>
       </c>
       <c r="AK182">
-        <v>9687260.775355332</v>
+        <v>9687260.775355328</v>
       </c>
       <c r="AL182">
-        <v>3902328.003958786</v>
+        <v>3902328.003958787</v>
       </c>
       <c r="AM182">
         <v>0</v>
       </c>
       <c r="AN182">
-        <v>2891090.29489923</v>
+        <v>2891090.294899228</v>
       </c>
     </row>
     <row r="183" spans="1:40">
@@ -22243,7 +22243,7 @@
         <v>1409361.70212766</v>
       </c>
       <c r="R184">
-        <v>3974804.382483128</v>
+        <v>3974804.382483129</v>
       </c>
       <c r="S184">
         <v>0</v>
@@ -22282,7 +22282,7 @@
         <v>4787234.042553192</v>
       </c>
       <c r="AE184">
-        <v>11924413.14744938</v>
+        <v>11924413.14744939</v>
       </c>
       <c r="AF184">
         <v>0</v>
@@ -22300,7 +22300,7 @@
         <v>38862218.90627506</v>
       </c>
       <c r="AK184">
-        <v>51597061.9708771</v>
+        <v>51597061.97087712</v>
       </c>
       <c r="AL184">
         <v>0</v>
@@ -22591,7 +22591,7 @@
         <v>10000</v>
       </c>
       <c r="R187">
-        <v>13514.33490044263</v>
+        <v>13514.33490044264</v>
       </c>
       <c r="S187">
         <v>0</v>
@@ -22606,16 +22606,16 @@
         <v>41</v>
       </c>
       <c r="AC187">
-        <v>14039.28563600561</v>
+        <v>14039.2856360056</v>
       </c>
       <c r="AD187">
         <v>10000</v>
       </c>
       <c r="AE187">
-        <v>13514.33490044263</v>
+        <v>13514.33490044264</v>
       </c>
       <c r="AF187">
-        <v>295.3164066481967</v>
+        <v>295.3164066481965</v>
       </c>
       <c r="AG187">
         <v>0</v>
@@ -22945,7 +22945,7 @@
         <v>162955.9223460197</v>
       </c>
       <c r="AF190">
-        <v>28691.78105528772</v>
+        <v>28691.78105528771</v>
       </c>
       <c r="AG190">
         <v>0</v>
@@ -22963,7 +22963,7 @@
         <v>310560.0205936962</v>
       </c>
       <c r="AL190">
-        <v>37713.20611689933</v>
+        <v>37713.20611689932</v>
       </c>
       <c r="AM190">
         <v>0</v>

</xml_diff>

<commit_message>
Updated p1_a and minor edits
</commit_message>
<xml_diff>
--- a/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
+++ b/outputs_processed_data/p1_b_ember_2024_30_50.xlsx
@@ -1976,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>224948.8426581832</v>
+        <v>224948.8426581833</v>
       </c>
       <c r="W3">
         <v>60.36830343223809</v>
@@ -1997,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>204199.349231843</v>
+        <v>204199.3492318431</v>
       </c>
       <c r="AI3">
         <v>799010.6069763988</v>
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="AN3">
-        <v>147895.963937356</v>
+        <v>147895.9639373561</v>
       </c>
     </row>
     <row r="4" spans="1:40">
@@ -2184,7 +2184,7 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <v>642008.4255763419</v>
+        <v>642008.4255763417</v>
       </c>
       <c r="V5">
         <v>3300</v>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="AH5">
-        <v>582788.9628365689</v>
+        <v>582788.9628365688</v>
       </c>
       <c r="AI5">
         <v>9603916.688964158</v>
@@ -2241,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="AN5">
-        <v>422097.9927458332</v>
+        <v>422097.9927458331</v>
       </c>
     </row>
     <row r="6" spans="1:40">
@@ -2348,7 +2348,7 @@
         <v>109847923.4591715</v>
       </c>
       <c r="AI6">
-        <v>2190022.675978826</v>
+        <v>2190022.675978827</v>
       </c>
       <c r="AJ6">
         <v>302585499.6266484</v>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>18320.18305656572</v>
+        <v>18320.18305656573</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -3100,7 +3100,7 @@
         <v>80000</v>
       </c>
       <c r="S13">
-        <v>297584.0373009847</v>
+        <v>297584.0373009848</v>
       </c>
       <c r="T13">
         <v>0</v>
@@ -3198,13 +3198,13 @@
         <v>260000</v>
       </c>
       <c r="Q14">
-        <v>25648.25627919201</v>
+        <v>25648.25627919203</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14">
-        <v>9881.451494935858</v>
+        <v>9881.45149493586</v>
       </c>
       <c r="T14">
         <v>0</v>
@@ -3219,13 +3219,13 @@
         <v>260000</v>
       </c>
       <c r="AD14">
-        <v>25648.25627919201</v>
+        <v>25648.25627919203</v>
       </c>
       <c r="AE14">
         <v>0</v>
       </c>
       <c r="AF14">
-        <v>9881.451494935858</v>
+        <v>9881.45149493586</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -3237,7 +3237,7 @@
         <v>286424.342787744</v>
       </c>
       <c r="AJ14">
-        <v>28254.94210930461</v>
+        <v>28254.94210930463</v>
       </c>
       <c r="AK14">
         <v>0</v>
@@ -3992,19 +3992,19 @@
         <v>0</v>
       </c>
       <c r="U21">
-        <v>2436083.738639095</v>
+        <v>2436083.738639096</v>
       </c>
       <c r="W21">
         <v>89.49593836999999</v>
       </c>
       <c r="AC21">
-        <v>7948580.752319794</v>
+        <v>7948580.752319796</v>
       </c>
       <c r="AD21">
-        <v>3742593.197986536</v>
+        <v>3742593.197986537</v>
       </c>
       <c r="AE21">
-        <v>5262562.920187895</v>
+        <v>5262562.920187896</v>
       </c>
       <c r="AF21">
         <v>1887476.514225975</v>
@@ -4013,16 +4013,16 @@
         <v>0</v>
       </c>
       <c r="AH21">
-        <v>2211377.076788362</v>
+        <v>2211377.076788363</v>
       </c>
       <c r="AI21">
-        <v>8205811.97394321</v>
+        <v>8205811.973943212</v>
       </c>
       <c r="AJ21">
-        <v>3863710.64654194</v>
+        <v>3863710.646541941</v>
       </c>
       <c r="AK21">
-        <v>5432869.485726019</v>
+        <v>5432869.48572602</v>
       </c>
       <c r="AL21">
         <v>1948558.851396438</v>
@@ -4031,7 +4031,7 @@
         <v>0</v>
       </c>
       <c r="AN21">
-        <v>1601639.503900957</v>
+        <v>1601639.503900958</v>
       </c>
     </row>
     <row r="22" spans="1:40">
@@ -4414,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>10992.10983393943</v>
+        <v>10992.10983393944</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -4747,7 +4747,7 @@
         <v>90000</v>
       </c>
       <c r="R28">
-        <v>3974.804382483129</v>
+        <v>3974.804382483128</v>
       </c>
       <c r="S28">
         <v>0</v>
@@ -4848,7 +4848,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>18320.18305656572</v>
+        <v>18320.18305656573</v>
       </c>
       <c r="R29">
         <v>0</v>
@@ -4964,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="U30">
-        <v>64200.84255763418</v>
+        <v>64200.84255763417</v>
       </c>
       <c r="W30">
         <v>39.43333333333333</v>
@@ -4985,7 +4985,7 @@
         <v>0</v>
       </c>
       <c r="AH30">
-        <v>58278.89628365689</v>
+        <v>58278.89628365688</v>
       </c>
       <c r="AI30">
         <v>11176069.09700907</v>
@@ -5003,7 +5003,7 @@
         <v>0</v>
       </c>
       <c r="AN30">
-        <v>42209.79927458332</v>
+        <v>42209.79927458331</v>
       </c>
     </row>
     <row r="31" spans="1:40">
@@ -5178,7 +5178,7 @@
         <v>140000</v>
       </c>
       <c r="Q32">
-        <v>73280.73222626289</v>
+        <v>73280.73222626293</v>
       </c>
       <c r="R32">
         <v>0</v>
@@ -5190,46 +5190,46 @@
         <v>0</v>
       </c>
       <c r="U32">
-        <v>449405.8979034393</v>
+        <v>449405.8979034392</v>
       </c>
       <c r="W32">
         <v>60</v>
       </c>
       <c r="AC32">
-        <v>504305.67978832</v>
+        <v>504305.6797883199</v>
       </c>
       <c r="AD32">
-        <v>73280.73222626289</v>
+        <v>73280.73222626293</v>
       </c>
       <c r="AE32">
         <v>29200.62185475808</v>
       </c>
       <c r="AF32">
-        <v>5141.377109056217</v>
+        <v>5141.377109056216</v>
       </c>
       <c r="AG32">
         <v>0</v>
       </c>
       <c r="AH32">
-        <v>407952.2739855982</v>
+        <v>407952.2739855981</v>
       </c>
       <c r="AI32">
-        <v>554096.1401805036</v>
+        <v>554096.1401805037</v>
       </c>
       <c r="AJ32">
-        <v>112815.4664275035</v>
+        <v>112815.4664275033</v>
       </c>
       <c r="AK32">
-        <v>51273.97097974452</v>
+        <v>51273.97097974444</v>
       </c>
       <c r="AL32">
-        <v>6226.512454160593</v>
+        <v>6226.512454160583</v>
       </c>
       <c r="AM32">
         <v>0</v>
       </c>
       <c r="AN32">
-        <v>295468.5949220833</v>
+        <v>295468.5949220831</v>
       </c>
     </row>
     <row r="33" spans="1:40">
@@ -5990,7 +5990,7 @@
         <v>0</v>
       </c>
       <c r="U39">
-        <v>513606.7404610735</v>
+        <v>513606.7404610734</v>
       </c>
       <c r="W39">
         <v>60</v>
@@ -6011,7 +6011,7 @@
         <v>0</v>
       </c>
       <c r="AH39">
-        <v>466231.1702692552</v>
+        <v>466231.1702692551</v>
       </c>
       <c r="AI39">
         <v>13780731.97535679</v>
@@ -6029,7 +6029,7 @@
         <v>0</v>
       </c>
       <c r="AN39">
-        <v>337678.3941966666</v>
+        <v>337678.3941966665</v>
       </c>
     </row>
     <row r="40" spans="1:40">
@@ -6082,7 +6082,7 @@
         <v>1050000</v>
       </c>
       <c r="Q40">
-        <v>3664.036611313144</v>
+        <v>3664.036611313147</v>
       </c>
       <c r="R40">
         <v>0</v>
@@ -6308,7 +6308,7 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <v>4763.247594707088</v>
+        <v>4763.247594707091</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -7322,7 +7322,7 @@
         <v>20530000</v>
       </c>
       <c r="S51">
-        <v>7694384.040326446</v>
+        <v>7694384.040326445</v>
       </c>
       <c r="T51">
         <v>0</v>
@@ -7361,7 +7361,7 @@
         <v>36129566.92913385</v>
       </c>
       <c r="AF51">
-        <v>6838639.807704589</v>
+        <v>6838639.807704587</v>
       </c>
       <c r="AG51">
         <v>0</v>
@@ -7379,7 +7379,7 @@
         <v>167134960.0077859</v>
       </c>
       <c r="AL51">
-        <v>21818999.09986462</v>
+        <v>21818999.09986461</v>
       </c>
       <c r="AM51">
         <v>0</v>
@@ -7792,7 +7792,7 @@
         <v>6140000</v>
       </c>
       <c r="S55">
-        <v>642294.3471708308</v>
+        <v>642294.3471708309</v>
       </c>
       <c r="T55">
         <v>0</v>
@@ -8268,7 +8268,7 @@
         <v>0</v>
       </c>
       <c r="U59">
-        <v>642008.4255763419</v>
+        <v>642008.4255763417</v>
       </c>
       <c r="V59">
         <v>24092</v>
@@ -8307,7 +8307,7 @@
         <v>0</v>
       </c>
       <c r="AH59">
-        <v>582788.9628365689</v>
+        <v>582788.9628365688</v>
       </c>
       <c r="AI59">
         <v>61030872.14316869</v>
@@ -8325,7 +8325,7 @@
         <v>0</v>
       </c>
       <c r="AN59">
-        <v>422097.9927458332</v>
+        <v>422097.9927458331</v>
       </c>
     </row>
     <row r="60" spans="1:40">
@@ -9056,7 +9056,7 @@
         <v>11340000</v>
       </c>
       <c r="Q66">
-        <v>238162.3797353544</v>
+        <v>238162.3797353545</v>
       </c>
       <c r="R66">
         <v>93150</v>
@@ -9113,7 +9113,7 @@
         <v>13808143.68723957</v>
       </c>
       <c r="AJ66">
-        <v>1042325.168689835</v>
+        <v>1042325.168689836</v>
       </c>
       <c r="AK66">
         <v>3510426.35669307</v>
@@ -9404,7 +9404,7 @@
         <v>0</v>
       </c>
       <c r="Q69">
-        <v>42136.42103010116</v>
+        <v>42136.42103010118</v>
       </c>
       <c r="R69">
         <v>0</v>
@@ -9425,7 +9425,7 @@
         <v>610711.2931188598</v>
       </c>
       <c r="AD69">
-        <v>42136.42103010116</v>
+        <v>42136.42103010118</v>
       </c>
       <c r="AE69">
         <v>35361.78601097557</v>
@@ -9508,7 +9508,7 @@
         <v>0</v>
       </c>
       <c r="Q70">
-        <v>18320.18305656572</v>
+        <v>18320.18305656573</v>
       </c>
       <c r="R70">
         <v>0</v>
@@ -9526,16 +9526,16 @@
         <v>60</v>
       </c>
       <c r="AC70">
-        <v>84833.91875074673</v>
+        <v>84833.91875074671</v>
       </c>
       <c r="AD70">
-        <v>18320.18305656572</v>
+        <v>18320.18305656573</v>
       </c>
       <c r="AE70">
-        <v>4912.106448885566</v>
+        <v>4912.106448885565</v>
       </c>
       <c r="AF70">
-        <v>864.8785556405029</v>
+        <v>864.8785556405028</v>
       </c>
       <c r="AG70">
         <v>0</v>
@@ -9544,16 +9544,16 @@
         <v>72620.72454122569</v>
       </c>
       <c r="AI70">
-        <v>93209.63221335488</v>
+        <v>93209.63221335487</v>
       </c>
       <c r="AJ70">
         <v>23677.09880764629</v>
       </c>
       <c r="AK70">
-        <v>10761.10320323802</v>
+        <v>10761.10320323803</v>
       </c>
       <c r="AL70">
-        <v>1306.786695766914</v>
+        <v>1306.786695766915</v>
       </c>
       <c r="AM70">
         <v>0</v>
@@ -11182,7 +11182,7 @@
         <v>0</v>
       </c>
       <c r="S85">
-        <v>494072.5747467929</v>
+        <v>494072.574746793</v>
       </c>
       <c r="T85">
         <v>0</v>
@@ -11280,7 +11280,7 @@
         <v>14100000</v>
       </c>
       <c r="Q86">
-        <v>18320.18305656572</v>
+        <v>18320.18305656573</v>
       </c>
       <c r="R86">
         <v>0</v>
@@ -11292,7 +11292,7 @@
         <v>0</v>
       </c>
       <c r="U86">
-        <v>834610.9532492445</v>
+        <v>834610.9532492443</v>
       </c>
       <c r="V86">
         <v>2716</v>
@@ -11319,7 +11319,7 @@
         <v>13025714.28571429</v>
       </c>
       <c r="AD86">
-        <v>18320.18305656572</v>
+        <v>18320.18305656573</v>
       </c>
       <c r="AE86">
         <v>0</v>
@@ -11331,13 +11331,13 @@
         <v>0</v>
       </c>
       <c r="AH86">
-        <v>757625.6516875396</v>
+        <v>757625.6516875394</v>
       </c>
       <c r="AI86">
         <v>17972636.26402408</v>
       </c>
       <c r="AJ86">
-        <v>111061.9048032908</v>
+        <v>111061.9048032909</v>
       </c>
       <c r="AK86">
         <v>0</v>
@@ -11349,7 +11349,7 @@
         <v>0</v>
       </c>
       <c r="AN86">
-        <v>548727.3905695832</v>
+        <v>548727.390569583</v>
       </c>
     </row>
     <row r="87" spans="1:40">
@@ -11756,7 +11756,7 @@
         <v>1750000</v>
       </c>
       <c r="S90">
-        <v>64229.43471708308</v>
+        <v>64229.43471708309</v>
       </c>
       <c r="T90">
         <v>0</v>
@@ -11795,7 +11795,7 @@
         <v>2143130.501339457</v>
       </c>
       <c r="AF90">
-        <v>78658.32035769837</v>
+        <v>78658.32035769838</v>
       </c>
       <c r="AG90">
         <v>0</v>
@@ -11813,7 +11813,7 @@
         <v>6206935.713709597</v>
       </c>
       <c r="AL90">
-        <v>78658.32035769837</v>
+        <v>78658.32035769838</v>
       </c>
       <c r="AM90">
         <v>0</v>
@@ -12446,7 +12446,7 @@
         <v>0</v>
       </c>
       <c r="Q96">
-        <v>3297.63295018183</v>
+        <v>3297.632950181832</v>
       </c>
       <c r="R96">
         <v>0</v>
@@ -12467,13 +12467,13 @@
         <v>13559.81221752944</v>
       </c>
       <c r="AD96">
-        <v>3297.63295018183</v>
+        <v>3297.632950181832</v>
       </c>
       <c r="AE96">
-        <v>1781.792621683487</v>
+        <v>1781.792621683486</v>
       </c>
       <c r="AF96">
-        <v>285.2306821534571</v>
+        <v>285.230682153457</v>
       </c>
       <c r="AG96">
         <v>0</v>
@@ -13014,7 +13014,7 @@
         <v>0</v>
       </c>
       <c r="U101">
-        <v>4691553.58917639</v>
+        <v>4691553.589176392</v>
       </c>
       <c r="W101">
         <v>50.10275</v>
@@ -13023,7 +13023,7 @@
         <v>700000</v>
       </c>
       <c r="AD101">
-        <v>2152374.959876992</v>
+        <v>2152374.959876993</v>
       </c>
       <c r="AE101">
         <v>1393965.01418051</v>
@@ -13035,16 +13035,16 @@
         <v>0</v>
       </c>
       <c r="AH101">
-        <v>4258800.260874717</v>
+        <v>4258800.260874718</v>
       </c>
       <c r="AI101">
         <v>700000</v>
       </c>
       <c r="AJ101">
-        <v>4573954.934667154</v>
+        <v>4573954.934667157</v>
       </c>
       <c r="AK101">
-        <v>1578958.984845792</v>
+        <v>1578958.984845793</v>
       </c>
       <c r="AL101">
         <v>30000</v>
@@ -13053,7 +13053,7 @@
         <v>0</v>
       </c>
       <c r="AN101">
-        <v>3084531.719460098</v>
+        <v>3084531.719460099</v>
       </c>
     </row>
     <row r="102" spans="1:40">
@@ -13314,7 +13314,7 @@
         <v>0</v>
       </c>
       <c r="Q104">
-        <v>8793.687867151546</v>
+        <v>8793.687867151551</v>
       </c>
       <c r="R104">
         <v>0</v>
@@ -13540,7 +13540,7 @@
         <v>480000</v>
       </c>
       <c r="Q106">
-        <v>54960.54916969717</v>
+        <v>54960.5491696972</v>
       </c>
       <c r="R106">
         <v>0</v>
@@ -14016,7 +14016,7 @@
         <v>0</v>
       </c>
       <c r="S110">
-        <v>290020.6013763674</v>
+        <v>290020.6013763675</v>
       </c>
       <c r="T110">
         <v>0</v>
@@ -14028,16 +14028,16 @@
         <v>58.73</v>
       </c>
       <c r="AC110">
-        <v>28303.78458141454</v>
+        <v>28303.7845814145</v>
       </c>
       <c r="AD110">
-        <v>29584.30053026902</v>
+        <v>29584.30053026898</v>
       </c>
       <c r="AE110">
-        <v>26714.04011989468</v>
+        <v>26714.04011989464</v>
       </c>
       <c r="AF110">
-        <v>290020.6013763674</v>
+        <v>290020.6013763675</v>
       </c>
       <c r="AG110">
         <v>0</v>
@@ -14046,16 +14046,16 @@
         <v>263250.1264619431</v>
       </c>
       <c r="AI110">
-        <v>18244.62213867975</v>
+        <v>18244.62213867973</v>
       </c>
       <c r="AJ110">
-        <v>83787.01920478714</v>
+        <v>83787.01920478707</v>
       </c>
       <c r="AK110">
-        <v>40327.38237111171</v>
+        <v>40327.38237111169</v>
       </c>
       <c r="AL110">
-        <v>304849.0140354746</v>
+        <v>304849.0140354747</v>
       </c>
       <c r="AM110">
         <v>0</v>
@@ -14248,7 +14248,7 @@
         <v>0</v>
       </c>
       <c r="U112">
-        <v>9764156.371198736</v>
+        <v>9764156.371198732</v>
       </c>
       <c r="V112">
         <v>934.9999999999999</v>
@@ -14287,25 +14287,25 @@
         <v>0</v>
       </c>
       <c r="AH112">
-        <v>8863501.377628464</v>
+        <v>8863501.377628462</v>
       </c>
       <c r="AI112">
-        <v>403769.6854969044</v>
+        <v>403769.6854969041</v>
       </c>
       <c r="AJ112">
-        <v>1912171.808597189</v>
+        <v>1912171.808597188</v>
       </c>
       <c r="AK112">
-        <v>11282632.24679526</v>
+        <v>11282632.24679525</v>
       </c>
       <c r="AL112">
-        <v>726286.1423423961</v>
+        <v>726286.1423423955</v>
       </c>
       <c r="AM112">
         <v>0</v>
       </c>
       <c r="AN112">
-        <v>6419589.900926217</v>
+        <v>6419589.900926215</v>
       </c>
     </row>
     <row r="113" spans="1:40">
@@ -14474,40 +14474,40 @@
         <v>0</v>
       </c>
       <c r="U114">
-        <v>946186.0533227291</v>
+        <v>946186.0533227292</v>
       </c>
       <c r="W114">
         <v>60.36830343223809</v>
       </c>
       <c r="AC114">
-        <v>806462.8688798031</v>
+        <v>806462.8688798032</v>
       </c>
       <c r="AD114">
         <v>206935.0890681745</v>
       </c>
       <c r="AE114">
-        <v>206807.2399870345</v>
+        <v>206807.2399870346</v>
       </c>
       <c r="AF114">
-        <v>88113.1725984443</v>
+        <v>88113.17259844433</v>
       </c>
       <c r="AG114">
         <v>0</v>
       </c>
       <c r="AH114">
-        <v>858908.9592887424</v>
+        <v>858908.9592887425</v>
       </c>
       <c r="AI114">
-        <v>897678.7004032618</v>
+        <v>897678.7004032622</v>
       </c>
       <c r="AJ114">
-        <v>358444.5050520057</v>
+        <v>358444.5050520056</v>
       </c>
       <c r="AK114">
-        <v>190940.7182530579</v>
+        <v>190940.7182530578</v>
       </c>
       <c r="AL114">
-        <v>98079.30571738277</v>
+        <v>98079.30571738283</v>
       </c>
       <c r="AM114">
         <v>0</v>
@@ -14572,7 +14572,7 @@
         <v>22487479.50819672</v>
       </c>
       <c r="S115">
-        <v>8690133.268765895</v>
+        <v>8690133.268765893</v>
       </c>
       <c r="T115">
         <v>12310000</v>
@@ -14611,7 +14611,7 @@
         <v>49634016.39344262</v>
       </c>
       <c r="AF115">
-        <v>4916973.274954379</v>
+        <v>4916973.274954378</v>
       </c>
       <c r="AG115">
         <v>14359595.87317959</v>
@@ -15039,7 +15039,7 @@
         <v>207350</v>
       </c>
       <c r="R119">
-        <v>834708.9203214571</v>
+        <v>834708.920321457</v>
       </c>
       <c r="S119">
         <v>270000</v>
@@ -16710,13 +16710,13 @@
         <v>0</v>
       </c>
       <c r="S134">
-        <v>49407.25747467929</v>
+        <v>49407.2574746793</v>
       </c>
       <c r="T134">
         <v>0</v>
       </c>
       <c r="U134">
-        <v>321004.212788171</v>
+        <v>321004.2127881708</v>
       </c>
       <c r="W134">
         <v>39.43333333333333</v>
@@ -16731,13 +16731,13 @@
         <v>0</v>
       </c>
       <c r="AF134">
-        <v>49407.25747467929</v>
+        <v>49407.2574746793</v>
       </c>
       <c r="AG134">
         <v>0</v>
       </c>
       <c r="AH134">
-        <v>291394.4814182845</v>
+        <v>291394.4814182844</v>
       </c>
       <c r="AI134">
         <v>12257748.43528943</v>
@@ -16749,13 +16749,13 @@
         <v>0</v>
       </c>
       <c r="AL134">
-        <v>49728.76240934369</v>
+        <v>49728.7624093437</v>
       </c>
       <c r="AM134">
         <v>0</v>
       </c>
       <c r="AN134">
-        <v>211048.9963729166</v>
+        <v>211048.9963729165</v>
       </c>
     </row>
     <row r="135" spans="1:40">
@@ -16948,7 +16948,7 @@
         <v>40</v>
       </c>
       <c r="AC136">
-        <v>578448.4003808844</v>
+        <v>578448.4003808845</v>
       </c>
       <c r="AD136">
         <v>18190266.13866498</v>
@@ -16966,7 +16966,7 @@
         <v>37699233.62746379</v>
       </c>
       <c r="AI136">
-        <v>578448.4003808844</v>
+        <v>578448.4003808845</v>
       </c>
       <c r="AJ136">
         <v>51415879.22679437</v>
@@ -17486,7 +17486,7 @@
         <v>1000000</v>
       </c>
       <c r="Q141">
-        <v>1832.018305656572</v>
+        <v>1832.018305656573</v>
       </c>
       <c r="R141">
         <v>0</v>
@@ -17825,7 +17825,7 @@
         <v>0</v>
       </c>
       <c r="T144">
-        <v>36078.38559683513</v>
+        <v>36078.38559683511</v>
       </c>
       <c r="U144">
         <v>9230000</v>
@@ -17846,7 +17846,7 @@
         <v>0</v>
       </c>
       <c r="AG144">
-        <v>42085.38074145374</v>
+        <v>42085.38074145372</v>
       </c>
       <c r="AH144">
         <v>8378616.093943913</v>
@@ -17864,7 +17864,7 @@
         <v>0</v>
       </c>
       <c r="AM144">
-        <v>70319.93749824954</v>
+        <v>70319.93749824951</v>
       </c>
       <c r="AN144">
         <v>6068400.846214077</v>
@@ -18042,7 +18042,7 @@
         <v>44000000</v>
       </c>
       <c r="Q146">
-        <v>3664.036611313144</v>
+        <v>3664.036611313147</v>
       </c>
       <c r="R146">
         <v>0</v>
@@ -18054,7 +18054,7 @@
         <v>0</v>
       </c>
       <c r="U146">
-        <v>192602.5276729026</v>
+        <v>192602.5276729025</v>
       </c>
       <c r="W146">
         <v>62.82165000000001</v>
@@ -18063,7 +18063,7 @@
         <v>44000000</v>
       </c>
       <c r="AD146">
-        <v>3664.036611313144</v>
+        <v>3664.036611313147</v>
       </c>
       <c r="AE146">
         <v>0</v>
@@ -18075,13 +18075,13 @@
         <v>0</v>
       </c>
       <c r="AH146">
-        <v>174836.6888509707</v>
+        <v>174836.6888509706</v>
       </c>
       <c r="AI146">
         <v>44047941.79802655</v>
       </c>
       <c r="AJ146">
-        <v>3668.028895476359</v>
+        <v>3668.028895476362</v>
       </c>
       <c r="AK146">
         <v>0</v>
@@ -18093,7 +18093,7 @@
         <v>0</v>
       </c>
       <c r="AN146">
-        <v>126629.39782375</v>
+        <v>126629.3978237499</v>
       </c>
     </row>
     <row r="147" spans="1:40">
@@ -18158,7 +18158,7 @@
         <v>0</v>
       </c>
       <c r="U147">
-        <v>668066.37255526</v>
+        <v>668066.3725552601</v>
       </c>
       <c r="W147">
         <v>50.10275</v>
@@ -18197,7 +18197,7 @@
         <v>0</v>
       </c>
       <c r="AN147">
-        <v>439230.1777401418</v>
+        <v>439230.1777401419</v>
       </c>
     </row>
     <row r="148" spans="1:40">
@@ -18256,7 +18256,7 @@
         <v>0</v>
       </c>
       <c r="S148">
-        <v>275730.5835345643</v>
+        <v>275730.5835345644</v>
       </c>
       <c r="T148">
         <v>0</v>
@@ -18268,7 +18268,7 @@
         <v>40</v>
       </c>
       <c r="AC148">
-        <v>814814.1445288163</v>
+        <v>814814.1445288165</v>
       </c>
       <c r="AD148">
         <v>25623177.68148089</v>
@@ -18286,7 +18286,7 @@
         <v>53103904.82077128</v>
       </c>
       <c r="AI148">
-        <v>814814.1445288163</v>
+        <v>814814.1445288165</v>
       </c>
       <c r="AJ148">
         <v>72425449.91012451</v>
@@ -18854,7 +18854,7 @@
         <v>0</v>
       </c>
       <c r="U153">
-        <v>7530214.063828211</v>
+        <v>7530214.063828212</v>
       </c>
       <c r="W153">
         <v>60</v>
@@ -18875,13 +18875,13 @@
         <v>0</v>
       </c>
       <c r="AH153">
-        <v>6835620.015821652</v>
+        <v>6835620.015821653</v>
       </c>
       <c r="AI153">
         <v>16227550.45802562</v>
       </c>
       <c r="AJ153">
-        <v>158042.2305477277</v>
+        <v>158042.2305477278</v>
       </c>
       <c r="AK153">
         <v>0</v>
@@ -19178,7 +19178,7 @@
         <v>0</v>
       </c>
       <c r="S156">
-        <v>158103.2239189737</v>
+        <v>158103.2239189738</v>
       </c>
       <c r="T156">
         <v>0</v>
@@ -19199,7 +19199,7 @@
         <v>0</v>
       </c>
       <c r="AF156">
-        <v>158103.2239189737</v>
+        <v>158103.2239189738</v>
       </c>
       <c r="AG156">
         <v>0</v>
@@ -19288,7 +19288,7 @@
         <v>0</v>
       </c>
       <c r="U157">
-        <v>1667014.005252741</v>
+        <v>1667014.005252742</v>
       </c>
       <c r="W157">
         <v>62.82165000000001</v>
@@ -19309,7 +19309,7 @@
         <v>0</v>
       </c>
       <c r="AH157">
-        <v>1513247.061022808</v>
+        <v>1513247.061022809</v>
       </c>
       <c r="AI157">
         <v>2817839.26845601</v>
@@ -20192,7 +20192,7 @@
         <v>0</v>
       </c>
       <c r="U165">
-        <v>64200.84255763418</v>
+        <v>64200.84255763417</v>
       </c>
       <c r="W165">
         <v>62.02077895833333</v>
@@ -20213,7 +20213,7 @@
         <v>0</v>
       </c>
       <c r="AH165">
-        <v>58278.89628365689</v>
+        <v>58278.89628365688</v>
       </c>
       <c r="AI165">
         <v>308761.7759046202</v>
@@ -20225,13 +20225,13 @@
         <v>0</v>
       </c>
       <c r="AL165">
-        <v>216133.2431332342</v>
+        <v>216133.2431332341</v>
       </c>
       <c r="AM165">
         <v>0</v>
       </c>
       <c r="AN165">
-        <v>42209.79927458332</v>
+        <v>42209.79927458331</v>
       </c>
     </row>
     <row r="166" spans="1:40">
@@ -20504,37 +20504,37 @@
         <v>0</v>
       </c>
       <c r="U168">
-        <v>744846.5279745497</v>
+        <v>744846.5279745499</v>
       </c>
       <c r="W168">
         <v>60</v>
       </c>
       <c r="AC168">
-        <v>892788.39930133</v>
+        <v>892788.3993013303</v>
       </c>
       <c r="AD168">
-        <v>60626.63917271326</v>
+        <v>60626.63917271328</v>
       </c>
       <c r="AE168">
-        <v>51694.79045973793</v>
+        <v>51694.79045973795</v>
       </c>
       <c r="AF168">
-        <v>9101.943569871151</v>
+        <v>9101.943569871153</v>
       </c>
       <c r="AG168">
         <v>0</v>
       </c>
       <c r="AH168">
-        <v>676141.1816691016</v>
+        <v>676141.1816691018</v>
       </c>
       <c r="AI168">
-        <v>980934.0363932474</v>
+        <v>980934.0363932482</v>
       </c>
       <c r="AJ168">
         <v>145532.5538148287</v>
       </c>
       <c r="AK168">
-        <v>66143.69622541798</v>
+        <v>66143.69622541797</v>
       </c>
       <c r="AL168">
         <v>8032.234298265621</v>
@@ -20543,7 +20543,7 @@
         <v>0</v>
       </c>
       <c r="AN168">
-        <v>489710.433440994</v>
+        <v>489710.4334409942</v>
       </c>
     </row>
     <row r="169" spans="1:40">
@@ -21369,7 +21369,7 @@
         <v>5984311.873583687</v>
       </c>
       <c r="AF176">
-        <v>96053.31544351931</v>
+        <v>96053.31544351934</v>
       </c>
       <c r="AG176">
         <v>0</v>
@@ -21387,7 +21387,7 @@
         <v>6728463.073520347</v>
       </c>
       <c r="AL176">
-        <v>96053.31544351931</v>
+        <v>96053.31544351934</v>
       </c>
       <c r="AM176">
         <v>0</v>
@@ -22032,19 +22032,19 @@
         <v>0</v>
       </c>
       <c r="U182">
-        <v>4397330.383764585</v>
+        <v>4397330.383764587</v>
       </c>
       <c r="W182">
         <v>89.49593836999999</v>
       </c>
       <c r="AC182">
-        <v>14172984.41348477</v>
+        <v>14172984.41348478</v>
       </c>
       <c r="AD182">
-        <v>6673356.755619106</v>
+        <v>6673356.755619111</v>
       </c>
       <c r="AE182">
-        <v>9383589.922142759</v>
+        <v>9383589.922142765</v>
       </c>
       <c r="AF182">
         <v>3780000</v>
@@ -22053,25 +22053,25 @@
         <v>0</v>
       </c>
       <c r="AH182">
-        <v>3991716.481451627</v>
+        <v>3991716.481451629</v>
       </c>
       <c r="AI182">
-        <v>14631649.20010926</v>
+        <v>14631649.20010927</v>
       </c>
       <c r="AJ182">
-        <v>6889319.298375659</v>
+        <v>6889319.298375663</v>
       </c>
       <c r="AK182">
-        <v>9687260.775355328</v>
+        <v>9687260.775355332</v>
       </c>
       <c r="AL182">
-        <v>3902328.003958787</v>
+        <v>3902328.003958786</v>
       </c>
       <c r="AM182">
         <v>0</v>
       </c>
       <c r="AN182">
-        <v>2891090.294899228</v>
+        <v>2891090.29489923</v>
       </c>
     </row>
     <row r="183" spans="1:40">
@@ -22249,7 +22249,7 @@
         <v>1409361.70212766</v>
       </c>
       <c r="R184">
-        <v>3974804.382483129</v>
+        <v>3974804.382483128</v>
       </c>
       <c r="S184">
         <v>0</v>
@@ -22288,7 +22288,7 @@
         <v>4787234.042553192</v>
       </c>
       <c r="AE184">
-        <v>11924413.14744939</v>
+        <v>11924413.14744938</v>
       </c>
       <c r="AF184">
         <v>0</v>
@@ -22306,7 +22306,7 @@
         <v>38862218.90627506</v>
       </c>
       <c r="AK184">
-        <v>51597061.97087712</v>
+        <v>51597061.97087711</v>
       </c>
       <c r="AL184">
         <v>0</v>
@@ -22368,13 +22368,13 @@
         <v>64980000.00000001</v>
       </c>
       <c r="Q185">
-        <v>2015.22013622223</v>
+        <v>2015.220136222231</v>
       </c>
       <c r="R185">
         <v>20000</v>
       </c>
       <c r="S185">
-        <v>296443.5448480757</v>
+        <v>296443.5448480758</v>
       </c>
       <c r="T185">
         <v>0</v>
@@ -22389,13 +22389,13 @@
         <v>64980000.00000001</v>
       </c>
       <c r="AD185">
-        <v>2015.22013622223</v>
+        <v>2015.220136222231</v>
       </c>
       <c r="AE185">
         <v>20000</v>
       </c>
       <c r="AF185">
-        <v>296443.5448480757</v>
+        <v>296443.5448480758</v>
       </c>
       <c r="AG185">
         <v>0</v>
@@ -22407,13 +22407,13 @@
         <v>69445887.83033092</v>
       </c>
       <c r="AJ185">
-        <v>2153.720399099926</v>
+        <v>2153.720399099927</v>
       </c>
       <c r="AK185">
         <v>21374.54226849213</v>
       </c>
       <c r="AL185">
-        <v>316817.2539788418</v>
+        <v>316817.2539788419</v>
       </c>
       <c r="AM185">
         <v>0</v>

</xml_diff>